<commit_message>
Renomeando dashboard.py para app.py
</commit_message>
<xml_diff>
--- a/GESTÃO MANUTENÇÃO.xlsx
+++ b/GESTÃO MANUTENÇÃO.xlsx
@@ -12,7 +12,7 @@
     <sheet name="PNEUS-PREVENTIVAS" sheetId="7" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'MANUTENÇÃO POR VEÍCULO'!$A$4:$N$35</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'MANUTENÇÃO POR VEÍCULO'!$A$4:$N$118</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
@@ -1904,18 +1904,6 @@
     <xf numFmtId="44" fontId="5" fillId="0" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1969,6 +1957,18 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="44" fontId="7" fillId="2" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1977,21 +1977,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="20">
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
     <dxf>
       <font>
         <b/>
@@ -2453,6 +2438,21 @@
         <bottom/>
       </border>
     </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
@@ -2467,23 +2467,23 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabela392134" displayName="Tabela392134" ref="A4:O181" totalsRowShown="0" headerRowDxfId="19" tableBorderDxfId="18">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabela392134" displayName="Tabela392134" ref="A4:O181" totalsRowShown="0" headerRowDxfId="16" tableBorderDxfId="15">
   <tableColumns count="15">
-    <tableColumn id="1" name="Colunas1" dataDxfId="17"/>
-    <tableColumn id="2" name="Colunas2" dataDxfId="16"/>
-    <tableColumn id="4" name="Colunas3" dataDxfId="15"/>
-    <tableColumn id="5" name="Colunas4" dataDxfId="14"/>
-    <tableColumn id="6" name="Colunas5" dataDxfId="13"/>
-    <tableColumn id="10" name="Colunas52" dataDxfId="12"/>
-    <tableColumn id="7" name="Colunas6" dataDxfId="11" dataCellStyle="Moeda"/>
-    <tableColumn id="3" name="Colunas7" dataDxfId="10" dataCellStyle="Moeda"/>
-    <tableColumn id="8" name="Colunas8" dataDxfId="9" dataCellStyle="Moeda"/>
-    <tableColumn id="9" name="Colunas9" dataDxfId="8" dataCellStyle="Moeda"/>
-    <tableColumn id="15" name="Colunas10" dataDxfId="7"/>
-    <tableColumn id="14" name="Colunas11" dataDxfId="6"/>
-    <tableColumn id="13" name="Colunas12" dataDxfId="5"/>
-    <tableColumn id="12" name="Colunas13" dataDxfId="4"/>
-    <tableColumn id="17" name="Colunas14" dataDxfId="3"/>
+    <tableColumn id="1" name="Colunas1" dataDxfId="14"/>
+    <tableColumn id="2" name="Colunas2" dataDxfId="13"/>
+    <tableColumn id="4" name="Colunas3" dataDxfId="12"/>
+    <tableColumn id="5" name="Colunas4" dataDxfId="11"/>
+    <tableColumn id="6" name="Colunas5" dataDxfId="10"/>
+    <tableColumn id="10" name="Colunas52" dataDxfId="9"/>
+    <tableColumn id="7" name="Colunas6" dataDxfId="8" dataCellStyle="Moeda"/>
+    <tableColumn id="3" name="Colunas7" dataDxfId="7" dataCellStyle="Moeda"/>
+    <tableColumn id="8" name="Colunas8" dataDxfId="6" dataCellStyle="Moeda"/>
+    <tableColumn id="9" name="Colunas9" dataDxfId="5" dataCellStyle="Moeda"/>
+    <tableColumn id="15" name="Colunas10" dataDxfId="4"/>
+    <tableColumn id="14" name="Colunas11" dataDxfId="3"/>
+    <tableColumn id="13" name="Colunas12" dataDxfId="2"/>
+    <tableColumn id="12" name="Colunas13" dataDxfId="1"/>
+    <tableColumn id="17" name="Colunas14" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2893,13 +2893,13 @@
       <c r="A8" s="58">
         <v>7</v>
       </c>
-      <c r="B8" s="273" t="s">
+      <c r="B8" s="269" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="273" t="s">
+      <c r="C8" s="269" t="s">
         <v>19</v>
       </c>
-      <c r="D8" s="274" t="s">
+      <c r="D8" s="270" t="s">
         <v>40</v>
       </c>
     </row>
@@ -2907,13 +2907,13 @@
       <c r="A9" s="58">
         <v>8</v>
       </c>
-      <c r="B9" s="275" t="s">
+      <c r="B9" s="271" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="275" t="s">
+      <c r="C9" s="271" t="s">
         <v>39</v>
       </c>
-      <c r="D9" s="276" t="s">
+      <c r="D9" s="272" t="s">
         <v>40</v>
       </c>
     </row>
@@ -2921,13 +2921,13 @@
       <c r="A10" s="58">
         <v>9</v>
       </c>
-      <c r="B10" s="273" t="s">
+      <c r="B10" s="269" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="273" t="s">
+      <c r="C10" s="269" t="s">
         <v>20</v>
       </c>
-      <c r="D10" s="274" t="s">
+      <c r="D10" s="270" t="s">
         <v>40</v>
       </c>
     </row>
@@ -2935,13 +2935,13 @@
       <c r="A11" s="58">
         <v>10</v>
       </c>
-      <c r="B11" s="276" t="s">
+      <c r="B11" s="272" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="276" t="s">
+      <c r="C11" s="272" t="s">
         <v>21</v>
       </c>
-      <c r="D11" s="276" t="s">
+      <c r="D11" s="272" t="s">
         <v>40</v>
       </c>
     </row>
@@ -2949,13 +2949,13 @@
       <c r="A12" s="58">
         <v>11</v>
       </c>
-      <c r="B12" s="274" t="s">
+      <c r="B12" s="270" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="274" t="s">
+      <c r="C12" s="270" t="s">
         <v>22</v>
       </c>
-      <c r="D12" s="274" t="s">
+      <c r="D12" s="270" t="s">
         <v>40</v>
       </c>
     </row>
@@ -2963,13 +2963,13 @@
       <c r="A13" s="58">
         <v>13</v>
       </c>
-      <c r="B13" s="276" t="s">
+      <c r="B13" s="272" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="275" t="s">
+      <c r="C13" s="271" t="s">
         <v>149</v>
       </c>
-      <c r="D13" s="276" t="s">
+      <c r="D13" s="272" t="s">
         <v>40</v>
       </c>
     </row>
@@ -2977,13 +2977,13 @@
       <c r="A14" s="33">
         <v>14</v>
       </c>
-      <c r="B14" s="273" t="s">
+      <c r="B14" s="269" t="s">
         <v>57</v>
       </c>
-      <c r="C14" s="273" t="s">
+      <c r="C14" s="269" t="s">
         <v>24</v>
       </c>
-      <c r="D14" s="273" t="s">
+      <c r="D14" s="269" t="s">
         <v>40</v>
       </c>
     </row>
@@ -2991,13 +2991,13 @@
       <c r="A15" s="57">
         <v>15</v>
       </c>
-      <c r="B15" s="275" t="s">
+      <c r="B15" s="271" t="s">
         <v>25</v>
       </c>
-      <c r="C15" s="275" t="s">
+      <c r="C15" s="271" t="s">
         <v>61</v>
       </c>
-      <c r="D15" s="276" t="s">
+      <c r="D15" s="272" t="s">
         <v>40</v>
       </c>
     </row>
@@ -3005,13 +3005,13 @@
       <c r="A16" s="57">
         <v>16</v>
       </c>
-      <c r="B16" s="273" t="s">
+      <c r="B16" s="269" t="s">
         <v>26</v>
       </c>
-      <c r="C16" s="273" t="s">
+      <c r="C16" s="269" t="s">
         <v>150</v>
       </c>
-      <c r="D16" s="274" t="s">
+      <c r="D16" s="270" t="s">
         <v>40</v>
       </c>
     </row>
@@ -3019,13 +3019,13 @@
       <c r="A17" s="57">
         <v>17</v>
       </c>
-      <c r="B17" s="275" t="s">
+      <c r="B17" s="271" t="s">
         <v>155</v>
       </c>
-      <c r="C17" s="275" t="s">
+      <c r="C17" s="271" t="s">
         <v>156</v>
       </c>
-      <c r="D17" s="276" t="s">
+      <c r="D17" s="272" t="s">
         <v>40</v>
       </c>
     </row>
@@ -3036,7 +3036,7 @@
       <c r="D18" s="109"/>
     </row>
     <row r="26" spans="1:4">
-      <c r="D26" s="277"/>
+      <c r="D26" s="273"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -3047,8 +3047,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N125"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -3070,16 +3070,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="25.2" thickBot="1">
-      <c r="A1" s="271" t="s">
+      <c r="A1" s="290" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="271"/>
-      <c r="C1" s="271"/>
-      <c r="D1" s="271"/>
-      <c r="E1" s="271"/>
-      <c r="F1" s="271"/>
-      <c r="G1" s="271"/>
-      <c r="H1" s="271"/>
+      <c r="B1" s="290"/>
+      <c r="C1" s="290"/>
+      <c r="D1" s="290"/>
+      <c r="E1" s="290"/>
+      <c r="F1" s="290"/>
+      <c r="G1" s="290"/>
+      <c r="H1" s="290"/>
       <c r="I1" s="70"/>
       <c r="J1" s="70"/>
       <c r="K1" s="70"/>
@@ -3087,13 +3087,13 @@
       <c r="M1" s="182"/>
       <c r="N1" s="178"/>
     </row>
-    <row r="2" spans="1:14" s="269" customFormat="1" ht="23.4" thickTop="1"/>
+    <row r="2" spans="1:14" s="288" customFormat="1" ht="23.4" thickTop="1"/>
     <row r="3" spans="1:14" ht="26.4">
-      <c r="A3" s="270" t="s">
+      <c r="A3" s="289" t="s">
         <v>49</v>
       </c>
-      <c r="B3" s="270"/>
-      <c r="C3" s="270"/>
+      <c r="B3" s="289"/>
+      <c r="C3" s="289"/>
       <c r="D3" s="184">
         <f>SUM(J5:J172)</f>
         <v>82845.56</v>
@@ -3105,11 +3105,11 @@
         <f>D3+J3</f>
         <v>128259.45999999999</v>
       </c>
-      <c r="G3" s="270" t="s">
+      <c r="G3" s="289" t="s">
         <v>50</v>
       </c>
-      <c r="H3" s="270"/>
-      <c r="I3" s="270"/>
+      <c r="H3" s="289"/>
+      <c r="I3" s="289"/>
       <c r="J3" s="187">
         <f>SUM(K5:K173)</f>
         <v>45413.9</v>
@@ -3119,7 +3119,7 @@
       <c r="M3" s="189"/>
       <c r="N3" s="190"/>
     </row>
-    <row r="4" spans="1:14" ht="34.799999999999997">
+    <row r="4" spans="1:14" ht="69.599999999999994">
       <c r="A4" s="191" t="s">
         <v>28</v>
       </c>
@@ -3163,29 +3163,29 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:14" s="277" customFormat="1" ht="15.6">
-      <c r="A5" s="278">
+    <row r="5" spans="1:14" s="273" customFormat="1" ht="15.6">
+      <c r="A5" s="274">
         <v>1</v>
       </c>
-      <c r="B5" s="279" t="s">
+      <c r="B5" s="275" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="278" t="s">
-        <v>0</v>
-      </c>
-      <c r="D5" s="280">
+      <c r="C5" s="274" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" s="276">
         <v>45706</v>
       </c>
-      <c r="E5" s="281" t="s">
+      <c r="E5" s="277" t="s">
         <v>157</v>
       </c>
       <c r="F5" s="268" t="s">
         <v>44</v>
       </c>
-      <c r="G5" s="282">
+      <c r="G5" s="278">
         <v>3000</v>
       </c>
-      <c r="H5" s="283">
+      <c r="H5" s="279">
         <v>2800</v>
       </c>
       <c r="I5" s="268">
@@ -3202,27 +3202,27 @@
       <c r="L5" s="268" t="s">
         <v>54</v>
       </c>
-      <c r="M5" s="284" t="s">
+      <c r="M5" s="280" t="s">
         <v>83</v>
       </c>
-      <c r="N5" s="279" t="s">
+      <c r="N5" s="275" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:14" s="277" customFormat="1" ht="15.6">
-      <c r="A6" s="288">
+    <row r="6" spans="1:14" s="273" customFormat="1" ht="15.6">
+      <c r="A6" s="284">
         <v>3</v>
       </c>
-      <c r="B6" s="289" t="s">
+      <c r="B6" s="285" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="288" t="s">
+      <c r="C6" s="284" t="s">
         <v>2</v>
       </c>
       <c r="D6" s="235">
         <v>45708</v>
       </c>
-      <c r="E6" s="290" t="s">
+      <c r="E6" s="286" t="s">
         <v>103</v>
       </c>
       <c r="F6" s="212" t="s">
@@ -3251,33 +3251,33 @@
       <c r="M6" s="236" t="s">
         <v>82</v>
       </c>
-      <c r="N6" s="289" t="s">
+      <c r="N6" s="285" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:14" s="277" customFormat="1" ht="15.6">
-      <c r="A7" s="287">
+    <row r="7" spans="1:14" s="273" customFormat="1" ht="15.6">
+      <c r="A7" s="283">
         <v>4</v>
       </c>
-      <c r="B7" s="279" t="s">
+      <c r="B7" s="275" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="278" t="s">
+      <c r="C7" s="274" t="s">
         <v>38</v>
       </c>
-      <c r="D7" s="280">
+      <c r="D7" s="276">
         <v>45724</v>
       </c>
-      <c r="E7" s="285" t="s">
+      <c r="E7" s="281" t="s">
         <v>152</v>
       </c>
       <c r="F7" s="268" t="s">
         <v>44</v>
       </c>
-      <c r="G7" s="282">
+      <c r="G7" s="278">
         <v>1944</v>
       </c>
-      <c r="H7" s="283">
+      <c r="H7" s="279">
         <v>2345.98</v>
       </c>
       <c r="I7" s="268">
@@ -3294,27 +3294,27 @@
       <c r="L7" s="268" t="s">
         <v>54</v>
       </c>
-      <c r="M7" s="286" t="s">
+      <c r="M7" s="282" t="s">
         <v>82</v>
       </c>
-      <c r="N7" s="279" t="s">
+      <c r="N7" s="275" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:14" s="277" customFormat="1" ht="15.6">
-      <c r="A8" s="288">
+    <row r="8" spans="1:14" s="273" customFormat="1" ht="15.6">
+      <c r="A8" s="284">
         <v>10</v>
       </c>
-      <c r="B8" s="289" t="s">
+      <c r="B8" s="285" t="s">
         <v>147</v>
       </c>
-      <c r="C8" s="288" t="s">
+      <c r="C8" s="284" t="s">
         <v>9</v>
       </c>
       <c r="D8" s="235">
         <v>45740</v>
       </c>
-      <c r="E8" s="290" t="s">
+      <c r="E8" s="286" t="s">
         <v>133</v>
       </c>
       <c r="F8" s="212" t="s">
@@ -3326,7 +3326,7 @@
       <c r="H8" s="214">
         <v>660.4</v>
       </c>
-      <c r="I8" s="291">
+      <c r="I8" s="287">
         <v>800</v>
       </c>
       <c r="J8" s="212">
@@ -3337,39 +3337,39 @@
         <f t="shared" si="1"/>
         <v>139.60000000000002</v>
       </c>
-      <c r="L8" s="291" t="s">
+      <c r="L8" s="287" t="s">
         <v>54</v>
       </c>
       <c r="M8" s="236" t="s">
         <v>82</v>
       </c>
-      <c r="N8" s="289" t="s">
+      <c r="N8" s="285" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:14" s="277" customFormat="1" ht="15.6">
-      <c r="A9" s="287">
+    <row r="9" spans="1:14" s="273" customFormat="1" ht="15.6">
+      <c r="A9" s="283">
         <v>11</v>
       </c>
-      <c r="B9" s="279" t="s">
+      <c r="B9" s="275" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="278" t="s">
+      <c r="C9" s="274" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="280">
+      <c r="D9" s="276">
         <v>45744</v>
       </c>
-      <c r="E9" s="285" t="s">
+      <c r="E9" s="281" t="s">
         <v>99</v>
       </c>
       <c r="F9" s="268" t="s">
         <v>44</v>
       </c>
-      <c r="G9" s="282">
+      <c r="G9" s="278">
         <v>180</v>
       </c>
-      <c r="H9" s="283">
+      <c r="H9" s="279">
         <v>180</v>
       </c>
       <c r="I9" s="268">
@@ -3386,10 +3386,10 @@
       <c r="L9" s="268" t="s">
         <v>54</v>
       </c>
-      <c r="M9" s="286" t="s">
+      <c r="M9" s="282" t="s">
         <v>82</v>
       </c>
-      <c r="N9" s="279" t="s">
+      <c r="N9" s="275" t="s">
         <v>40</v>
       </c>
     </row>
@@ -4634,16 +4634,16 @@
       </c>
     </row>
     <row r="37" spans="1:14" ht="15.6">
-      <c r="A37" s="278">
+      <c r="A37" s="274">
         <v>10</v>
       </c>
-      <c r="B37" s="279" t="s">
+      <c r="B37" s="275" t="s">
         <v>147</v>
       </c>
-      <c r="C37" s="278" t="s">
+      <c r="C37" s="274" t="s">
         <v>9</v>
       </c>
-      <c r="D37" s="280">
+      <c r="D37" s="276">
         <v>45747</v>
       </c>
       <c r="E37" s="216" t="s">
@@ -6574,6 +6574,7 @@
       <c r="N125" s="261"/>
     </row>
   </sheetData>
+  <autoFilter ref="A4:N118"/>
   <mergeCells count="4">
     <mergeCell ref="A2:XFD2"/>
     <mergeCell ref="A3:C3"/>
@@ -6581,17 +6582,17 @@
     <mergeCell ref="G3:I3"/>
   </mergeCells>
   <conditionalFormatting sqref="G5">
-    <cfRule type="expression" dxfId="2" priority="3">
+    <cfRule type="expression" dxfId="19" priority="3">
       <formula>G5=_xludf.MAX($G5:$I5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5">
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="18" priority="2">
       <formula>G5=_xludf.MAX($G5:$I5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I5">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="17" priority="1">
       <formula>G5=_xludf.MAX($G5:$I5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6629,40 +6630,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="25.2" thickBot="1">
-      <c r="A1" s="271" t="s">
+      <c r="A1" s="290" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="271"/>
-      <c r="C1" s="271"/>
-      <c r="D1" s="271"/>
-      <c r="E1" s="271"/>
-      <c r="F1" s="271"/>
-      <c r="G1" s="271"/>
-      <c r="H1" s="271"/>
-      <c r="I1" s="271"/>
-      <c r="J1" s="271"/>
-      <c r="K1" s="271"/>
+      <c r="B1" s="290"/>
+      <c r="C1" s="290"/>
+      <c r="D1" s="290"/>
+      <c r="E1" s="290"/>
+      <c r="F1" s="290"/>
+      <c r="G1" s="290"/>
+      <c r="H1" s="290"/>
+      <c r="I1" s="290"/>
+      <c r="J1" s="290"/>
+      <c r="K1" s="290"/>
       <c r="L1" s="70"/>
       <c r="M1" s="70"/>
       <c r="N1" s="70"/>
     </row>
-    <row r="2" spans="1:15" s="269" customFormat="1" ht="23.4" thickTop="1"/>
+    <row r="2" spans="1:15" s="288" customFormat="1" ht="23.4" thickTop="1"/>
     <row r="3" spans="1:15" ht="21">
-      <c r="A3" s="272" t="s">
+      <c r="A3" s="291" t="s">
         <v>49</v>
       </c>
-      <c r="B3" s="272"/>
-      <c r="C3" s="272"/>
+      <c r="B3" s="291"/>
+      <c r="C3" s="291"/>
       <c r="D3" s="67">
         <f>SUM(K6:K180)</f>
         <v>753.6</v>
       </c>
       <c r="E3" s="110"/>
-      <c r="F3" s="272" t="s">
+      <c r="F3" s="291" t="s">
         <v>50</v>
       </c>
-      <c r="G3" s="272"/>
-      <c r="H3" s="272"/>
+      <c r="G3" s="291"/>
+      <c r="H3" s="291"/>
       <c r="I3" s="68">
         <f>SUM(L6:L181)</f>
         <v>111.38</v>

</xml_diff>

<commit_message>
Correção do nome da coluna DATA
</commit_message>
<xml_diff>
--- a/GESTÃO MANUTENÇÃO.xlsx
+++ b/GESTÃO MANUTENÇÃO.xlsx
@@ -276,9 +276,6 @@
     <t>JEEP/COMPASS LONG.</t>
   </si>
   <si>
-    <t>DATA DE ATUALIZAÇÃO</t>
-  </si>
-  <si>
     <t>TROCAR PARA-LAMA DIANTEIRO POIS ESTÁ QUEBRADO</t>
   </si>
   <si>
@@ -496,6 +493,9 @@
   </si>
   <si>
     <t>3 BANCOS DE COURO, APOIOS DE BRAÇOS TROCADOS E HIGIENIZAÇÃO + LAVAGEM COMPLETA DE CARPÊTE</t>
+  </si>
+  <si>
+    <t>DATA</t>
   </si>
 </sst>
 </file>
@@ -2852,7 +2852,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="61" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C5" s="179" t="s">
         <v>16</v>
@@ -2967,7 +2967,7 @@
         <v>11</v>
       </c>
       <c r="C13" s="271" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D13" s="272" t="s">
         <v>40</v>
@@ -3009,7 +3009,7 @@
         <v>26</v>
       </c>
       <c r="C16" s="269" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D16" s="270" t="s">
         <v>40</v>
@@ -3020,10 +3020,10 @@
         <v>17</v>
       </c>
       <c r="B17" s="271" t="s">
+        <v>154</v>
+      </c>
+      <c r="C17" s="271" t="s">
         <v>155</v>
-      </c>
-      <c r="C17" s="271" t="s">
-        <v>156</v>
       </c>
       <c r="D17" s="272" t="s">
         <v>40</v>
@@ -3047,8 +3047,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A38" sqref="A38"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -3099,7 +3099,7 @@
         <v>82845.56</v>
       </c>
       <c r="E3" s="185" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F3" s="186">
         <f>D3+J3</f>
@@ -3124,13 +3124,13 @@
         <v>28</v>
       </c>
       <c r="B4" s="192" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C4" s="193" t="s">
         <v>33</v>
       </c>
       <c r="D4" s="193" t="s">
-        <v>85</v>
+        <v>158</v>
       </c>
       <c r="E4" s="192" t="s">
         <v>79</v>
@@ -3177,7 +3177,7 @@
         <v>45706</v>
       </c>
       <c r="E5" s="277" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F5" s="268" t="s">
         <v>44</v>
@@ -3223,7 +3223,7 @@
         <v>45708</v>
       </c>
       <c r="E6" s="286" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F6" s="212" t="s">
         <v>44</v>
@@ -3269,7 +3269,7 @@
         <v>45724</v>
       </c>
       <c r="E7" s="281" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F7" s="268" t="s">
         <v>44</v>
@@ -3306,7 +3306,7 @@
         <v>10</v>
       </c>
       <c r="B8" s="285" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C8" s="284" t="s">
         <v>9</v>
@@ -3315,7 +3315,7 @@
         <v>45740</v>
       </c>
       <c r="E8" s="286" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F8" s="212" t="s">
         <v>44</v>
@@ -3361,7 +3361,7 @@
         <v>45744</v>
       </c>
       <c r="E9" s="281" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F9" s="268" t="s">
         <v>44</v>
@@ -3407,7 +3407,7 @@
         <v>45737</v>
       </c>
       <c r="E10" s="218" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F10" s="215" t="s">
         <v>44</v>
@@ -3444,7 +3444,7 @@
         <v>15</v>
       </c>
       <c r="B11" s="230" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C11" s="231" t="s">
         <v>25</v>
@@ -3453,7 +3453,7 @@
         <v>45707</v>
       </c>
       <c r="E11" s="221" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F11" s="222" t="s">
         <v>44</v>
@@ -3812,7 +3812,7 @@
         <v>15</v>
       </c>
       <c r="B19" s="241" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C19" s="201" t="s">
         <v>25</v>
@@ -3867,7 +3867,7 @@
         <v>45744</v>
       </c>
       <c r="E20" s="211" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F20" s="212" t="s">
         <v>44</v>
@@ -3913,7 +3913,7 @@
         <v>45744</v>
       </c>
       <c r="E21" s="202" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F21" s="203" t="s">
         <v>44</v>
@@ -3950,7 +3950,7 @@
         <v>5</v>
       </c>
       <c r="B22" s="239" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C22" s="210" t="s">
         <v>3</v>
@@ -3959,7 +3959,7 @@
         <v>45740</v>
       </c>
       <c r="E22" s="245" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F22" s="246" t="s">
         <v>44</v>
@@ -3996,7 +3996,7 @@
         <v>5</v>
       </c>
       <c r="B23" s="238" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C23" s="201" t="s">
         <v>3</v>
@@ -4005,7 +4005,7 @@
         <v>45740</v>
       </c>
       <c r="E23" s="247" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F23" s="248" t="s">
         <v>44</v>
@@ -4042,7 +4042,7 @@
         <v>5</v>
       </c>
       <c r="B24" s="239" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C24" s="210" t="s">
         <v>3</v>
@@ -4051,7 +4051,7 @@
         <v>45740</v>
       </c>
       <c r="E24" s="245" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F24" s="246" t="s">
         <v>44</v>
@@ -4095,10 +4095,10 @@
       </c>
       <c r="D25" s="201"/>
       <c r="E25" s="202" t="s">
+        <v>88</v>
+      </c>
+      <c r="F25" s="203" t="s">
         <v>89</v>
-      </c>
-      <c r="F25" s="203" t="s">
-        <v>90</v>
       </c>
       <c r="G25" s="204">
         <v>120</v>
@@ -4141,7 +4141,7 @@
         <v>45744</v>
       </c>
       <c r="E26" s="254" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F26" s="215" t="s">
         <v>44</v>
@@ -4187,7 +4187,7 @@
         <v>45744</v>
       </c>
       <c r="E27" s="256" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F27" s="203" t="s">
         <v>44</v>
@@ -4233,7 +4233,7 @@
         <v>45744</v>
       </c>
       <c r="E28" s="218" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F28" s="215" t="s">
         <v>44</v>
@@ -4279,7 +4279,7 @@
         <v>45739</v>
       </c>
       <c r="E29" s="216" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F29" s="203" t="s">
         <v>44</v>
@@ -4325,7 +4325,7 @@
         <v>45740</v>
       </c>
       <c r="E30" s="218" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F30" s="215" t="s">
         <v>44</v>
@@ -4359,19 +4359,19 @@
     </row>
     <row r="31" spans="1:14" s="266" customFormat="1" ht="15">
       <c r="A31" s="263" t="s">
+        <v>134</v>
+      </c>
+      <c r="B31" s="264" t="s">
         <v>135</v>
       </c>
-      <c r="B31" s="264" t="s">
+      <c r="C31" s="258" t="s">
         <v>136</v>
-      </c>
-      <c r="C31" s="258" t="s">
-        <v>137</v>
       </c>
       <c r="D31" s="258">
         <v>45740</v>
       </c>
       <c r="E31" s="263" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F31" s="222" t="s">
         <v>44</v>
@@ -4417,7 +4417,7 @@
         <v>45742</v>
       </c>
       <c r="E32" s="259" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F32" s="215" t="s">
         <v>44</v>
@@ -4463,7 +4463,7 @@
         <v>45742</v>
       </c>
       <c r="E33" s="216" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F33" s="203" t="s">
         <v>44</v>
@@ -4509,7 +4509,7 @@
         <v>45743</v>
       </c>
       <c r="E34" s="218" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F34" s="215" t="s">
         <v>44</v>
@@ -4555,7 +4555,7 @@
         <v>45744</v>
       </c>
       <c r="E35" s="216" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F35" s="203" t="s">
         <v>44</v>
@@ -4601,7 +4601,7 @@
         <v>45747</v>
       </c>
       <c r="E36" s="267" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F36" s="215" t="s">
         <v>44</v>
@@ -4638,7 +4638,7 @@
         <v>10</v>
       </c>
       <c r="B37" s="275" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C37" s="274" t="s">
         <v>9</v>
@@ -4647,7 +4647,7 @@
         <v>45747</v>
       </c>
       <c r="E37" s="216" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F37" s="203" t="s">
         <v>44</v>
@@ -6691,7 +6691,7 @@
         <v>69</v>
       </c>
       <c r="F4" s="63" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G4" s="63" t="s">
         <v>70</v>
@@ -6732,16 +6732,16 @@
         <v>33</v>
       </c>
       <c r="D5" s="75" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E5" s="39" t="s">
+        <v>94</v>
+      </c>
+      <c r="F5" s="39" t="s">
+        <v>110</v>
+      </c>
+      <c r="G5" s="39" t="s">
         <v>95</v>
-      </c>
-      <c r="F5" s="39" t="s">
-        <v>111</v>
-      </c>
-      <c r="G5" s="39" t="s">
-        <v>96</v>
       </c>
       <c r="H5" s="40" t="s">
         <v>31</v>
@@ -6759,7 +6759,7 @@
         <v>35</v>
       </c>
       <c r="M5" s="39" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="N5" s="74" t="s">
         <v>80</v>
@@ -6773,20 +6773,20 @@
         <v>1</v>
       </c>
       <c r="B6" s="80" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C6" s="90" t="s">
         <v>0</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E6" s="76" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F6" s="76"/>
       <c r="G6" s="10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H6" s="11"/>
       <c r="I6" s="43"/>
@@ -6814,14 +6814,14 @@
         <v>1</v>
       </c>
       <c r="D7" s="114" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E7" s="77" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F7" s="77"/>
       <c r="G7" s="12" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H7" s="13"/>
       <c r="I7" s="47"/>
@@ -6849,14 +6849,14 @@
         <v>2</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E8" s="71" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F8" s="71"/>
       <c r="G8" s="10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H8" s="45"/>
       <c r="I8" s="48"/>
@@ -6881,19 +6881,19 @@
         <v>16</v>
       </c>
       <c r="C9" s="91" t="s">
+        <v>125</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="E9" s="71" t="s">
+        <v>100</v>
+      </c>
+      <c r="F9" s="71" t="s">
         <v>126</v>
       </c>
-      <c r="D9" s="9" t="s">
-        <v>112</v>
-      </c>
-      <c r="E9" s="71" t="s">
-        <v>101</v>
-      </c>
-      <c r="F9" s="71" t="s">
-        <v>127</v>
-      </c>
       <c r="G9" s="111" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H9" s="45">
         <v>0</v>
@@ -6927,14 +6927,14 @@
         <v>3</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E10" s="71" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F10" s="71"/>
       <c r="G10" s="10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H10" s="45"/>
       <c r="I10" s="48"/>
@@ -6964,16 +6964,16 @@
         <v>4</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E11" s="71" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F11" s="71" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G11" s="10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H11" s="45"/>
       <c r="I11" s="48"/>
@@ -7003,14 +7003,14 @@
         <v>5</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E12" s="71" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F12" s="71"/>
       <c r="G12" s="10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H12" s="45"/>
       <c r="I12" s="48"/>
@@ -7040,14 +7040,14 @@
         <v>6</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E13" s="71" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F13" s="71"/>
       <c r="G13" s="87" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H13" s="45"/>
       <c r="I13" s="48"/>
@@ -7075,16 +7075,16 @@
         <v>7</v>
       </c>
       <c r="D14" s="113" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E14" s="72" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F14" s="72" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G14" s="10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H14" s="11"/>
       <c r="I14" s="54"/>
@@ -7112,16 +7112,16 @@
         <v>8</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E15" s="71" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F15" s="71" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G15" s="10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H15" s="45"/>
       <c r="I15" s="48"/>
@@ -7149,14 +7149,14 @@
         <v>9</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E16" s="72" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F16" s="72"/>
       <c r="G16" s="10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H16" s="11"/>
       <c r="I16" s="54"/>
@@ -7184,14 +7184,14 @@
         <v>10</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E17" s="71" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F17" s="71"/>
       <c r="G17" s="87" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H17" s="45">
         <v>0</v>
@@ -7225,14 +7225,14 @@
         <v>11</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E18" s="72" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F18" s="72"/>
       <c r="G18" s="10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H18" s="11"/>
       <c r="I18" s="54"/>
@@ -7260,14 +7260,14 @@
         <v>12</v>
       </c>
       <c r="D19" s="113" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E19" s="78" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F19" s="78"/>
       <c r="G19" s="10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H19" s="45"/>
       <c r="I19" s="48"/>
@@ -7289,20 +7289,20 @@
         <v>15</v>
       </c>
       <c r="B20" s="81" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C20" s="97" t="s">
         <v>25</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E20" s="79" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F20" s="112"/>
       <c r="G20" s="10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H20" s="11"/>
       <c r="I20" s="54"/>
@@ -7330,14 +7330,14 @@
         <v>26</v>
       </c>
       <c r="D21" s="120" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E21" s="78" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F21" s="78"/>
       <c r="G21" s="121" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H21" s="122"/>
       <c r="I21" s="123"/>
@@ -7376,11 +7376,11 @@
       <c r="B23" s="140"/>
       <c r="C23" s="141"/>
       <c r="D23" s="146" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E23" s="139"/>
       <c r="F23" s="154" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G23" s="142"/>
       <c r="H23" s="143"/>
@@ -7420,16 +7420,16 @@
         <v>33</v>
       </c>
       <c r="D25" s="164" t="s">
+        <v>119</v>
+      </c>
+      <c r="E25" s="165" t="s">
         <v>120</v>
       </c>
-      <c r="E25" s="165" t="s">
+      <c r="F25" s="165" t="s">
         <v>121</v>
       </c>
-      <c r="F25" s="165" t="s">
+      <c r="G25" s="166" t="s">
         <v>122</v>
-      </c>
-      <c r="G25" s="166" t="s">
-        <v>123</v>
       </c>
       <c r="H25" s="167" t="s">
         <v>31</v>
@@ -7447,7 +7447,7 @@
         <v>35</v>
       </c>
       <c r="M25" s="168" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="N25" s="168" t="s">
         <v>80</v>
@@ -7461,7 +7461,7 @@
         <v>1</v>
       </c>
       <c r="B26" s="127" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C26" s="128" t="s">
         <v>0</v>
@@ -7618,10 +7618,10 @@
         <v>4</v>
       </c>
       <c r="D31" s="173" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E31" s="149" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F31" s="181">
         <v>128893</v>
@@ -7650,7 +7650,7 @@
         <v>54</v>
       </c>
       <c r="N31" s="111" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="O31" s="11" t="s">
         <v>41</v>
@@ -7783,10 +7783,10 @@
         <v>9</v>
       </c>
       <c r="D36" s="173" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E36" s="150" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F36" s="176">
         <v>226526</v>
@@ -7815,10 +7815,10 @@
         <v>54</v>
       </c>
       <c r="N36" s="111" t="s">
+        <v>130</v>
+      </c>
+      <c r="O36" s="102" t="s">
         <v>131</v>
-      </c>
-      <c r="O36" s="102" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="37" spans="1:15" s="46" customFormat="1" ht="15.6">
@@ -7919,7 +7919,7 @@
         <v>15</v>
       </c>
       <c r="B40" s="81" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C40" s="97" t="s">
         <v>25</v>

</xml_diff>

<commit_message>
Ajustes finais para gráficos e layout
</commit_message>
<xml_diff>
--- a/GESTÃO MANUTENÇÃO.xlsx
+++ b/GESTÃO MANUTENÇÃO.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="160">
   <si>
     <t>AWF-1G58</t>
   </si>
@@ -496,6 +496,9 @@
   </si>
   <si>
     <t>DATA</t>
+  </si>
+  <si>
+    <t>CATEGORIA</t>
   </si>
 </sst>
 </file>
@@ -3047,8 +3050,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N125"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -3160,7 +3163,7 @@
         <v>80</v>
       </c>
       <c r="N4" s="197" t="s">
-        <v>37</v>
+        <v>159</v>
       </c>
     </row>
     <row r="5" spans="1:14" s="273" customFormat="1" ht="15.6">

</xml_diff>

<commit_message>
Ajuste nas cores do gráfico de pizza e formatação das datas no gráfico de barras
</commit_message>
<xml_diff>
--- a/GESTÃO MANUTENÇÃO.xlsx
+++ b/GESTÃO MANUTENÇÃO.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="171">
   <si>
     <t>AWF-1G58</t>
   </si>
@@ -279,9 +279,6 @@
     <t>TROCAR PARA-LAMA DIANTEIRO POIS ESTÁ QUEBRADO</t>
   </si>
   <si>
-    <t>FIAT UNO MILLE WAY</t>
-  </si>
-  <si>
     <t>TROCA DO PARACHOQUE TRASEIRO E ARRUMAR AS TRANCAS INTERNAS E EXTERNAS</t>
   </si>
   <si>
@@ -459,9 +456,6 @@
     <t xml:space="preserve">VALOR TOTAL EM CASO DE NÃO ECONOMIA: </t>
   </si>
   <si>
-    <t>I/M.BENZ-MARTICAR VAN</t>
-  </si>
-  <si>
     <t>10.000 KM</t>
   </si>
   <si>
@@ -499,6 +493,45 @@
   </si>
   <si>
     <t>CATEGORIA</t>
+  </si>
+  <si>
+    <t>VOLVO VM 270</t>
+  </si>
+  <si>
+    <t>VW 9.170</t>
+  </si>
+  <si>
+    <t>M.BENZ 1418</t>
+  </si>
+  <si>
+    <t>M.BENZ VAN</t>
+  </si>
+  <si>
+    <t>M.BENZ 1114</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M.BENZ 914 </t>
+  </si>
+  <si>
+    <t>VOLVO FH-410</t>
+  </si>
+  <si>
+    <t>S-R NOMA CG</t>
+  </si>
+  <si>
+    <t>FIAT UNO VIVACE</t>
+  </si>
+  <si>
+    <t>FIAT UNO-WAY</t>
+  </si>
+  <si>
+    <t>VW TITAN 19.320</t>
+  </si>
+  <si>
+    <t>M.BENZ 1113</t>
+  </si>
+  <si>
+    <t>TROCA DE RETROVISOR QUEBRADO E PARABRISA TAMBÉM</t>
   </si>
 </sst>
 </file>
@@ -1133,7 +1166,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="292">
+  <cellXfs count="293">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1827,9 +1860,6 @@
     <xf numFmtId="44" fontId="5" fillId="23" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="14" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1856,9 +1886,6 @@
     </xf>
     <xf numFmtId="44" fontId="7" fillId="4" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="25" fillId="0" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="14" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1973,6 +2000,15 @@
     </xf>
     <xf numFmtId="0" fontId="18" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2855,7 +2891,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="61" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C5" s="179" t="s">
         <v>16</v>
@@ -2896,13 +2932,13 @@
       <c r="A8" s="58">
         <v>7</v>
       </c>
-      <c r="B8" s="269" t="s">
+      <c r="B8" s="267" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="269" t="s">
+      <c r="C8" s="267" t="s">
         <v>19</v>
       </c>
-      <c r="D8" s="270" t="s">
+      <c r="D8" s="268" t="s">
         <v>40</v>
       </c>
     </row>
@@ -2910,13 +2946,13 @@
       <c r="A9" s="58">
         <v>8</v>
       </c>
-      <c r="B9" s="271" t="s">
+      <c r="B9" s="269" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="271" t="s">
+      <c r="C9" s="269" t="s">
         <v>39</v>
       </c>
-      <c r="D9" s="272" t="s">
+      <c r="D9" s="270" t="s">
         <v>40</v>
       </c>
     </row>
@@ -2924,13 +2960,13 @@
       <c r="A10" s="58">
         <v>9</v>
       </c>
-      <c r="B10" s="269" t="s">
+      <c r="B10" s="267" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="269" t="s">
+      <c r="C10" s="267" t="s">
         <v>20</v>
       </c>
-      <c r="D10" s="270" t="s">
+      <c r="D10" s="268" t="s">
         <v>40</v>
       </c>
     </row>
@@ -2938,13 +2974,13 @@
       <c r="A11" s="58">
         <v>10</v>
       </c>
-      <c r="B11" s="272" t="s">
+      <c r="B11" s="270" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="272" t="s">
+      <c r="C11" s="270" t="s">
         <v>21</v>
       </c>
-      <c r="D11" s="272" t="s">
+      <c r="D11" s="270" t="s">
         <v>40</v>
       </c>
     </row>
@@ -2952,13 +2988,13 @@
       <c r="A12" s="58">
         <v>11</v>
       </c>
-      <c r="B12" s="270" t="s">
+      <c r="B12" s="268" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="270" t="s">
+      <c r="C12" s="268" t="s">
         <v>22</v>
       </c>
-      <c r="D12" s="270" t="s">
+      <c r="D12" s="268" t="s">
         <v>40</v>
       </c>
     </row>
@@ -2966,13 +3002,13 @@
       <c r="A13" s="58">
         <v>13</v>
       </c>
-      <c r="B13" s="272" t="s">
+      <c r="B13" s="270" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="271" t="s">
-        <v>148</v>
-      </c>
-      <c r="D13" s="272" t="s">
+      <c r="C13" s="269" t="s">
+        <v>146</v>
+      </c>
+      <c r="D13" s="270" t="s">
         <v>40</v>
       </c>
     </row>
@@ -2980,13 +3016,13 @@
       <c r="A14" s="33">
         <v>14</v>
       </c>
-      <c r="B14" s="269" t="s">
+      <c r="B14" s="267" t="s">
         <v>57</v>
       </c>
-      <c r="C14" s="269" t="s">
+      <c r="C14" s="267" t="s">
         <v>24</v>
       </c>
-      <c r="D14" s="269" t="s">
+      <c r="D14" s="267" t="s">
         <v>40</v>
       </c>
     </row>
@@ -2994,13 +3030,13 @@
       <c r="A15" s="57">
         <v>15</v>
       </c>
-      <c r="B15" s="271" t="s">
+      <c r="B15" s="269" t="s">
         <v>25</v>
       </c>
-      <c r="C15" s="271" t="s">
+      <c r="C15" s="269" t="s">
         <v>61</v>
       </c>
-      <c r="D15" s="272" t="s">
+      <c r="D15" s="270" t="s">
         <v>40</v>
       </c>
     </row>
@@ -3008,13 +3044,13 @@
       <c r="A16" s="57">
         <v>16</v>
       </c>
-      <c r="B16" s="269" t="s">
+      <c r="B16" s="267" t="s">
         <v>26</v>
       </c>
-      <c r="C16" s="269" t="s">
-        <v>149</v>
-      </c>
-      <c r="D16" s="270" t="s">
+      <c r="C16" s="267" t="s">
+        <v>147</v>
+      </c>
+      <c r="D16" s="268" t="s">
         <v>40</v>
       </c>
     </row>
@@ -3022,13 +3058,13 @@
       <c r="A17" s="57">
         <v>17</v>
       </c>
-      <c r="B17" s="271" t="s">
-        <v>154</v>
-      </c>
-      <c r="C17" s="271" t="s">
-        <v>155</v>
-      </c>
-      <c r="D17" s="272" t="s">
+      <c r="B17" s="269" t="s">
+        <v>152</v>
+      </c>
+      <c r="C17" s="269" t="s">
+        <v>153</v>
+      </c>
+      <c r="D17" s="270" t="s">
         <v>40</v>
       </c>
     </row>
@@ -3039,7 +3075,7 @@
       <c r="D18" s="109"/>
     </row>
     <row r="26" spans="1:4">
-      <c r="D26" s="273"/>
+      <c r="D26" s="271"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -3050,8 +3086,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="N5" sqref="N5"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E43" sqref="E43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -3073,16 +3109,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="25.2" thickBot="1">
-      <c r="A1" s="290" t="s">
+      <c r="A1" s="288" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="290"/>
-      <c r="C1" s="290"/>
-      <c r="D1" s="290"/>
-      <c r="E1" s="290"/>
-      <c r="F1" s="290"/>
-      <c r="G1" s="290"/>
-      <c r="H1" s="290"/>
+      <c r="B1" s="288"/>
+      <c r="C1" s="288"/>
+      <c r="D1" s="288"/>
+      <c r="E1" s="288"/>
+      <c r="F1" s="288"/>
+      <c r="G1" s="288"/>
+      <c r="H1" s="288"/>
       <c r="I1" s="70"/>
       <c r="J1" s="70"/>
       <c r="K1" s="70"/>
@@ -3090,32 +3126,32 @@
       <c r="M1" s="182"/>
       <c r="N1" s="178"/>
     </row>
-    <row r="2" spans="1:14" s="288" customFormat="1" ht="23.4" thickTop="1"/>
+    <row r="2" spans="1:14" s="286" customFormat="1" ht="23.4" thickTop="1"/>
     <row r="3" spans="1:14" ht="26.4">
-      <c r="A3" s="289" t="s">
+      <c r="A3" s="287" t="s">
         <v>49</v>
       </c>
-      <c r="B3" s="289"/>
-      <c r="C3" s="289"/>
+      <c r="B3" s="287"/>
+      <c r="C3" s="287"/>
       <c r="D3" s="184">
         <f>SUM(J5:J172)</f>
-        <v>82845.56</v>
+        <v>84250.559999999998</v>
       </c>
       <c r="E3" s="185" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F3" s="186">
         <f>D3+J3</f>
-        <v>128259.45999999999</v>
-      </c>
-      <c r="G3" s="289" t="s">
+        <v>130689.45999999999</v>
+      </c>
+      <c r="G3" s="287" t="s">
         <v>50</v>
       </c>
-      <c r="H3" s="289"/>
-      <c r="I3" s="289"/>
+      <c r="H3" s="287"/>
+      <c r="I3" s="287"/>
       <c r="J3" s="187">
         <f>SUM(K5:K173)</f>
-        <v>45413.9</v>
+        <v>46438.9</v>
       </c>
       <c r="K3" s="188"/>
       <c r="L3" s="189"/>
@@ -3127,13 +3163,13 @@
         <v>28</v>
       </c>
       <c r="B4" s="192" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C4" s="193" t="s">
         <v>33</v>
       </c>
       <c r="D4" s="193" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E4" s="192" t="s">
         <v>79</v>
@@ -3163,70 +3199,70 @@
         <v>80</v>
       </c>
       <c r="N4" s="197" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" s="273" customFormat="1" ht="15.6">
-      <c r="A5" s="274">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" s="271" customFormat="1" ht="15.6">
+      <c r="A5" s="272">
         <v>1</v>
       </c>
-      <c r="B5" s="275" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="274" t="s">
-        <v>0</v>
-      </c>
-      <c r="D5" s="276">
+      <c r="B5" s="273" t="s">
+        <v>158</v>
+      </c>
+      <c r="C5" s="272" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" s="274">
         <v>45706</v>
       </c>
-      <c r="E5" s="277" t="s">
-        <v>156</v>
-      </c>
-      <c r="F5" s="268" t="s">
+      <c r="E5" s="275" t="s">
+        <v>154</v>
+      </c>
+      <c r="F5" s="266" t="s">
         <v>44</v>
       </c>
-      <c r="G5" s="278">
+      <c r="G5" s="276">
         <v>3000</v>
       </c>
-      <c r="H5" s="279">
+      <c r="H5" s="277">
         <v>2800</v>
       </c>
-      <c r="I5" s="268">
+      <c r="I5" s="266">
         <v>3280</v>
       </c>
-      <c r="J5" s="268">
+      <c r="J5" s="266">
         <f t="shared" ref="J5:J67" si="0">MIN(G5:I5)</f>
         <v>2800</v>
       </c>
-      <c r="K5" s="268">
+      <c r="K5" s="266">
         <f t="shared" ref="K5:K67" si="1">MAX(G5:I5) - J5</f>
         <v>480</v>
       </c>
-      <c r="L5" s="268" t="s">
+      <c r="L5" s="266" t="s">
         <v>54</v>
       </c>
-      <c r="M5" s="280" t="s">
+      <c r="M5" s="278" t="s">
         <v>83</v>
       </c>
-      <c r="N5" s="275" t="s">
+      <c r="N5" s="273" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:14" s="273" customFormat="1" ht="15.6">
-      <c r="A6" s="284">
+    <row r="6" spans="1:14" s="271" customFormat="1" ht="15.6">
+      <c r="A6" s="282">
         <v>3</v>
       </c>
-      <c r="B6" s="285" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" s="284" t="s">
+      <c r="B6" s="283" t="s">
+        <v>159</v>
+      </c>
+      <c r="C6" s="282" t="s">
         <v>2</v>
       </c>
       <c r="D6" s="235">
         <v>45708</v>
       </c>
-      <c r="E6" s="286" t="s">
-        <v>102</v>
+      <c r="E6" s="284" t="s">
+        <v>101</v>
       </c>
       <c r="F6" s="212" t="s">
         <v>44</v>
@@ -3254,71 +3290,71 @@
       <c r="M6" s="236" t="s">
         <v>82</v>
       </c>
-      <c r="N6" s="285" t="s">
+      <c r="N6" s="283" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:14" s="273" customFormat="1" ht="15.6">
-      <c r="A7" s="283">
+    <row r="7" spans="1:14" s="271" customFormat="1" ht="15.6">
+      <c r="A7" s="281">
         <v>4</v>
       </c>
-      <c r="B7" s="275" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" s="274" t="s">
+      <c r="B7" s="273" t="s">
+        <v>160</v>
+      </c>
+      <c r="C7" s="272" t="s">
         <v>38</v>
       </c>
-      <c r="D7" s="276">
+      <c r="D7" s="274">
         <v>45724</v>
       </c>
-      <c r="E7" s="281" t="s">
-        <v>151</v>
-      </c>
-      <c r="F7" s="268" t="s">
+      <c r="E7" s="279" t="s">
+        <v>149</v>
+      </c>
+      <c r="F7" s="266" t="s">
         <v>44</v>
       </c>
-      <c r="G7" s="278">
+      <c r="G7" s="276">
         <v>1944</v>
       </c>
-      <c r="H7" s="279">
+      <c r="H7" s="277">
         <v>2345.98</v>
       </c>
-      <c r="I7" s="268">
+      <c r="I7" s="266">
         <v>1389.9</v>
       </c>
-      <c r="J7" s="268">
+      <c r="J7" s="266">
         <f t="shared" si="0"/>
         <v>1389.9</v>
       </c>
-      <c r="K7" s="268">
+      <c r="K7" s="266">
         <f t="shared" si="1"/>
         <v>956.07999999999993</v>
       </c>
-      <c r="L7" s="268" t="s">
+      <c r="L7" s="266" t="s">
         <v>54</v>
       </c>
-      <c r="M7" s="282" t="s">
+      <c r="M7" s="280" t="s">
         <v>82</v>
       </c>
-      <c r="N7" s="275" t="s">
+      <c r="N7" s="273" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:14" s="273" customFormat="1" ht="15.6">
-      <c r="A8" s="284">
+    <row r="8" spans="1:14" s="271" customFormat="1" ht="15.6">
+      <c r="A8" s="282">
         <v>10</v>
       </c>
-      <c r="B8" s="285" t="s">
-        <v>146</v>
-      </c>
-      <c r="C8" s="284" t="s">
+      <c r="B8" s="283" t="s">
+        <v>161</v>
+      </c>
+      <c r="C8" s="282" t="s">
         <v>9</v>
       </c>
       <c r="D8" s="235">
         <v>45740</v>
       </c>
-      <c r="E8" s="286" t="s">
-        <v>132</v>
+      <c r="E8" s="284" t="s">
+        <v>131</v>
       </c>
       <c r="F8" s="212" t="s">
         <v>44</v>
@@ -3329,7 +3365,7 @@
       <c r="H8" s="214">
         <v>660.4</v>
       </c>
-      <c r="I8" s="287">
+      <c r="I8" s="285">
         <v>800</v>
       </c>
       <c r="J8" s="212">
@@ -3340,59 +3376,59 @@
         <f t="shared" si="1"/>
         <v>139.60000000000002</v>
       </c>
-      <c r="L8" s="287" t="s">
+      <c r="L8" s="285" t="s">
         <v>54</v>
       </c>
       <c r="M8" s="236" t="s">
         <v>82</v>
       </c>
-      <c r="N8" s="285" t="s">
+      <c r="N8" s="283" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:14" s="273" customFormat="1" ht="15.6">
-      <c r="A9" s="283">
+    <row r="9" spans="1:14" s="271" customFormat="1" ht="15.6">
+      <c r="A9" s="281">
         <v>11</v>
       </c>
-      <c r="B9" s="275" t="s">
-        <v>22</v>
-      </c>
-      <c r="C9" s="274" t="s">
+      <c r="B9" s="273" t="s">
+        <v>162</v>
+      </c>
+      <c r="C9" s="272" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="276">
+      <c r="D9" s="274">
         <v>45744</v>
       </c>
-      <c r="E9" s="281" t="s">
-        <v>98</v>
-      </c>
-      <c r="F9" s="268" t="s">
+      <c r="E9" s="279" t="s">
+        <v>97</v>
+      </c>
+      <c r="F9" s="266" t="s">
         <v>44</v>
       </c>
-      <c r="G9" s="278">
+      <c r="G9" s="276">
         <v>180</v>
       </c>
-      <c r="H9" s="279">
+      <c r="H9" s="277">
         <v>180</v>
       </c>
-      <c r="I9" s="268">
+      <c r="I9" s="266">
         <v>190</v>
       </c>
-      <c r="J9" s="268">
+      <c r="J9" s="266">
         <f t="shared" si="0"/>
         <v>180</v>
       </c>
-      <c r="K9" s="268">
+      <c r="K9" s="266">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="L9" s="268" t="s">
+      <c r="L9" s="266" t="s">
         <v>54</v>
       </c>
-      <c r="M9" s="282" t="s">
+      <c r="M9" s="280" t="s">
         <v>82</v>
       </c>
-      <c r="N9" s="275" t="s">
+      <c r="N9" s="273" t="s">
         <v>40</v>
       </c>
     </row>
@@ -3401,7 +3437,7 @@
         <v>14</v>
       </c>
       <c r="B10" s="228" t="s">
-        <v>24</v>
+        <v>163</v>
       </c>
       <c r="C10" s="229" t="s">
         <v>12</v>
@@ -3410,7 +3446,7 @@
         <v>45737</v>
       </c>
       <c r="E10" s="218" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F10" s="215" t="s">
         <v>44</v>
@@ -3447,7 +3483,7 @@
         <v>15</v>
       </c>
       <c r="B11" s="230" t="s">
-        <v>108</v>
+        <v>164</v>
       </c>
       <c r="C11" s="231" t="s">
         <v>25</v>
@@ -3456,7 +3492,7 @@
         <v>45707</v>
       </c>
       <c r="E11" s="221" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F11" s="222" t="s">
         <v>44</v>
@@ -3493,7 +3529,7 @@
         <v>16</v>
       </c>
       <c r="B12" s="228" t="s">
-        <v>62</v>
+        <v>165</v>
       </c>
       <c r="C12" s="229" t="s">
         <v>26</v>
@@ -3539,7 +3575,7 @@
         <v>6</v>
       </c>
       <c r="B13" s="230" t="s">
-        <v>18</v>
+        <v>166</v>
       </c>
       <c r="C13" s="201" t="s">
         <v>4</v>
@@ -3672,12 +3708,12 @@
         <v>41</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="15">
+    <row r="16" spans="1:14" ht="15.6">
       <c r="A16" s="218">
         <v>14</v>
       </c>
-      <c r="B16" s="239" t="s">
-        <v>55</v>
+      <c r="B16" s="228" t="s">
+        <v>163</v>
       </c>
       <c r="C16" s="210" t="s">
         <v>57</v>
@@ -3718,12 +3754,12 @@
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="1:14" ht="15">
+    <row r="17" spans="1:14" ht="15.6">
       <c r="A17" s="216">
         <v>14</v>
       </c>
-      <c r="B17" s="238" t="s">
-        <v>55</v>
+      <c r="B17" s="290" t="s">
+        <v>163</v>
       </c>
       <c r="C17" s="201" t="s">
         <v>57</v>
@@ -3764,12 +3800,12 @@
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="1:14" ht="15">
+    <row r="18" spans="1:14" ht="15.6">
       <c r="A18" s="218">
         <v>14</v>
       </c>
-      <c r="B18" s="239" t="s">
-        <v>55</v>
+      <c r="B18" s="228" t="s">
+        <v>163</v>
       </c>
       <c r="C18" s="210" t="s">
         <v>57</v>
@@ -3810,12 +3846,12 @@
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="1:14" ht="15">
+    <row r="19" spans="1:14" ht="15.6">
       <c r="A19" s="216">
         <v>15</v>
       </c>
-      <c r="B19" s="241" t="s">
-        <v>108</v>
+      <c r="B19" s="230" t="s">
+        <v>164</v>
       </c>
       <c r="C19" s="201" t="s">
         <v>25</v>
@@ -3857,11 +3893,11 @@
       </c>
     </row>
     <row r="20" spans="1:14" ht="15.6">
-      <c r="A20" s="242">
+      <c r="A20" s="241">
         <v>1</v>
       </c>
-      <c r="B20" s="208" t="s">
-        <v>13</v>
+      <c r="B20" s="283" t="s">
+        <v>158</v>
       </c>
       <c r="C20" s="209" t="s">
         <v>0</v>
@@ -3875,7 +3911,7 @@
       <c r="F20" s="212" t="s">
         <v>44</v>
       </c>
-      <c r="G20" s="243">
+      <c r="G20" s="242">
         <v>900</v>
       </c>
       <c r="H20" s="220">
@@ -3895,7 +3931,7 @@
       <c r="L20" s="215" t="s">
         <v>54</v>
       </c>
-      <c r="M20" s="244" t="s">
+      <c r="M20" s="243" t="s">
         <v>81</v>
       </c>
       <c r="N20" s="240" t="s">
@@ -3906,8 +3942,8 @@
       <c r="A21" s="198">
         <v>1</v>
       </c>
-      <c r="B21" s="199" t="s">
-        <v>13</v>
+      <c r="B21" s="273" t="s">
+        <v>158</v>
       </c>
       <c r="C21" s="200" t="s">
         <v>0</v>
@@ -3916,7 +3952,7 @@
         <v>45744</v>
       </c>
       <c r="E21" s="202" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F21" s="203" t="s">
         <v>44</v>
@@ -3953,7 +3989,7 @@
         <v>5</v>
       </c>
       <c r="B22" s="239" t="s">
-        <v>86</v>
+        <v>167</v>
       </c>
       <c r="C22" s="210" t="s">
         <v>3</v>
@@ -3961,13 +3997,13 @@
       <c r="D22" s="210">
         <v>45740</v>
       </c>
-      <c r="E22" s="245" t="s">
-        <v>87</v>
-      </c>
-      <c r="F22" s="246" t="s">
+      <c r="E22" s="244" t="s">
+        <v>86</v>
+      </c>
+      <c r="F22" s="245" t="s">
         <v>44</v>
       </c>
-      <c r="G22" s="243">
+      <c r="G22" s="242">
         <v>6500</v>
       </c>
       <c r="H22" s="220">
@@ -3998,8 +4034,8 @@
       <c r="A23" s="216">
         <v>5</v>
       </c>
-      <c r="B23" s="238" t="s">
-        <v>86</v>
+      <c r="B23" s="291" t="s">
+        <v>167</v>
       </c>
       <c r="C23" s="201" t="s">
         <v>3</v>
@@ -4007,13 +4043,13 @@
       <c r="D23" s="201">
         <v>45740</v>
       </c>
-      <c r="E23" s="247" t="s">
-        <v>90</v>
-      </c>
-      <c r="F23" s="248" t="s">
+      <c r="E23" s="246" t="s">
+        <v>89</v>
+      </c>
+      <c r="F23" s="247" t="s">
         <v>44</v>
       </c>
-      <c r="G23" s="249">
+      <c r="G23" s="248">
         <v>0</v>
       </c>
       <c r="H23" s="223">
@@ -4036,7 +4072,7 @@
       <c r="M23" s="225" t="s">
         <v>82</v>
       </c>
-      <c r="N23" s="250" t="s">
+      <c r="N23" s="249" t="s">
         <v>41</v>
       </c>
     </row>
@@ -4045,7 +4081,7 @@
         <v>5</v>
       </c>
       <c r="B24" s="239" t="s">
-        <v>86</v>
+        <v>167</v>
       </c>
       <c r="C24" s="210" t="s">
         <v>3</v>
@@ -4053,10 +4089,10 @@
       <c r="D24" s="210">
         <v>45740</v>
       </c>
-      <c r="E24" s="245" t="s">
-        <v>91</v>
-      </c>
-      <c r="F24" s="246" t="s">
+      <c r="E24" s="244" t="s">
+        <v>90</v>
+      </c>
+      <c r="F24" s="245" t="s">
         <v>44</v>
       </c>
       <c r="G24" s="219">
@@ -4091,17 +4127,19 @@
         <v>6</v>
       </c>
       <c r="B25" s="230" t="s">
-        <v>18</v>
+        <v>166</v>
       </c>
       <c r="C25" s="201" t="s">
         <v>4</v>
       </c>
-      <c r="D25" s="201"/>
+      <c r="D25" s="201">
+        <v>45740</v>
+      </c>
       <c r="E25" s="202" t="s">
+        <v>87</v>
+      </c>
+      <c r="F25" s="203" t="s">
         <v>88</v>
-      </c>
-      <c r="F25" s="203" t="s">
-        <v>89</v>
       </c>
       <c r="G25" s="204">
         <v>120</v>
@@ -4123,33 +4161,33 @@
       <c r="L25" s="203" t="s">
         <v>54</v>
       </c>
-      <c r="M25" s="251" t="s">
-        <v>83</v>
+      <c r="M25" s="217" t="s">
+        <v>82</v>
       </c>
       <c r="N25" s="233" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="26" spans="1:14" ht="15.6">
-      <c r="A26" s="242">
+      <c r="A26" s="241">
         <v>8</v>
       </c>
-      <c r="B26" s="252" t="s">
-        <v>39</v>
-      </c>
-      <c r="C26" s="253" t="s">
+      <c r="B26" s="250" t="s">
+        <v>168</v>
+      </c>
+      <c r="C26" s="251" t="s">
         <v>7</v>
       </c>
       <c r="D26" s="210">
         <v>45744</v>
       </c>
-      <c r="E26" s="254" t="s">
-        <v>92</v>
+      <c r="E26" s="252" t="s">
+        <v>91</v>
       </c>
       <c r="F26" s="215" t="s">
         <v>44</v>
       </c>
-      <c r="G26" s="243">
+      <c r="G26" s="242">
         <v>2600</v>
       </c>
       <c r="H26" s="220">
@@ -4169,7 +4207,7 @@
       <c r="L26" s="215" t="s">
         <v>54</v>
       </c>
-      <c r="M26" s="244" t="s">
+      <c r="M26" s="243" t="s">
         <v>81</v>
       </c>
       <c r="N26" s="240" t="s">
@@ -4181,21 +4219,21 @@
         <v>8</v>
       </c>
       <c r="B27" s="227" t="s">
-        <v>39</v>
-      </c>
-      <c r="C27" s="255" t="s">
+        <v>168</v>
+      </c>
+      <c r="C27" s="253" t="s">
         <v>7</v>
       </c>
       <c r="D27" s="201">
         <v>45744</v>
       </c>
-      <c r="E27" s="256" t="s">
-        <v>150</v>
+      <c r="E27" s="254" t="s">
+        <v>148</v>
       </c>
       <c r="F27" s="203" t="s">
         <v>44</v>
       </c>
-      <c r="G27" s="257">
+      <c r="G27" s="255">
         <v>1150</v>
       </c>
       <c r="H27" s="205">
@@ -4223,11 +4261,11 @@
       </c>
     </row>
     <row r="28" spans="1:14" ht="15.6">
-      <c r="A28" s="242">
+      <c r="A28" s="241">
         <v>3</v>
       </c>
-      <c r="B28" s="208" t="s">
-        <v>15</v>
+      <c r="B28" s="283" t="s">
+        <v>159</v>
       </c>
       <c r="C28" s="209" t="s">
         <v>2</v>
@@ -4236,7 +4274,7 @@
         <v>45744</v>
       </c>
       <c r="E28" s="218" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F28" s="215" t="s">
         <v>44</v>
@@ -4272,8 +4310,8 @@
       <c r="A29" s="198">
         <v>3</v>
       </c>
-      <c r="B29" s="199" t="s">
-        <v>15</v>
+      <c r="B29" s="273" t="s">
+        <v>159</v>
       </c>
       <c r="C29" s="200" t="s">
         <v>2</v>
@@ -4282,7 +4320,7 @@
         <v>45739</v>
       </c>
       <c r="E29" s="216" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F29" s="203" t="s">
         <v>44</v>
@@ -4328,7 +4366,7 @@
         <v>45740</v>
       </c>
       <c r="E30" s="218" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F30" s="215" t="s">
         <v>44</v>
@@ -4360,26 +4398,26 @@
         <v>40</v>
       </c>
     </row>
-    <row r="31" spans="1:14" s="266" customFormat="1" ht="15">
-      <c r="A31" s="263" t="s">
+    <row r="31" spans="1:14" s="264" customFormat="1" ht="15">
+      <c r="A31" s="261" t="s">
+        <v>133</v>
+      </c>
+      <c r="B31" s="262" t="s">
         <v>134</v>
       </c>
-      <c r="B31" s="264" t="s">
+      <c r="C31" s="256" t="s">
         <v>135</v>
       </c>
-      <c r="C31" s="258" t="s">
+      <c r="D31" s="256">
+        <v>45740</v>
+      </c>
+      <c r="E31" s="261" t="s">
         <v>136</v>
-      </c>
-      <c r="D31" s="258">
-        <v>45740</v>
-      </c>
-      <c r="E31" s="263" t="s">
-        <v>137</v>
       </c>
       <c r="F31" s="222" t="s">
         <v>44</v>
       </c>
-      <c r="G31" s="265">
+      <c r="G31" s="263">
         <v>2849.9</v>
       </c>
       <c r="H31" s="223">
@@ -4402,7 +4440,7 @@
       <c r="M31" s="225" t="s">
         <v>82</v>
       </c>
-      <c r="N31" s="250" t="s">
+      <c r="N31" s="249" t="s">
         <v>41</v>
       </c>
     </row>
@@ -4419,13 +4457,13 @@
       <c r="D32" s="210">
         <v>45742</v>
       </c>
-      <c r="E32" s="259" t="s">
-        <v>139</v>
+      <c r="E32" s="257" t="s">
+        <v>138</v>
       </c>
       <c r="F32" s="215" t="s">
         <v>44</v>
       </c>
-      <c r="G32" s="243">
+      <c r="G32" s="242">
         <v>8459</v>
       </c>
       <c r="H32" s="220">
@@ -4457,7 +4495,7 @@
         <v>6</v>
       </c>
       <c r="B33" s="230" t="s">
-        <v>18</v>
+        <v>166</v>
       </c>
       <c r="C33" s="201" t="s">
         <v>4</v>
@@ -4466,12 +4504,12 @@
         <v>45742</v>
       </c>
       <c r="E33" s="216" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F33" s="203" t="s">
         <v>44</v>
       </c>
-      <c r="G33" s="257">
+      <c r="G33" s="255">
         <v>918</v>
       </c>
       <c r="H33" s="205">
@@ -4499,20 +4537,20 @@
       </c>
     </row>
     <row r="34" spans="1:14" ht="15.6">
-      <c r="A34" s="242">
+      <c r="A34" s="241">
         <v>2</v>
       </c>
       <c r="B34" s="208" t="s">
-        <v>14</v>
+        <v>169</v>
       </c>
       <c r="C34" s="209" t="s">
         <v>1</v>
       </c>
-      <c r="D34" s="260">
+      <c r="D34" s="258">
         <v>45743</v>
       </c>
       <c r="E34" s="218" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F34" s="215" t="s">
         <v>44</v>
@@ -4548,8 +4586,8 @@
       <c r="A35" s="198">
         <v>1</v>
       </c>
-      <c r="B35" s="199" t="s">
-        <v>13</v>
+      <c r="B35" s="273" t="s">
+        <v>158</v>
       </c>
       <c r="C35" s="200" t="s">
         <v>0</v>
@@ -4558,7 +4596,7 @@
         <v>45744</v>
       </c>
       <c r="E35" s="216" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F35" s="203" t="s">
         <v>44</v>
@@ -4590,12 +4628,12 @@
         <v>40</v>
       </c>
     </row>
-    <row r="36" spans="1:14" ht="15">
+    <row r="36" spans="1:14" ht="15.6">
       <c r="A36" s="218">
         <v>14</v>
       </c>
-      <c r="B36" s="239" t="s">
-        <v>55</v>
+      <c r="B36" s="228" t="s">
+        <v>163</v>
       </c>
       <c r="C36" s="210" t="s">
         <v>57</v>
@@ -4603,8 +4641,8 @@
       <c r="D36" s="210">
         <v>45747</v>
       </c>
-      <c r="E36" s="267" t="s">
-        <v>152</v>
+      <c r="E36" s="265" t="s">
+        <v>150</v>
       </c>
       <c r="F36" s="215" t="s">
         <v>44</v>
@@ -4637,20 +4675,20 @@
       </c>
     </row>
     <row r="37" spans="1:14" ht="15.6">
-      <c r="A37" s="274">
+      <c r="A37" s="272">
         <v>10</v>
       </c>
-      <c r="B37" s="275" t="s">
-        <v>146</v>
-      </c>
-      <c r="C37" s="274" t="s">
+      <c r="B37" s="273" t="s">
+        <v>161</v>
+      </c>
+      <c r="C37" s="272" t="s">
         <v>9</v>
       </c>
-      <c r="D37" s="276">
+      <c r="D37" s="274">
         <v>45747</v>
       </c>
       <c r="E37" s="216" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="F37" s="203" t="s">
         <v>44</v>
@@ -4683,26 +4721,50 @@
       </c>
     </row>
     <row r="38" spans="1:14" ht="15.6">
-      <c r="A38" s="242"/>
-      <c r="B38" s="208"/>
-      <c r="C38" s="209"/>
-      <c r="D38" s="260"/>
-      <c r="E38" s="218"/>
-      <c r="F38" s="215"/>
-      <c r="G38" s="219"/>
-      <c r="H38" s="220"/>
-      <c r="I38" s="215"/>
+      <c r="A38" s="292">
+        <v>4</v>
+      </c>
+      <c r="B38" s="283" t="s">
+        <v>160</v>
+      </c>
+      <c r="C38" s="282" t="s">
+        <v>38</v>
+      </c>
+      <c r="D38" s="235">
+        <v>45749</v>
+      </c>
+      <c r="E38" s="218" t="s">
+        <v>170</v>
+      </c>
+      <c r="F38" s="215" t="s">
+        <v>44</v>
+      </c>
+      <c r="G38" s="219">
+        <v>1405</v>
+      </c>
+      <c r="H38" s="220">
+        <v>2430</v>
+      </c>
+      <c r="I38" s="215">
+        <v>2250</v>
+      </c>
       <c r="J38" s="212">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1405</v>
       </c>
       <c r="K38" s="212">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="L38" s="215"/>
-      <c r="M38" s="232"/>
-      <c r="N38" s="240"/>
+        <v>1025</v>
+      </c>
+      <c r="L38" s="215" t="s">
+        <v>54</v>
+      </c>
+      <c r="M38" s="226" t="s">
+        <v>82</v>
+      </c>
+      <c r="N38" s="240" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="39" spans="1:14" ht="15.6">
       <c r="A39" s="198"/>
@@ -4727,10 +4789,10 @@
       <c r="N39" s="233"/>
     </row>
     <row r="40" spans="1:14" ht="15.6">
-      <c r="A40" s="242"/>
+      <c r="A40" s="241"/>
       <c r="B40" s="208"/>
       <c r="C40" s="209"/>
-      <c r="D40" s="260"/>
+      <c r="D40" s="258"/>
       <c r="E40" s="218"/>
       <c r="F40" s="215"/>
       <c r="G40" s="219"/>
@@ -4771,10 +4833,10 @@
       <c r="N41" s="233"/>
     </row>
     <row r="42" spans="1:14" ht="15.6">
-      <c r="A42" s="242"/>
+      <c r="A42" s="241"/>
       <c r="B42" s="208"/>
       <c r="C42" s="209"/>
-      <c r="D42" s="260"/>
+      <c r="D42" s="258"/>
       <c r="E42" s="218"/>
       <c r="F42" s="215"/>
       <c r="G42" s="219"/>
@@ -4815,10 +4877,10 @@
       <c r="N43" s="233"/>
     </row>
     <row r="44" spans="1:14" ht="15.6">
-      <c r="A44" s="242"/>
+      <c r="A44" s="241"/>
       <c r="B44" s="208"/>
       <c r="C44" s="209"/>
-      <c r="D44" s="260"/>
+      <c r="D44" s="258"/>
       <c r="E44" s="218"/>
       <c r="F44" s="215"/>
       <c r="G44" s="219"/>
@@ -4859,10 +4921,10 @@
       <c r="N45" s="233"/>
     </row>
     <row r="46" spans="1:14" ht="15.6">
-      <c r="A46" s="242"/>
+      <c r="A46" s="241"/>
       <c r="B46" s="208"/>
       <c r="C46" s="209"/>
-      <c r="D46" s="260"/>
+      <c r="D46" s="258"/>
       <c r="E46" s="218"/>
       <c r="F46" s="215"/>
       <c r="G46" s="219"/>
@@ -4903,10 +4965,10 @@
       <c r="N47" s="233"/>
     </row>
     <row r="48" spans="1:14" ht="15.6">
-      <c r="A48" s="242"/>
+      <c r="A48" s="241"/>
       <c r="B48" s="208"/>
       <c r="C48" s="209"/>
-      <c r="D48" s="260"/>
+      <c r="D48" s="258"/>
       <c r="E48" s="218"/>
       <c r="F48" s="215"/>
       <c r="G48" s="219"/>
@@ -4947,10 +5009,10 @@
       <c r="N49" s="233"/>
     </row>
     <row r="50" spans="1:14" ht="15.6">
-      <c r="A50" s="242"/>
+      <c r="A50" s="241"/>
       <c r="B50" s="208"/>
       <c r="C50" s="209"/>
-      <c r="D50" s="260"/>
+      <c r="D50" s="258"/>
       <c r="E50" s="218"/>
       <c r="F50" s="215"/>
       <c r="G50" s="219"/>
@@ -4991,10 +5053,10 @@
       <c r="N51" s="233"/>
     </row>
     <row r="52" spans="1:14" ht="15.6">
-      <c r="A52" s="242"/>
+      <c r="A52" s="241"/>
       <c r="B52" s="208"/>
       <c r="C52" s="209"/>
-      <c r="D52" s="260"/>
+      <c r="D52" s="258"/>
       <c r="E52" s="218"/>
       <c r="F52" s="215"/>
       <c r="G52" s="219"/>
@@ -5035,10 +5097,10 @@
       <c r="N53" s="233"/>
     </row>
     <row r="54" spans="1:14" ht="15.6">
-      <c r="A54" s="242"/>
+      <c r="A54" s="241"/>
       <c r="B54" s="208"/>
       <c r="C54" s="209"/>
-      <c r="D54" s="260"/>
+      <c r="D54" s="258"/>
       <c r="E54" s="218"/>
       <c r="F54" s="215"/>
       <c r="G54" s="219"/>
@@ -5079,10 +5141,10 @@
       <c r="N55" s="233"/>
     </row>
     <row r="56" spans="1:14" ht="15.6">
-      <c r="A56" s="242"/>
+      <c r="A56" s="241"/>
       <c r="B56" s="208"/>
       <c r="C56" s="209"/>
-      <c r="D56" s="260"/>
+      <c r="D56" s="258"/>
       <c r="E56" s="218"/>
       <c r="F56" s="215"/>
       <c r="G56" s="219"/>
@@ -5110,7 +5172,7 @@
       <c r="G57" s="204"/>
       <c r="H57" s="205"/>
       <c r="I57" s="203"/>
-      <c r="J57" s="268">
+      <c r="J57" s="266">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -5123,10 +5185,10 @@
       <c r="N57" s="233"/>
     </row>
     <row r="58" spans="1:14" ht="15.6">
-      <c r="A58" s="242"/>
+      <c r="A58" s="241"/>
       <c r="B58" s="208"/>
       <c r="C58" s="209"/>
-      <c r="D58" s="260"/>
+      <c r="D58" s="258"/>
       <c r="E58" s="218"/>
       <c r="F58" s="215"/>
       <c r="G58" s="219"/>
@@ -5167,10 +5229,10 @@
       <c r="N59" s="233"/>
     </row>
     <row r="60" spans="1:14" ht="15.6">
-      <c r="A60" s="242"/>
+      <c r="A60" s="241"/>
       <c r="B60" s="208"/>
       <c r="C60" s="209"/>
-      <c r="D60" s="260"/>
+      <c r="D60" s="258"/>
       <c r="E60" s="218"/>
       <c r="F60" s="215"/>
       <c r="G60" s="219"/>
@@ -5211,10 +5273,10 @@
       <c r="N61" s="233"/>
     </row>
     <row r="62" spans="1:14" ht="15.6">
-      <c r="A62" s="242"/>
+      <c r="A62" s="241"/>
       <c r="B62" s="208"/>
       <c r="C62" s="209"/>
-      <c r="D62" s="260"/>
+      <c r="D62" s="258"/>
       <c r="E62" s="218"/>
       <c r="F62" s="215"/>
       <c r="G62" s="219"/>
@@ -5255,10 +5317,10 @@
       <c r="N63" s="233"/>
     </row>
     <row r="64" spans="1:14" ht="15.6">
-      <c r="A64" s="242"/>
+      <c r="A64" s="241"/>
       <c r="B64" s="208"/>
       <c r="C64" s="209"/>
-      <c r="D64" s="260"/>
+      <c r="D64" s="258"/>
       <c r="E64" s="218"/>
       <c r="F64" s="215"/>
       <c r="G64" s="219"/>
@@ -5299,10 +5361,10 @@
       <c r="N65" s="233"/>
     </row>
     <row r="66" spans="1:14" ht="15.6">
-      <c r="A66" s="242"/>
+      <c r="A66" s="241"/>
       <c r="B66" s="208"/>
       <c r="C66" s="209"/>
-      <c r="D66" s="260"/>
+      <c r="D66" s="258"/>
       <c r="E66" s="218"/>
       <c r="F66" s="215"/>
       <c r="G66" s="219"/>
@@ -5343,10 +5405,10 @@
       <c r="N67" s="233"/>
     </row>
     <row r="68" spans="1:14" ht="15.6">
-      <c r="A68" s="242"/>
+      <c r="A68" s="241"/>
       <c r="B68" s="208"/>
       <c r="C68" s="209"/>
-      <c r="D68" s="260"/>
+      <c r="D68" s="258"/>
       <c r="E68" s="218"/>
       <c r="F68" s="215"/>
       <c r="G68" s="219"/>
@@ -5387,10 +5449,10 @@
       <c r="N69" s="233"/>
     </row>
     <row r="70" spans="1:14" ht="15.6">
-      <c r="A70" s="242"/>
+      <c r="A70" s="241"/>
       <c r="B70" s="208"/>
       <c r="C70" s="209"/>
-      <c r="D70" s="260"/>
+      <c r="D70" s="258"/>
       <c r="E70" s="218"/>
       <c r="F70" s="215"/>
       <c r="G70" s="219"/>
@@ -5431,10 +5493,10 @@
       <c r="N71" s="233"/>
     </row>
     <row r="72" spans="1:14" ht="15.6">
-      <c r="A72" s="242"/>
+      <c r="A72" s="241"/>
       <c r="B72" s="208"/>
       <c r="C72" s="209"/>
-      <c r="D72" s="260"/>
+      <c r="D72" s="258"/>
       <c r="E72" s="218"/>
       <c r="F72" s="215"/>
       <c r="G72" s="219"/>
@@ -5475,10 +5537,10 @@
       <c r="N73" s="233"/>
     </row>
     <row r="74" spans="1:14" ht="15.6">
-      <c r="A74" s="242"/>
+      <c r="A74" s="241"/>
       <c r="B74" s="208"/>
       <c r="C74" s="209"/>
-      <c r="D74" s="260"/>
+      <c r="D74" s="258"/>
       <c r="E74" s="218"/>
       <c r="F74" s="215"/>
       <c r="G74" s="219"/>
@@ -5519,10 +5581,10 @@
       <c r="N75" s="233"/>
     </row>
     <row r="76" spans="1:14" ht="15.6">
-      <c r="A76" s="242"/>
+      <c r="A76" s="241"/>
       <c r="B76" s="208"/>
       <c r="C76" s="209"/>
-      <c r="D76" s="260"/>
+      <c r="D76" s="258"/>
       <c r="E76" s="218"/>
       <c r="F76" s="215"/>
       <c r="G76" s="219"/>
@@ -5563,10 +5625,10 @@
       <c r="N77" s="233"/>
     </row>
     <row r="78" spans="1:14" ht="15.6">
-      <c r="A78" s="242"/>
+      <c r="A78" s="241"/>
       <c r="B78" s="208"/>
       <c r="C78" s="209"/>
-      <c r="D78" s="260"/>
+      <c r="D78" s="258"/>
       <c r="E78" s="218"/>
       <c r="F78" s="215"/>
       <c r="G78" s="219"/>
@@ -5607,10 +5669,10 @@
       <c r="N79" s="233"/>
     </row>
     <row r="80" spans="1:14" ht="15.6">
-      <c r="A80" s="242"/>
+      <c r="A80" s="241"/>
       <c r="B80" s="208"/>
       <c r="C80" s="209"/>
-      <c r="D80" s="260"/>
+      <c r="D80" s="258"/>
       <c r="E80" s="218"/>
       <c r="F80" s="215"/>
       <c r="G80" s="219"/>
@@ -5651,10 +5713,10 @@
       <c r="N81" s="233"/>
     </row>
     <row r="82" spans="1:14" ht="15.6">
-      <c r="A82" s="242"/>
+      <c r="A82" s="241"/>
       <c r="B82" s="208"/>
       <c r="C82" s="209"/>
-      <c r="D82" s="260"/>
+      <c r="D82" s="258"/>
       <c r="E82" s="218"/>
       <c r="F82" s="215"/>
       <c r="G82" s="219"/>
@@ -5695,10 +5757,10 @@
       <c r="N83" s="233"/>
     </row>
     <row r="84" spans="1:14" ht="15.6">
-      <c r="A84" s="242"/>
+      <c r="A84" s="241"/>
       <c r="B84" s="208"/>
       <c r="C84" s="209"/>
-      <c r="D84" s="260"/>
+      <c r="D84" s="258"/>
       <c r="E84" s="218"/>
       <c r="F84" s="215"/>
       <c r="G84" s="219"/>
@@ -5739,10 +5801,10 @@
       <c r="N85" s="233"/>
     </row>
     <row r="86" spans="1:14" ht="15.6">
-      <c r="A86" s="242"/>
+      <c r="A86" s="241"/>
       <c r="B86" s="208"/>
       <c r="C86" s="209"/>
-      <c r="D86" s="260"/>
+      <c r="D86" s="258"/>
       <c r="E86" s="218"/>
       <c r="F86" s="215"/>
       <c r="G86" s="219"/>
@@ -5783,10 +5845,10 @@
       <c r="N87" s="233"/>
     </row>
     <row r="88" spans="1:14" ht="15.6">
-      <c r="A88" s="242"/>
+      <c r="A88" s="241"/>
       <c r="B88" s="208"/>
       <c r="C88" s="209"/>
-      <c r="D88" s="260"/>
+      <c r="D88" s="258"/>
       <c r="E88" s="218"/>
       <c r="F88" s="215"/>
       <c r="G88" s="219"/>
@@ -5827,10 +5889,10 @@
       <c r="N89" s="233"/>
     </row>
     <row r="90" spans="1:14" ht="15.6">
-      <c r="A90" s="242"/>
+      <c r="A90" s="241"/>
       <c r="B90" s="208"/>
       <c r="C90" s="209"/>
-      <c r="D90" s="260"/>
+      <c r="D90" s="258"/>
       <c r="E90" s="218"/>
       <c r="F90" s="215"/>
       <c r="G90" s="219"/>
@@ -5871,10 +5933,10 @@
       <c r="N91" s="233"/>
     </row>
     <row r="92" spans="1:14" ht="15.6">
-      <c r="A92" s="242"/>
+      <c r="A92" s="241"/>
       <c r="B92" s="208"/>
       <c r="C92" s="209"/>
-      <c r="D92" s="260"/>
+      <c r="D92" s="258"/>
       <c r="E92" s="218"/>
       <c r="F92" s="215"/>
       <c r="G92" s="219"/>
@@ -5915,10 +5977,10 @@
       <c r="N93" s="233"/>
     </row>
     <row r="94" spans="1:14" ht="15.6">
-      <c r="A94" s="242"/>
+      <c r="A94" s="241"/>
       <c r="B94" s="208"/>
       <c r="C94" s="209"/>
-      <c r="D94" s="260"/>
+      <c r="D94" s="258"/>
       <c r="E94" s="218"/>
       <c r="F94" s="215"/>
       <c r="G94" s="219"/>
@@ -5959,10 +6021,10 @@
       <c r="N95" s="233"/>
     </row>
     <row r="96" spans="1:14" ht="15.6">
-      <c r="A96" s="242"/>
+      <c r="A96" s="241"/>
       <c r="B96" s="208"/>
       <c r="C96" s="209"/>
-      <c r="D96" s="260"/>
+      <c r="D96" s="258"/>
       <c r="E96" s="218"/>
       <c r="F96" s="215"/>
       <c r="G96" s="219"/>
@@ -6003,10 +6065,10 @@
       <c r="N97" s="233"/>
     </row>
     <row r="98" spans="1:14" ht="15.6">
-      <c r="A98" s="242"/>
+      <c r="A98" s="241"/>
       <c r="B98" s="208"/>
       <c r="C98" s="209"/>
-      <c r="D98" s="260"/>
+      <c r="D98" s="258"/>
       <c r="E98" s="218"/>
       <c r="F98" s="215"/>
       <c r="G98" s="219"/>
@@ -6047,10 +6109,10 @@
       <c r="N99" s="233"/>
     </row>
     <row r="100" spans="1:14" ht="15.6">
-      <c r="A100" s="242"/>
+      <c r="A100" s="241"/>
       <c r="B100" s="208"/>
       <c r="C100" s="209"/>
-      <c r="D100" s="260"/>
+      <c r="D100" s="258"/>
       <c r="E100" s="218"/>
       <c r="F100" s="215"/>
       <c r="G100" s="219"/>
@@ -6091,10 +6153,10 @@
       <c r="N101" s="233"/>
     </row>
     <row r="102" spans="1:14" ht="15.6">
-      <c r="A102" s="242"/>
+      <c r="A102" s="241"/>
       <c r="B102" s="208"/>
       <c r="C102" s="209"/>
-      <c r="D102" s="260"/>
+      <c r="D102" s="258"/>
       <c r="E102" s="218"/>
       <c r="F102" s="215"/>
       <c r="G102" s="219"/>
@@ -6135,10 +6197,10 @@
       <c r="N103" s="233"/>
     </row>
     <row r="104" spans="1:14" ht="15.6">
-      <c r="A104" s="242"/>
+      <c r="A104" s="241"/>
       <c r="B104" s="208"/>
       <c r="C104" s="209"/>
-      <c r="D104" s="260"/>
+      <c r="D104" s="258"/>
       <c r="E104" s="218"/>
       <c r="F104" s="215"/>
       <c r="G104" s="219"/>
@@ -6179,10 +6241,10 @@
       <c r="N105" s="233"/>
     </row>
     <row r="106" spans="1:14" ht="15.6">
-      <c r="A106" s="242"/>
+      <c r="A106" s="241"/>
       <c r="B106" s="208"/>
       <c r="C106" s="209"/>
-      <c r="D106" s="260"/>
+      <c r="D106" s="258"/>
       <c r="E106" s="218"/>
       <c r="F106" s="215"/>
       <c r="G106" s="219"/>
@@ -6223,10 +6285,10 @@
       <c r="N107" s="233"/>
     </row>
     <row r="108" spans="1:14" ht="15.6">
-      <c r="A108" s="242"/>
+      <c r="A108" s="241"/>
       <c r="B108" s="208"/>
       <c r="C108" s="209"/>
-      <c r="D108" s="260"/>
+      <c r="D108" s="258"/>
       <c r="E108" s="218"/>
       <c r="F108" s="215"/>
       <c r="G108" s="219"/>
@@ -6267,10 +6329,10 @@
       <c r="N109" s="233"/>
     </row>
     <row r="110" spans="1:14" ht="15.6">
-      <c r="A110" s="242"/>
+      <c r="A110" s="241"/>
       <c r="B110" s="208"/>
       <c r="C110" s="209"/>
-      <c r="D110" s="260"/>
+      <c r="D110" s="258"/>
       <c r="E110" s="218"/>
       <c r="F110" s="215"/>
       <c r="G110" s="219"/>
@@ -6311,10 +6373,10 @@
       <c r="N111" s="233"/>
     </row>
     <row r="112" spans="1:14" ht="15.6">
-      <c r="A112" s="242"/>
+      <c r="A112" s="241"/>
       <c r="B112" s="208"/>
       <c r="C112" s="209"/>
-      <c r="D112" s="260"/>
+      <c r="D112" s="258"/>
       <c r="E112" s="218"/>
       <c r="F112" s="215"/>
       <c r="G112" s="219"/>
@@ -6355,10 +6417,10 @@
       <c r="N113" s="233"/>
     </row>
     <row r="114" spans="1:14" ht="15.6">
-      <c r="A114" s="242"/>
+      <c r="A114" s="241"/>
       <c r="B114" s="208"/>
       <c r="C114" s="209"/>
-      <c r="D114" s="260"/>
+      <c r="D114" s="258"/>
       <c r="E114" s="218"/>
       <c r="F114" s="215"/>
       <c r="G114" s="219"/>
@@ -6399,10 +6461,10 @@
       <c r="N115" s="233"/>
     </row>
     <row r="116" spans="1:14" ht="15.6">
-      <c r="A116" s="242"/>
+      <c r="A116" s="241"/>
       <c r="B116" s="208"/>
       <c r="C116" s="209"/>
-      <c r="D116" s="260"/>
+      <c r="D116" s="258"/>
       <c r="E116" s="218"/>
       <c r="F116" s="215"/>
       <c r="G116" s="219"/>
@@ -6443,10 +6505,10 @@
       <c r="N117" s="233"/>
     </row>
     <row r="118" spans="1:14" ht="15.6">
-      <c r="A118" s="242"/>
+      <c r="A118" s="241"/>
       <c r="B118" s="208"/>
       <c r="C118" s="209"/>
-      <c r="D118" s="260"/>
+      <c r="D118" s="258"/>
       <c r="E118" s="218"/>
       <c r="F118" s="215"/>
       <c r="G118" s="219"/>
@@ -6481,100 +6543,100 @@
       <c r="N119" s="233"/>
     </row>
     <row r="120" spans="1:14">
-      <c r="A120" s="261"/>
-      <c r="B120" s="261"/>
-      <c r="C120" s="261"/>
-      <c r="D120" s="261"/>
-      <c r="E120" s="261"/>
-      <c r="F120" s="261"/>
-      <c r="G120" s="262"/>
-      <c r="H120" s="261"/>
-      <c r="I120" s="261"/>
-      <c r="J120" s="261"/>
-      <c r="K120" s="261"/>
-      <c r="L120" s="261"/>
-      <c r="M120" s="261"/>
-      <c r="N120" s="261"/>
+      <c r="A120" s="259"/>
+      <c r="B120" s="259"/>
+      <c r="C120" s="259"/>
+      <c r="D120" s="259"/>
+      <c r="E120" s="259"/>
+      <c r="F120" s="259"/>
+      <c r="G120" s="260"/>
+      <c r="H120" s="259"/>
+      <c r="I120" s="259"/>
+      <c r="J120" s="259"/>
+      <c r="K120" s="259"/>
+      <c r="L120" s="259"/>
+      <c r="M120" s="259"/>
+      <c r="N120" s="259"/>
     </row>
     <row r="121" spans="1:14">
-      <c r="A121" s="261"/>
-      <c r="B121" s="261"/>
-      <c r="C121" s="261"/>
-      <c r="D121" s="261"/>
-      <c r="E121" s="261"/>
-      <c r="F121" s="261"/>
-      <c r="G121" s="262"/>
-      <c r="H121" s="261"/>
-      <c r="I121" s="261"/>
-      <c r="J121" s="261"/>
-      <c r="K121" s="261"/>
-      <c r="L121" s="261"/>
-      <c r="M121" s="261"/>
-      <c r="N121" s="261"/>
+      <c r="A121" s="259"/>
+      <c r="B121" s="259"/>
+      <c r="C121" s="259"/>
+      <c r="D121" s="259"/>
+      <c r="E121" s="259"/>
+      <c r="F121" s="259"/>
+      <c r="G121" s="260"/>
+      <c r="H121" s="259"/>
+      <c r="I121" s="259"/>
+      <c r="J121" s="259"/>
+      <c r="K121" s="259"/>
+      <c r="L121" s="259"/>
+      <c r="M121" s="259"/>
+      <c r="N121" s="259"/>
     </row>
     <row r="122" spans="1:14">
-      <c r="A122" s="261"/>
-      <c r="B122" s="261"/>
-      <c r="C122" s="261"/>
-      <c r="D122" s="261"/>
-      <c r="E122" s="261"/>
-      <c r="F122" s="261"/>
-      <c r="G122" s="262"/>
-      <c r="H122" s="261"/>
-      <c r="I122" s="261"/>
-      <c r="J122" s="261"/>
-      <c r="K122" s="261"/>
-      <c r="L122" s="261"/>
-      <c r="M122" s="261"/>
-      <c r="N122" s="261"/>
+      <c r="A122" s="259"/>
+      <c r="B122" s="259"/>
+      <c r="C122" s="259"/>
+      <c r="D122" s="259"/>
+      <c r="E122" s="259"/>
+      <c r="F122" s="259"/>
+      <c r="G122" s="260"/>
+      <c r="H122" s="259"/>
+      <c r="I122" s="259"/>
+      <c r="J122" s="259"/>
+      <c r="K122" s="259"/>
+      <c r="L122" s="259"/>
+      <c r="M122" s="259"/>
+      <c r="N122" s="259"/>
     </row>
     <row r="123" spans="1:14">
-      <c r="A123" s="261"/>
-      <c r="B123" s="261"/>
-      <c r="C123" s="261"/>
-      <c r="D123" s="261"/>
-      <c r="E123" s="261"/>
-      <c r="F123" s="261"/>
-      <c r="G123" s="262"/>
-      <c r="H123" s="261"/>
-      <c r="I123" s="261"/>
-      <c r="J123" s="261"/>
-      <c r="K123" s="261"/>
-      <c r="L123" s="261"/>
-      <c r="M123" s="261"/>
-      <c r="N123" s="261"/>
+      <c r="A123" s="259"/>
+      <c r="B123" s="259"/>
+      <c r="C123" s="259"/>
+      <c r="D123" s="259"/>
+      <c r="E123" s="259"/>
+      <c r="F123" s="259"/>
+      <c r="G123" s="260"/>
+      <c r="H123" s="259"/>
+      <c r="I123" s="259"/>
+      <c r="J123" s="259"/>
+      <c r="K123" s="259"/>
+      <c r="L123" s="259"/>
+      <c r="M123" s="259"/>
+      <c r="N123" s="259"/>
     </row>
     <row r="124" spans="1:14">
-      <c r="A124" s="261"/>
-      <c r="B124" s="261"/>
-      <c r="C124" s="261"/>
-      <c r="D124" s="261"/>
-      <c r="E124" s="261"/>
-      <c r="F124" s="261"/>
-      <c r="G124" s="262"/>
-      <c r="H124" s="261"/>
-      <c r="I124" s="261"/>
-      <c r="J124" s="261"/>
-      <c r="K124" s="261"/>
-      <c r="L124" s="261"/>
-      <c r="M124" s="261"/>
-      <c r="N124" s="261"/>
+      <c r="A124" s="259"/>
+      <c r="B124" s="259"/>
+      <c r="C124" s="259"/>
+      <c r="D124" s="259"/>
+      <c r="E124" s="259"/>
+      <c r="F124" s="259"/>
+      <c r="G124" s="260"/>
+      <c r="H124" s="259"/>
+      <c r="I124" s="259"/>
+      <c r="J124" s="259"/>
+      <c r="K124" s="259"/>
+      <c r="L124" s="259"/>
+      <c r="M124" s="259"/>
+      <c r="N124" s="259"/>
     </row>
     <row r="125" spans="1:14">
-      <c r="A125" s="261"/>
-      <c r="B125" s="261"/>
-      <c r="C125" s="261"/>
-      <c r="D125" s="261"/>
-      <c r="E125" s="261"/>
-      <c r="F125" s="261"/>
-      <c r="G125" s="262"/>
-      <c r="H125" s="261"/>
-      <c r="I125" s="261"/>
-      <c r="J125" s="261"/>
-      <c r="K125" s="261"/>
-      <c r="L125" s="261"/>
-      <c r="M125" s="261"/>
-      <c r="N125" s="261"/>
+      <c r="A125" s="259"/>
+      <c r="B125" s="259"/>
+      <c r="C125" s="259"/>
+      <c r="D125" s="259"/>
+      <c r="E125" s="259"/>
+      <c r="F125" s="259"/>
+      <c r="G125" s="260"/>
+      <c r="H125" s="259"/>
+      <c r="I125" s="259"/>
+      <c r="J125" s="259"/>
+      <c r="K125" s="259"/>
+      <c r="L125" s="259"/>
+      <c r="M125" s="259"/>
+      <c r="N125" s="259"/>
     </row>
   </sheetData>
   <autoFilter ref="A4:N118"/>
@@ -6633,40 +6695,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="25.2" thickBot="1">
-      <c r="A1" s="290" t="s">
+      <c r="A1" s="288" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="290"/>
-      <c r="C1" s="290"/>
-      <c r="D1" s="290"/>
-      <c r="E1" s="290"/>
-      <c r="F1" s="290"/>
-      <c r="G1" s="290"/>
-      <c r="H1" s="290"/>
-      <c r="I1" s="290"/>
-      <c r="J1" s="290"/>
-      <c r="K1" s="290"/>
+      <c r="B1" s="288"/>
+      <c r="C1" s="288"/>
+      <c r="D1" s="288"/>
+      <c r="E1" s="288"/>
+      <c r="F1" s="288"/>
+      <c r="G1" s="288"/>
+      <c r="H1" s="288"/>
+      <c r="I1" s="288"/>
+      <c r="J1" s="288"/>
+      <c r="K1" s="288"/>
       <c r="L1" s="70"/>
       <c r="M1" s="70"/>
       <c r="N1" s="70"/>
     </row>
-    <row r="2" spans="1:15" s="288" customFormat="1" ht="23.4" thickTop="1"/>
+    <row r="2" spans="1:15" s="286" customFormat="1" ht="23.4" thickTop="1"/>
     <row r="3" spans="1:15" ht="21">
-      <c r="A3" s="291" t="s">
+      <c r="A3" s="289" t="s">
         <v>49</v>
       </c>
-      <c r="B3" s="291"/>
-      <c r="C3" s="291"/>
+      <c r="B3" s="289"/>
+      <c r="C3" s="289"/>
       <c r="D3" s="67">
         <f>SUM(K6:K180)</f>
         <v>753.6</v>
       </c>
       <c r="E3" s="110"/>
-      <c r="F3" s="291" t="s">
+      <c r="F3" s="289" t="s">
         <v>50</v>
       </c>
-      <c r="G3" s="291"/>
-      <c r="H3" s="291"/>
+      <c r="G3" s="289"/>
+      <c r="H3" s="289"/>
       <c r="I3" s="68">
         <f>SUM(L6:L181)</f>
         <v>111.38</v>
@@ -6694,7 +6756,7 @@
         <v>69</v>
       </c>
       <c r="F4" s="63" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G4" s="63" t="s">
         <v>70</v>
@@ -6735,16 +6797,16 @@
         <v>33</v>
       </c>
       <c r="D5" s="75" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E5" s="39" t="s">
+        <v>93</v>
+      </c>
+      <c r="F5" s="39" t="s">
+        <v>109</v>
+      </c>
+      <c r="G5" s="39" t="s">
         <v>94</v>
-      </c>
-      <c r="F5" s="39" t="s">
-        <v>110</v>
-      </c>
-      <c r="G5" s="39" t="s">
-        <v>95</v>
       </c>
       <c r="H5" s="40" t="s">
         <v>31</v>
@@ -6762,7 +6824,7 @@
         <v>35</v>
       </c>
       <c r="M5" s="39" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="N5" s="74" t="s">
         <v>80</v>
@@ -6776,20 +6838,20 @@
         <v>1</v>
       </c>
       <c r="B6" s="80" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C6" s="90" t="s">
         <v>0</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E6" s="76" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F6" s="76"/>
       <c r="G6" s="10" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H6" s="11"/>
       <c r="I6" s="43"/>
@@ -6817,14 +6879,14 @@
         <v>1</v>
       </c>
       <c r="D7" s="114" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E7" s="77" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F7" s="77"/>
       <c r="G7" s="12" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H7" s="13"/>
       <c r="I7" s="47"/>
@@ -6852,14 +6914,14 @@
         <v>2</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E8" s="71" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F8" s="71"/>
       <c r="G8" s="10" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H8" s="45"/>
       <c r="I8" s="48"/>
@@ -6884,19 +6946,19 @@
         <v>16</v>
       </c>
       <c r="C9" s="91" t="s">
+        <v>124</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="E9" s="71" t="s">
+        <v>99</v>
+      </c>
+      <c r="F9" s="71" t="s">
         <v>125</v>
       </c>
-      <c r="D9" s="9" t="s">
-        <v>111</v>
-      </c>
-      <c r="E9" s="71" t="s">
-        <v>100</v>
-      </c>
-      <c r="F9" s="71" t="s">
-        <v>126</v>
-      </c>
       <c r="G9" s="111" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H9" s="45">
         <v>0</v>
@@ -6930,14 +6992,14 @@
         <v>3</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E10" s="71" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F10" s="71"/>
       <c r="G10" s="10" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H10" s="45"/>
       <c r="I10" s="48"/>
@@ -6967,16 +7029,16 @@
         <v>4</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E11" s="71" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F11" s="71" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G11" s="10" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H11" s="45"/>
       <c r="I11" s="48"/>
@@ -7006,14 +7068,14 @@
         <v>5</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E12" s="71" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F12" s="71"/>
       <c r="G12" s="10" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H12" s="45"/>
       <c r="I12" s="48"/>
@@ -7043,14 +7105,14 @@
         <v>6</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E13" s="71" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F13" s="71"/>
       <c r="G13" s="87" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H13" s="45"/>
       <c r="I13" s="48"/>
@@ -7078,16 +7140,16 @@
         <v>7</v>
       </c>
       <c r="D14" s="113" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E14" s="72" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F14" s="72" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G14" s="10" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H14" s="11"/>
       <c r="I14" s="54"/>
@@ -7115,16 +7177,16 @@
         <v>8</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E15" s="71" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F15" s="71" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G15" s="10" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H15" s="45"/>
       <c r="I15" s="48"/>
@@ -7152,14 +7214,14 @@
         <v>9</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E16" s="72" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F16" s="72"/>
       <c r="G16" s="10" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H16" s="11"/>
       <c r="I16" s="54"/>
@@ -7187,14 +7249,14 @@
         <v>10</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E17" s="71" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F17" s="71"/>
       <c r="G17" s="87" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H17" s="45">
         <v>0</v>
@@ -7228,14 +7290,14 @@
         <v>11</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E18" s="72" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F18" s="72"/>
       <c r="G18" s="10" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H18" s="11"/>
       <c r="I18" s="54"/>
@@ -7263,14 +7325,14 @@
         <v>12</v>
       </c>
       <c r="D19" s="113" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E19" s="78" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F19" s="78"/>
       <c r="G19" s="10" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H19" s="45"/>
       <c r="I19" s="48"/>
@@ -7292,20 +7354,20 @@
         <v>15</v>
       </c>
       <c r="B20" s="81" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C20" s="97" t="s">
         <v>25</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E20" s="79" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F20" s="112"/>
       <c r="G20" s="10" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H20" s="11"/>
       <c r="I20" s="54"/>
@@ -7333,14 +7395,14 @@
         <v>26</v>
       </c>
       <c r="D21" s="120" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E21" s="78" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F21" s="78"/>
       <c r="G21" s="121" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H21" s="122"/>
       <c r="I21" s="123"/>
@@ -7379,11 +7441,11 @@
       <c r="B23" s="140"/>
       <c r="C23" s="141"/>
       <c r="D23" s="146" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E23" s="139"/>
       <c r="F23" s="154" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G23" s="142"/>
       <c r="H23" s="143"/>
@@ -7423,16 +7485,16 @@
         <v>33</v>
       </c>
       <c r="D25" s="164" t="s">
+        <v>118</v>
+      </c>
+      <c r="E25" s="165" t="s">
         <v>119</v>
       </c>
-      <c r="E25" s="165" t="s">
+      <c r="F25" s="165" t="s">
         <v>120</v>
       </c>
-      <c r="F25" s="165" t="s">
+      <c r="G25" s="166" t="s">
         <v>121</v>
-      </c>
-      <c r="G25" s="166" t="s">
-        <v>122</v>
       </c>
       <c r="H25" s="167" t="s">
         <v>31</v>
@@ -7450,7 +7512,7 @@
         <v>35</v>
       </c>
       <c r="M25" s="168" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="N25" s="168" t="s">
         <v>80</v>
@@ -7464,7 +7526,7 @@
         <v>1</v>
       </c>
       <c r="B26" s="127" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C26" s="128" t="s">
         <v>0</v>
@@ -7621,10 +7683,10 @@
         <v>4</v>
       </c>
       <c r="D31" s="173" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E31" s="149" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F31" s="181">
         <v>128893</v>
@@ -7653,7 +7715,7 @@
         <v>54</v>
       </c>
       <c r="N31" s="111" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="O31" s="11" t="s">
         <v>41</v>
@@ -7786,10 +7848,10 @@
         <v>9</v>
       </c>
       <c r="D36" s="173" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E36" s="150" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F36" s="176">
         <v>226526</v>
@@ -7818,10 +7880,10 @@
         <v>54</v>
       </c>
       <c r="N36" s="111" t="s">
+        <v>129</v>
+      </c>
+      <c r="O36" s="102" t="s">
         <v>130</v>
-      </c>
-      <c r="O36" s="102" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="37" spans="1:15" s="46" customFormat="1" ht="15.6">
@@ -7922,7 +7984,7 @@
         <v>15</v>
       </c>
       <c r="B40" s="81" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C40" s="97" t="s">
         <v>25</v>

</xml_diff>

<commit_message>
Atualizando dados da planilha
</commit_message>
<xml_diff>
--- a/GESTÃO MANUTENÇÃO.xlsx
+++ b/GESTÃO MANUTENÇÃO.xlsx
@@ -1989,6 +1989,15 @@
     <xf numFmtId="44" fontId="7" fillId="2" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -2000,15 +2009,6 @@
     </xf>
     <xf numFmtId="0" fontId="18" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2819,7 +2819,7 @@
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D26" sqref="C26:D30"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -3086,8 +3086,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E43" sqref="E43"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -3109,16 +3109,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="25.2" thickBot="1">
-      <c r="A1" s="288" t="s">
+      <c r="A1" s="291" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="288"/>
-      <c r="C1" s="288"/>
-      <c r="D1" s="288"/>
-      <c r="E1" s="288"/>
-      <c r="F1" s="288"/>
-      <c r="G1" s="288"/>
-      <c r="H1" s="288"/>
+      <c r="B1" s="291"/>
+      <c r="C1" s="291"/>
+      <c r="D1" s="291"/>
+      <c r="E1" s="291"/>
+      <c r="F1" s="291"/>
+      <c r="G1" s="291"/>
+      <c r="H1" s="291"/>
       <c r="I1" s="70"/>
       <c r="J1" s="70"/>
       <c r="K1" s="70"/>
@@ -3126,13 +3126,13 @@
       <c r="M1" s="182"/>
       <c r="N1" s="178"/>
     </row>
-    <row r="2" spans="1:14" s="286" customFormat="1" ht="23.4" thickTop="1"/>
+    <row r="2" spans="1:14" s="289" customFormat="1" ht="23.4" thickTop="1"/>
     <row r="3" spans="1:14" ht="26.4">
-      <c r="A3" s="287" t="s">
+      <c r="A3" s="290" t="s">
         <v>49</v>
       </c>
-      <c r="B3" s="287"/>
-      <c r="C3" s="287"/>
+      <c r="B3" s="290"/>
+      <c r="C3" s="290"/>
       <c r="D3" s="184">
         <f>SUM(J5:J172)</f>
         <v>84250.559999999998</v>
@@ -3144,11 +3144,11 @@
         <f>D3+J3</f>
         <v>130689.45999999999</v>
       </c>
-      <c r="G3" s="287" t="s">
+      <c r="G3" s="290" t="s">
         <v>50</v>
       </c>
-      <c r="H3" s="287"/>
-      <c r="I3" s="287"/>
+      <c r="H3" s="290"/>
+      <c r="I3" s="290"/>
       <c r="J3" s="187">
         <f>SUM(K5:K173)</f>
         <v>46438.9</v>
@@ -3219,7 +3219,7 @@
         <v>154</v>
       </c>
       <c r="F5" s="266" t="s">
-        <v>44</v>
+        <v>88</v>
       </c>
       <c r="G5" s="276">
         <v>3000</v>
@@ -3265,7 +3265,7 @@
         <v>101</v>
       </c>
       <c r="F6" s="212" t="s">
-        <v>44</v>
+        <v>88</v>
       </c>
       <c r="G6" s="213">
         <v>1520</v>
@@ -3357,7 +3357,7 @@
         <v>131</v>
       </c>
       <c r="F8" s="212" t="s">
-        <v>44</v>
+        <v>88</v>
       </c>
       <c r="G8" s="213">
         <v>714.4</v>
@@ -3403,7 +3403,7 @@
         <v>97</v>
       </c>
       <c r="F9" s="266" t="s">
-        <v>44</v>
+        <v>88</v>
       </c>
       <c r="G9" s="276">
         <v>180</v>
@@ -3495,7 +3495,7 @@
         <v>92</v>
       </c>
       <c r="F11" s="222" t="s">
-        <v>44</v>
+        <v>88</v>
       </c>
       <c r="G11" s="204">
         <v>1246</v>
@@ -3758,7 +3758,7 @@
       <c r="A17" s="216">
         <v>14</v>
       </c>
-      <c r="B17" s="290" t="s">
+      <c r="B17" s="286" t="s">
         <v>163</v>
       </c>
       <c r="C17" s="201" t="s">
@@ -3863,7 +3863,7 @@
         <v>63</v>
       </c>
       <c r="F19" s="203" t="s">
-        <v>44</v>
+        <v>88</v>
       </c>
       <c r="G19" s="204">
         <v>850</v>
@@ -4034,7 +4034,7 @@
       <c r="A23" s="216">
         <v>5</v>
       </c>
-      <c r="B23" s="291" t="s">
+      <c r="B23" s="287" t="s">
         <v>167</v>
       </c>
       <c r="C23" s="201" t="s">
@@ -4277,7 +4277,7 @@
         <v>137</v>
       </c>
       <c r="F28" s="215" t="s">
-        <v>44</v>
+        <v>88</v>
       </c>
       <c r="G28" s="219">
         <v>160</v>
@@ -4323,7 +4323,7 @@
         <v>117</v>
       </c>
       <c r="F29" s="203" t="s">
-        <v>44</v>
+        <v>88</v>
       </c>
       <c r="G29" s="204">
         <v>600</v>
@@ -4415,7 +4415,7 @@
         <v>136</v>
       </c>
       <c r="F31" s="222" t="s">
-        <v>44</v>
+        <v>88</v>
       </c>
       <c r="G31" s="263">
         <v>2849.9</v>
@@ -4721,7 +4721,7 @@
       </c>
     </row>
     <row r="38" spans="1:14" ht="15.6">
-      <c r="A38" s="292">
+      <c r="A38" s="288">
         <v>4</v>
       </c>
       <c r="B38" s="283" t="s">
@@ -6695,40 +6695,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="25.2" thickBot="1">
-      <c r="A1" s="288" t="s">
+      <c r="A1" s="291" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="288"/>
-      <c r="C1" s="288"/>
-      <c r="D1" s="288"/>
-      <c r="E1" s="288"/>
-      <c r="F1" s="288"/>
-      <c r="G1" s="288"/>
-      <c r="H1" s="288"/>
-      <c r="I1" s="288"/>
-      <c r="J1" s="288"/>
-      <c r="K1" s="288"/>
+      <c r="B1" s="291"/>
+      <c r="C1" s="291"/>
+      <c r="D1" s="291"/>
+      <c r="E1" s="291"/>
+      <c r="F1" s="291"/>
+      <c r="G1" s="291"/>
+      <c r="H1" s="291"/>
+      <c r="I1" s="291"/>
+      <c r="J1" s="291"/>
+      <c r="K1" s="291"/>
       <c r="L1" s="70"/>
       <c r="M1" s="70"/>
       <c r="N1" s="70"/>
     </row>
-    <row r="2" spans="1:15" s="286" customFormat="1" ht="23.4" thickTop="1"/>
+    <row r="2" spans="1:15" s="289" customFormat="1" ht="23.4" thickTop="1"/>
     <row r="3" spans="1:15" ht="21">
-      <c r="A3" s="289" t="s">
+      <c r="A3" s="292" t="s">
         <v>49</v>
       </c>
-      <c r="B3" s="289"/>
-      <c r="C3" s="289"/>
+      <c r="B3" s="292"/>
+      <c r="C3" s="292"/>
       <c r="D3" s="67">
         <f>SUM(K6:K180)</f>
         <v>753.6</v>
       </c>
       <c r="E3" s="110"/>
-      <c r="F3" s="289" t="s">
+      <c r="F3" s="292" t="s">
         <v>50</v>
       </c>
-      <c r="G3" s="289"/>
-      <c r="H3" s="289"/>
+      <c r="G3" s="292"/>
+      <c r="H3" s="292"/>
       <c r="I3" s="68">
         <f>SUM(L6:L181)</f>
         <v>111.38</v>

</xml_diff>

<commit_message>
chore: atualização dos dados da planilha
</commit_message>
<xml_diff>
--- a/GESTÃO MANUTENÇÃO.xlsx
+++ b/GESTÃO MANUTENÇÃO.xlsx
@@ -1908,6 +1908,72 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="7" fillId="0" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="17" fillId="0" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="9" fillId="0" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="7" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="9" fillId="2" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="44" fontId="17" fillId="2" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="5" fillId="2" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="7" fillId="2" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="6" fillId="2" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="25" fillId="2" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1919,72 +1985,6 @@
     </xf>
     <xf numFmtId="0" fontId="18" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="7" fillId="0" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="6" fillId="0" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="17" fillId="0" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="7" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="9" fillId="0" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="7" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="9" fillId="2" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="44" fontId="17" fillId="2" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="5" fillId="2" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="7" fillId="2" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="6" fillId="2" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="25" fillId="2" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3062,8 +3062,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N125"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A40" sqref="A40"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -3085,16 +3085,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="25.2" thickBot="1">
-      <c r="A1" s="257" t="s">
+      <c r="A1" s="279" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="257"/>
-      <c r="C1" s="257"/>
-      <c r="D1" s="257"/>
-      <c r="E1" s="257"/>
-      <c r="F1" s="257"/>
-      <c r="G1" s="257"/>
-      <c r="H1" s="257"/>
+      <c r="B1" s="279"/>
+      <c r="C1" s="279"/>
+      <c r="D1" s="279"/>
+      <c r="E1" s="279"/>
+      <c r="F1" s="279"/>
+      <c r="G1" s="279"/>
+      <c r="H1" s="279"/>
       <c r="I1" s="70"/>
       <c r="J1" s="70"/>
       <c r="K1" s="70"/>
@@ -3102,32 +3102,32 @@
       <c r="M1" s="182"/>
       <c r="N1" s="178"/>
     </row>
-    <row r="2" spans="1:14" s="255" customFormat="1" ht="23.4" thickTop="1"/>
+    <row r="2" spans="1:14" s="277" customFormat="1" ht="23.4" thickTop="1"/>
     <row r="3" spans="1:14" ht="26.4">
-      <c r="A3" s="256" t="s">
+      <c r="A3" s="278" t="s">
         <v>49</v>
       </c>
-      <c r="B3" s="256"/>
-      <c r="C3" s="256"/>
+      <c r="B3" s="278"/>
+      <c r="C3" s="278"/>
       <c r="D3" s="184">
         <f>SUMIFS(J5:J1000, M5:M1000, "REALIZADO") + SUMIFS(J5:J1000, M5:M1000, "ENVIADO P/ APROVAÇÃO")</f>
-        <v>76900.56</v>
+        <v>84100.56</v>
       </c>
       <c r="E3" s="185" t="s">
         <v>144</v>
       </c>
       <c r="F3" s="186">
         <f>D3+J3</f>
-        <v>118445.45999999999</v>
-      </c>
-      <c r="G3" s="256" t="s">
+        <v>126136.95999999999</v>
+      </c>
+      <c r="G3" s="278" t="s">
         <v>50</v>
       </c>
-      <c r="H3" s="256"/>
-      <c r="I3" s="256"/>
+      <c r="H3" s="278"/>
+      <c r="I3" s="278"/>
       <c r="J3" s="187">
         <f>SUMIFS(K5:K1000, M5:M1000, "REALIZADO") + SUMIFS(K5:K1000, M5:M1000, "ENVIADO P/ APROVAÇÃO")</f>
-        <v>41544.9</v>
+        <v>42036.4</v>
       </c>
       <c r="K3" s="188"/>
       <c r="L3" s="189"/>
@@ -3207,11 +3207,11 @@
         <v>7200</v>
       </c>
       <c r="J5" s="232">
-        <f>MIN(G5:I5)</f>
+        <f t="shared" ref="J5:J36" si="0">MIN(G5:I5)</f>
         <v>6123.26</v>
       </c>
       <c r="K5" s="232">
-        <f>MAX(G5:I5) - J5</f>
+        <f t="shared" ref="K5:K36" si="1">MAX(G5:I5) - J5</f>
         <v>1076.7399999999998</v>
       </c>
       <c r="L5" s="232" t="s">
@@ -3220,7 +3220,7 @@
       <c r="M5" s="246" t="s">
         <v>82</v>
       </c>
-      <c r="N5" s="259" t="s">
+      <c r="N5" s="255" t="s">
         <v>41</v>
       </c>
     </row>
@@ -3253,17 +3253,17 @@
         <v>3280</v>
       </c>
       <c r="J6" s="209">
-        <f>MIN(G6:I6)</f>
+        <f t="shared" si="0"/>
         <v>2800</v>
       </c>
       <c r="K6" s="209">
-        <f>MAX(G6:I6) - J6</f>
+        <f t="shared" si="1"/>
         <v>480</v>
       </c>
       <c r="L6" s="209" t="s">
         <v>54</v>
       </c>
-      <c r="M6" s="277" t="s">
+      <c r="M6" s="273" t="s">
         <v>83</v>
       </c>
       <c r="N6" s="249" t="s">
@@ -3295,18 +3295,18 @@
       <c r="H7" s="243">
         <v>950</v>
       </c>
-      <c r="I7" s="260">
+      <c r="I7" s="256">
         <v>870</v>
       </c>
       <c r="J7" s="232">
-        <f>MIN(G7:I7)</f>
+        <f t="shared" si="0"/>
         <v>870</v>
       </c>
       <c r="K7" s="232">
-        <f>MAX(G7:I7) - J7</f>
+        <f t="shared" si="1"/>
         <v>376</v>
       </c>
-      <c r="L7" s="260" t="s">
+      <c r="L7" s="256" t="s">
         <v>54</v>
       </c>
       <c r="M7" s="246" t="s">
@@ -3345,11 +3345,11 @@
         <v>1400</v>
       </c>
       <c r="J8" s="209">
-        <f>MIN(G8:I8)</f>
+        <f t="shared" si="0"/>
         <v>1400</v>
       </c>
       <c r="K8" s="209">
-        <f>MAX(G8:I8) - J8</f>
+        <f t="shared" si="1"/>
         <v>470</v>
       </c>
       <c r="L8" s="209" t="s">
@@ -3366,7 +3366,7 @@
       <c r="A9" s="241" t="s">
         <v>45</v>
       </c>
-      <c r="B9" s="261" t="s">
+      <c r="B9" s="257" t="s">
         <v>46</v>
       </c>
       <c r="C9" s="240" t="s">
@@ -3391,11 +3391,11 @@
         <v>6845</v>
       </c>
       <c r="J9" s="232">
-        <f>MIN(G9:I9)</f>
+        <f t="shared" si="0"/>
         <v>6345</v>
       </c>
       <c r="K9" s="232">
-        <f>MAX(G9:I9) - J9</f>
+        <f t="shared" si="1"/>
         <v>1630</v>
       </c>
       <c r="L9" s="232" t="s">
@@ -3404,7 +3404,7 @@
       <c r="M9" s="246" t="s">
         <v>82</v>
       </c>
-      <c r="N9" s="259" t="s">
+      <c r="N9" s="255" t="s">
         <v>41</v>
       </c>
     </row>
@@ -3437,11 +3437,11 @@
         <v>1389.9</v>
       </c>
       <c r="J10" s="209">
-        <f>MIN(G10:I10)</f>
+        <f t="shared" si="0"/>
         <v>1389.9</v>
       </c>
       <c r="K10" s="209">
-        <f>MAX(G10:I10) - J10</f>
+        <f t="shared" si="1"/>
         <v>956.07999999999993</v>
       </c>
       <c r="L10" s="209" t="s">
@@ -3483,11 +3483,11 @@
         <v>6680</v>
       </c>
       <c r="J11" s="232">
-        <f>MIN(G11:I11)</f>
+        <f t="shared" si="0"/>
         <v>6680</v>
       </c>
       <c r="K11" s="232">
-        <f>MAX(G11:I11) - J11</f>
+        <f t="shared" si="1"/>
         <v>455.97999999999956</v>
       </c>
       <c r="L11" s="232" t="s">
@@ -3496,7 +3496,7 @@
       <c r="M11" s="246" t="s">
         <v>82</v>
       </c>
-      <c r="N11" s="259" t="s">
+      <c r="N11" s="255" t="s">
         <v>41</v>
       </c>
     </row>
@@ -3504,7 +3504,7 @@
       <c r="A12" s="250">
         <v>15</v>
       </c>
-      <c r="B12" s="270" t="s">
+      <c r="B12" s="266" t="s">
         <v>164</v>
       </c>
       <c r="C12" s="221" t="s">
@@ -3529,11 +3529,11 @@
         <v>700</v>
       </c>
       <c r="J12" s="209">
-        <f>MIN(G12:I12)</f>
+        <f t="shared" si="0"/>
         <v>700</v>
       </c>
       <c r="K12" s="209">
-        <f>MAX(G12:I12) - J12</f>
+        <f t="shared" si="1"/>
         <v>280</v>
       </c>
       <c r="L12" s="209" t="s">
@@ -3575,11 +3575,11 @@
         <v>17517.5</v>
       </c>
       <c r="J13" s="232">
-        <f>MIN(G13:I13)</f>
+        <f t="shared" si="0"/>
         <v>10100</v>
       </c>
       <c r="K13" s="232">
-        <f>MAX(G13:I13) - J13</f>
+        <f t="shared" si="1"/>
         <v>7417.5</v>
       </c>
       <c r="L13" s="232" t="s">
@@ -3588,7 +3588,7 @@
       <c r="M13" s="246" t="s">
         <v>82</v>
       </c>
-      <c r="N13" s="259" t="s">
+      <c r="N13" s="255" t="s">
         <v>40</v>
       </c>
     </row>
@@ -3596,7 +3596,7 @@
       <c r="A14" s="250">
         <v>14</v>
       </c>
-      <c r="B14" s="270" t="s">
+      <c r="B14" s="266" t="s">
         <v>163</v>
       </c>
       <c r="C14" s="221" t="s">
@@ -3621,11 +3621,11 @@
         <v>400</v>
       </c>
       <c r="J14" s="209">
-        <f>MIN(G14:I14)</f>
+        <f t="shared" si="0"/>
         <v>400</v>
       </c>
       <c r="K14" s="209">
-        <f>MAX(G14:I14) - J14</f>
+        <f t="shared" si="1"/>
         <v>300</v>
       </c>
       <c r="L14" s="209" t="s">
@@ -3667,11 +3667,11 @@
         <v>2000</v>
       </c>
       <c r="J15" s="232">
-        <f>MIN(G15:I15)</f>
+        <f t="shared" si="0"/>
         <v>2000</v>
       </c>
       <c r="K15" s="232">
-        <f>MAX(G15:I15) - J15</f>
+        <f t="shared" si="1"/>
         <v>999</v>
       </c>
       <c r="L15" s="232" t="s">
@@ -3680,7 +3680,7 @@
       <c r="M15" s="246" t="s">
         <v>82</v>
       </c>
-      <c r="N15" s="259" t="s">
+      <c r="N15" s="255" t="s">
         <v>40</v>
       </c>
     </row>
@@ -3688,7 +3688,7 @@
       <c r="A16" s="254">
         <v>14</v>
       </c>
-      <c r="B16" s="270" t="s">
+      <c r="B16" s="266" t="s">
         <v>163</v>
       </c>
       <c r="C16" s="254" t="s">
@@ -3713,11 +3713,11 @@
         <v>545</v>
       </c>
       <c r="J16" s="209">
-        <f>MIN(G16:I16)</f>
+        <f t="shared" si="0"/>
         <v>300</v>
       </c>
       <c r="K16" s="209">
-        <f>MAX(G16:I16) - J16</f>
+        <f t="shared" si="1"/>
         <v>400</v>
       </c>
       <c r="L16" s="209" t="s">
@@ -3726,7 +3726,7 @@
       <c r="M16" s="222" t="s">
         <v>82</v>
       </c>
-      <c r="N16" s="270" t="s">
+      <c r="N16" s="266" t="s">
         <v>40</v>
       </c>
     </row>
@@ -3759,11 +3759,11 @@
         <v>650</v>
       </c>
       <c r="J17" s="232">
-        <f>MIN(G17:I17)</f>
+        <f t="shared" si="0"/>
         <v>600</v>
       </c>
       <c r="K17" s="232">
-        <f>MAX(G17:I17) - J17</f>
+        <f t="shared" si="1"/>
         <v>185</v>
       </c>
       <c r="L17" s="232" t="s">
@@ -3805,11 +3805,11 @@
         <v>800</v>
       </c>
       <c r="J18" s="209">
-        <f>MIN(G18:I18)</f>
+        <f t="shared" si="0"/>
         <v>660.4</v>
       </c>
       <c r="K18" s="209">
-        <f>MAX(G18:I18) - J18</f>
+        <f t="shared" si="1"/>
         <v>139.60000000000002</v>
       </c>
       <c r="L18" s="251" t="s">
@@ -3835,13 +3835,13 @@
       <c r="D19" s="240">
         <v>45740</v>
       </c>
-      <c r="E19" s="262" t="s">
+      <c r="E19" s="258" t="s">
         <v>86</v>
       </c>
-      <c r="F19" s="263" t="s">
+      <c r="F19" s="259" t="s">
         <v>44</v>
       </c>
-      <c r="G19" s="264">
+      <c r="G19" s="260">
         <v>6500</v>
       </c>
       <c r="H19" s="243">
@@ -3851,11 +3851,11 @@
         <v>6348.9</v>
       </c>
       <c r="J19" s="232">
-        <f>MIN(G19:I19)</f>
+        <f t="shared" si="0"/>
         <v>5736</v>
       </c>
       <c r="K19" s="232">
-        <f>MAX(G19:I19) - J19</f>
+        <f t="shared" si="1"/>
         <v>764</v>
       </c>
       <c r="L19" s="232" t="s">
@@ -3864,7 +3864,7 @@
       <c r="M19" s="246" t="s">
         <v>82</v>
       </c>
-      <c r="N19" s="259" t="s">
+      <c r="N19" s="255" t="s">
         <v>41</v>
       </c>
     </row>
@@ -3872,7 +3872,7 @@
       <c r="A20" s="250">
         <v>5</v>
       </c>
-      <c r="B20" s="274" t="s">
+      <c r="B20" s="270" t="s">
         <v>167</v>
       </c>
       <c r="C20" s="221" t="s">
@@ -3881,10 +3881,10 @@
       <c r="D20" s="221">
         <v>45740</v>
       </c>
-      <c r="E20" s="275" t="s">
+      <c r="E20" s="271" t="s">
         <v>89</v>
       </c>
-      <c r="F20" s="276" t="s">
+      <c r="F20" s="272" t="s">
         <v>44</v>
       </c>
       <c r="G20" s="210">
@@ -3897,11 +3897,11 @@
         <v>0</v>
       </c>
       <c r="J20" s="209">
-        <f>MIN(G20:I20)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K20" s="209">
-        <f>MAX(G20:I20) - J20</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="L20" s="251" t="s">
@@ -3910,7 +3910,7 @@
       <c r="M20" s="222" t="s">
         <v>82</v>
       </c>
-      <c r="N20" s="273" t="s">
+      <c r="N20" s="269" t="s">
         <v>41</v>
       </c>
     </row>
@@ -3927,10 +3927,10 @@
       <c r="D21" s="240">
         <v>45740</v>
       </c>
-      <c r="E21" s="262" t="s">
+      <c r="E21" s="258" t="s">
         <v>90</v>
       </c>
-      <c r="F21" s="263" t="s">
+      <c r="F21" s="259" t="s">
         <v>44</v>
       </c>
       <c r="G21" s="242">
@@ -3943,11 +3943,11 @@
         <v>0</v>
       </c>
       <c r="J21" s="232">
-        <f>MIN(G21:I21)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K21" s="232">
-        <f>MAX(G21:I21) - J21</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="L21" s="232" t="s">
@@ -3956,7 +3956,7 @@
       <c r="M21" s="246" t="s">
         <v>82</v>
       </c>
-      <c r="N21" s="259" t="s">
+      <c r="N21" s="255" t="s">
         <v>41</v>
       </c>
     </row>
@@ -3964,7 +3964,7 @@
       <c r="A22" s="208">
         <v>6</v>
       </c>
-      <c r="B22" s="270" t="s">
+      <c r="B22" s="266" t="s">
         <v>166</v>
       </c>
       <c r="C22" s="221" t="s">
@@ -3989,11 +3989,11 @@
         <v>150</v>
       </c>
       <c r="J22" s="209">
-        <f>MIN(G22:I22)</f>
+        <f t="shared" si="0"/>
         <v>120</v>
       </c>
       <c r="K22" s="209">
-        <f>MAX(G22:I22) - J22</f>
+        <f t="shared" si="1"/>
         <v>30</v>
       </c>
       <c r="L22" s="209" t="s">
@@ -4035,11 +4035,11 @@
         <v>2980</v>
       </c>
       <c r="J23" s="232">
-        <f>MIN(G23:I23)</f>
+        <f t="shared" si="0"/>
         <v>1219</v>
       </c>
       <c r="K23" s="232">
-        <f>MAX(G23:I23) - J23</f>
+        <f t="shared" si="1"/>
         <v>1761</v>
       </c>
       <c r="L23" s="232" t="s">
@@ -4048,7 +4048,7 @@
       <c r="M23" s="246" t="s">
         <v>82</v>
       </c>
-      <c r="N23" s="259" t="s">
+      <c r="N23" s="255" t="s">
         <v>40</v>
       </c>
     </row>
@@ -4071,7 +4071,7 @@
       <c r="F24" s="209" t="s">
         <v>88</v>
       </c>
-      <c r="G24" s="272">
+      <c r="G24" s="268">
         <v>2849.9</v>
       </c>
       <c r="H24" s="211">
@@ -4081,11 +4081,11 @@
         <v>2520</v>
       </c>
       <c r="J24" s="209">
-        <f>MIN(G24:I24)</f>
+        <f t="shared" si="0"/>
         <v>2520</v>
       </c>
       <c r="K24" s="209">
-        <f>MAX(G24:I24) - J24</f>
+        <f t="shared" si="1"/>
         <v>1370</v>
       </c>
       <c r="L24" s="251" t="s">
@@ -4094,7 +4094,7 @@
       <c r="M24" s="222" t="s">
         <v>82</v>
       </c>
-      <c r="N24" s="273" t="s">
+      <c r="N24" s="269" t="s">
         <v>41</v>
       </c>
     </row>
@@ -4117,7 +4117,7 @@
       <c r="F25" s="232" t="s">
         <v>44</v>
       </c>
-      <c r="G25" s="264">
+      <c r="G25" s="260">
         <v>8459</v>
       </c>
       <c r="H25" s="243">
@@ -4127,11 +4127,11 @@
         <v>2826</v>
       </c>
       <c r="J25" s="232">
-        <f>MIN(G25:I25)</f>
+        <f t="shared" si="0"/>
         <v>2826</v>
       </c>
       <c r="K25" s="232">
-        <f>MAX(G25:I25) - J25</f>
+        <f t="shared" si="1"/>
         <v>5633</v>
       </c>
       <c r="L25" s="232" t="s">
@@ -4140,7 +4140,7 @@
       <c r="M25" s="246" t="s">
         <v>82</v>
       </c>
-      <c r="N25" s="259" t="s">
+      <c r="N25" s="255" t="s">
         <v>40</v>
       </c>
     </row>
@@ -4148,7 +4148,7 @@
       <c r="A26" s="208">
         <v>6</v>
       </c>
-      <c r="B26" s="270" t="s">
+      <c r="B26" s="266" t="s">
         <v>166</v>
       </c>
       <c r="C26" s="221" t="s">
@@ -4163,7 +4163,7 @@
       <c r="F26" s="209" t="s">
         <v>44</v>
       </c>
-      <c r="G26" s="271">
+      <c r="G26" s="267">
         <v>918</v>
       </c>
       <c r="H26" s="211">
@@ -4173,11 +4173,11 @@
         <v>2134</v>
       </c>
       <c r="J26" s="209">
-        <f>MIN(G26:I26)</f>
+        <f t="shared" si="0"/>
         <v>918</v>
       </c>
       <c r="K26" s="209">
-        <f>MAX(G26:I26) - J26</f>
+        <f t="shared" si="1"/>
         <v>1216</v>
       </c>
       <c r="L26" s="209" t="s">
@@ -4200,7 +4200,7 @@
       <c r="C27" s="238" t="s">
         <v>1</v>
       </c>
-      <c r="D27" s="265">
+      <c r="D27" s="261">
         <v>45743</v>
       </c>
       <c r="E27" s="245" t="s">
@@ -4219,11 +4219,11 @@
         <v>1800</v>
       </c>
       <c r="J27" s="232">
-        <f>MIN(G27:I27)</f>
+        <f t="shared" si="0"/>
         <v>1800</v>
       </c>
       <c r="K27" s="232">
-        <f>MAX(G27:I27) - J27</f>
+        <f t="shared" si="1"/>
         <v>989</v>
       </c>
       <c r="L27" s="232" t="s">
@@ -4232,7 +4232,7 @@
       <c r="M27" s="244" t="s">
         <v>83</v>
       </c>
-      <c r="N27" s="259" t="s">
+      <c r="N27" s="255" t="s">
         <v>40</v>
       </c>
     </row>
@@ -4265,11 +4265,11 @@
         <v>190</v>
       </c>
       <c r="J28" s="209">
-        <f>MIN(G28:I28)</f>
+        <f t="shared" si="0"/>
         <v>180</v>
       </c>
       <c r="K28" s="209">
-        <f>MAX(G28:I28) - J28</f>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="L28" s="209" t="s">
@@ -4311,11 +4311,11 @@
         <v>160</v>
       </c>
       <c r="J29" s="232">
-        <f>MIN(G29:I29)</f>
+        <f t="shared" si="0"/>
         <v>160</v>
       </c>
       <c r="K29" s="232">
-        <f>MAX(G29:I29) - J29</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="L29" s="232" t="s">
@@ -4357,11 +4357,11 @@
         <v>249.5</v>
       </c>
       <c r="J30" s="209">
-        <f>MIN(G30:I30)</f>
+        <f t="shared" si="0"/>
         <v>158</v>
       </c>
       <c r="K30" s="209">
-        <f>MAX(G30:I30) - J30</f>
+        <f t="shared" si="1"/>
         <v>122</v>
       </c>
       <c r="L30" s="209" t="s">
@@ -4393,7 +4393,7 @@
       <c r="F31" s="232" t="s">
         <v>44</v>
       </c>
-      <c r="G31" s="264">
+      <c r="G31" s="260">
         <v>900</v>
       </c>
       <c r="H31" s="243">
@@ -4403,20 +4403,20 @@
         <v>850</v>
       </c>
       <c r="J31" s="232">
-        <f>MIN(G31:I31)</f>
+        <f t="shared" si="0"/>
         <v>800</v>
       </c>
       <c r="K31" s="232">
-        <f>MAX(G31:I31) - J31</f>
+        <f t="shared" si="1"/>
         <v>100</v>
       </c>
       <c r="L31" s="232" t="s">
         <v>54</v>
       </c>
-      <c r="M31" s="266" t="s">
+      <c r="M31" s="262" t="s">
         <v>81</v>
       </c>
-      <c r="N31" s="259" t="s">
+      <c r="N31" s="255" t="s">
         <v>40</v>
       </c>
     </row>
@@ -4449,17 +4449,17 @@
         <v>5400</v>
       </c>
       <c r="J32" s="209">
-        <f>MIN(G32:I32)</f>
+        <f t="shared" si="0"/>
         <v>2800</v>
       </c>
       <c r="K32" s="209">
-        <f>MAX(G32:I32) - J32</f>
+        <f t="shared" si="1"/>
         <v>2600</v>
       </c>
       <c r="L32" s="209" t="s">
         <v>54</v>
       </c>
-      <c r="M32" s="269" t="s">
+      <c r="M32" s="265" t="s">
         <v>81</v>
       </c>
       <c r="N32" s="223" t="s">
@@ -4479,13 +4479,13 @@
       <c r="D33" s="240">
         <v>45744</v>
       </c>
-      <c r="E33" s="267" t="s">
+      <c r="E33" s="263" t="s">
         <v>91</v>
       </c>
       <c r="F33" s="232" t="s">
         <v>44</v>
       </c>
-      <c r="G33" s="264">
+      <c r="G33" s="260">
         <v>2700</v>
       </c>
       <c r="H33" s="243">
@@ -4495,20 +4495,20 @@
         <v>2700</v>
       </c>
       <c r="J33" s="232">
-        <f>MIN(G33:I33)</f>
+        <f t="shared" si="0"/>
         <v>2700</v>
       </c>
       <c r="K33" s="232">
-        <f>MAX(G33:I33) - J33</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="L33" s="232" t="s">
         <v>54</v>
       </c>
-      <c r="M33" s="266" t="s">
+      <c r="M33" s="262" t="s">
         <v>81</v>
       </c>
-      <c r="N33" s="259" t="s">
+      <c r="N33" s="255" t="s">
         <v>40</v>
       </c>
     </row>
@@ -4516,7 +4516,7 @@
       <c r="A34" s="248">
         <v>8</v>
       </c>
-      <c r="B34" s="270" t="s">
+      <c r="B34" s="266" t="s">
         <v>168</v>
       </c>
       <c r="C34" s="254" t="s">
@@ -4531,7 +4531,7 @@
       <c r="F34" s="209" t="s">
         <v>44</v>
       </c>
-      <c r="G34" s="271">
+      <c r="G34" s="267">
         <v>1350</v>
       </c>
       <c r="H34" s="211">
@@ -4541,17 +4541,17 @@
         <v>1350</v>
       </c>
       <c r="J34" s="209">
-        <f>MIN(G34:I34)</f>
+        <f t="shared" si="0"/>
         <v>1350</v>
       </c>
       <c r="K34" s="209">
-        <f>MAX(G34:I34) - J34</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="L34" s="209" t="s">
         <v>54</v>
       </c>
-      <c r="M34" s="269" t="s">
+      <c r="M34" s="265" t="s">
         <v>81</v>
       </c>
       <c r="N34" s="223" t="s">
@@ -4587,11 +4587,11 @@
         <v>11400</v>
       </c>
       <c r="J35" s="232">
-        <f>MIN(G35:I35)</f>
+        <f t="shared" si="0"/>
         <v>9500</v>
       </c>
       <c r="K35" s="232">
-        <f>MAX(G35:I35) - J35</f>
+        <f t="shared" si="1"/>
         <v>4500</v>
       </c>
       <c r="L35" s="232" t="s">
@@ -4608,7 +4608,7 @@
       <c r="A36" s="250">
         <v>14</v>
       </c>
-      <c r="B36" s="270" t="s">
+      <c r="B36" s="266" t="s">
         <v>163</v>
       </c>
       <c r="C36" s="221" t="s">
@@ -4633,11 +4633,11 @@
         <v>6490</v>
       </c>
       <c r="J36" s="209">
-        <f>MIN(G36:I36)</f>
+        <f t="shared" si="0"/>
         <v>5990</v>
       </c>
       <c r="K36" s="209">
-        <f>MAX(G36:I36) - J36</f>
+        <f t="shared" si="1"/>
         <v>1469</v>
       </c>
       <c r="L36" s="209" t="s">
@@ -4679,11 +4679,11 @@
         <v>4000</v>
       </c>
       <c r="J37" s="232">
-        <f>MIN(G37:I37)</f>
+        <f t="shared" ref="J37:J68" si="2">MIN(G37:I37)</f>
         <v>4000</v>
       </c>
       <c r="K37" s="232">
-        <f>MAX(G37:I37) - J37</f>
+        <f t="shared" ref="K37:K68" si="3">MAX(G37:I37) - J37</f>
         <v>7490</v>
       </c>
       <c r="L37" s="232" t="s">
@@ -4692,7 +4692,7 @@
       <c r="M37" s="246" t="s">
         <v>82</v>
       </c>
-      <c r="N37" s="259" t="s">
+      <c r="N37" s="255" t="s">
         <v>41</v>
       </c>
     </row>
@@ -4725,11 +4725,11 @@
         <v>2250</v>
       </c>
       <c r="J38" s="209">
-        <f>MIN(G38:I38)</f>
+        <f t="shared" si="2"/>
         <v>1405</v>
       </c>
       <c r="K38" s="209">
-        <f>MAX(G38:I38) - J38</f>
+        <f t="shared" si="3"/>
         <v>1025</v>
       </c>
       <c r="L38" s="209" t="s">
@@ -4765,26 +4765,26 @@
         <v>7691.5</v>
       </c>
       <c r="H39" s="243">
-        <v>7691.5</v>
+        <v>7500</v>
       </c>
       <c r="I39" s="232">
-        <v>7691.5</v>
+        <v>7200</v>
       </c>
       <c r="J39" s="232">
-        <f>MIN(G39:I39)</f>
-        <v>7691.5</v>
+        <f t="shared" si="2"/>
+        <v>7200</v>
       </c>
       <c r="K39" s="232">
-        <f>MAX(G39:I39) - J39</f>
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>491.5</v>
       </c>
       <c r="L39" s="232" t="s">
         <v>54</v>
       </c>
-      <c r="M39" s="266" t="s">
-        <v>81</v>
-      </c>
-      <c r="N39" s="259" t="s">
+      <c r="M39" s="244" t="s">
+        <v>83</v>
+      </c>
+      <c r="N39" s="255" t="s">
         <v>40</v>
       </c>
     </row>
@@ -4798,7 +4798,7 @@
       <c r="C40" s="248" t="s">
         <v>11</v>
       </c>
-      <c r="D40" s="268">
+      <c r="D40" s="264">
         <v>45750</v>
       </c>
       <c r="E40" s="250" t="s">
@@ -4817,17 +4817,17 @@
         <v>11553.8</v>
       </c>
       <c r="J40" s="209">
-        <f>MIN(G40:I40)</f>
+        <f t="shared" si="2"/>
         <v>11553.8</v>
       </c>
       <c r="K40" s="209">
-        <f>MAX(G40:I40) - J40</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="L40" s="209" t="s">
         <v>54</v>
       </c>
-      <c r="M40" s="269" t="s">
+      <c r="M40" s="265" t="s">
         <v>81</v>
       </c>
       <c r="N40" s="223" t="s">
@@ -4835,13 +4835,13 @@
       </c>
     </row>
     <row r="41" spans="1:14" ht="15.6">
-      <c r="A41" s="278">
+      <c r="A41" s="274">
         <v>4</v>
       </c>
-      <c r="B41" s="279" t="s">
+      <c r="B41" s="275" t="s">
         <v>160</v>
       </c>
-      <c r="C41" s="280" t="s">
+      <c r="C41" s="276" t="s">
         <v>38</v>
       </c>
       <c r="D41" s="227">
@@ -4863,11 +4863,11 @@
         <v>280</v>
       </c>
       <c r="J41" s="202">
-        <f>MIN(G41:I41)</f>
+        <f t="shared" si="2"/>
         <v>150</v>
       </c>
       <c r="K41" s="202">
-        <f>MAX(G41:I41) - J41</f>
+        <f t="shared" si="3"/>
         <v>130</v>
       </c>
       <c r="L41" s="202" t="s">
@@ -4891,11 +4891,11 @@
       <c r="H42" s="217"/>
       <c r="I42" s="212"/>
       <c r="J42" s="209">
-        <f>MIN(G42:I42)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K42" s="209">
-        <f>MAX(G42:I42) - J42</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="L42" s="212"/>
@@ -4913,11 +4913,11 @@
       <c r="H43" s="204"/>
       <c r="I43" s="202"/>
       <c r="J43" s="202">
-        <f>MIN(G43:I43)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K43" s="202">
-        <f>MAX(G43:I43) - J43</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="L43" s="202"/>
@@ -4935,11 +4935,11 @@
       <c r="H44" s="217"/>
       <c r="I44" s="212"/>
       <c r="J44" s="209">
-        <f>MIN(G44:I44)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K44" s="209">
-        <f>MAX(G44:I44) - J44</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="L44" s="212"/>
@@ -4957,11 +4957,11 @@
       <c r="H45" s="204"/>
       <c r="I45" s="202"/>
       <c r="J45" s="202">
-        <f>MIN(G45:I45)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K45" s="202">
-        <f>MAX(G45:I45) - J45</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="L45" s="202"/>
@@ -4979,11 +4979,11 @@
       <c r="H46" s="217"/>
       <c r="I46" s="212"/>
       <c r="J46" s="209">
-        <f>MIN(G46:I46)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K46" s="209">
-        <f>MAX(G46:I46) - J46</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="L46" s="212"/>
@@ -5001,11 +5001,11 @@
       <c r="H47" s="204"/>
       <c r="I47" s="202"/>
       <c r="J47" s="202">
-        <f>MIN(G47:I47)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K47" s="202">
-        <f>MAX(G47:I47) - J47</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="L47" s="202"/>
@@ -5023,11 +5023,11 @@
       <c r="H48" s="217"/>
       <c r="I48" s="212"/>
       <c r="J48" s="209">
-        <f>MIN(G48:I48)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K48" s="209">
-        <f>MAX(G48:I48) - J48</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="L48" s="212"/>
@@ -5045,11 +5045,11 @@
       <c r="H49" s="204"/>
       <c r="I49" s="202"/>
       <c r="J49" s="202">
-        <f>MIN(G49:I49)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K49" s="202">
-        <f>MAX(G49:I49) - J49</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="L49" s="202"/>
@@ -5067,11 +5067,11 @@
       <c r="H50" s="217"/>
       <c r="I50" s="212"/>
       <c r="J50" s="209">
-        <f>MIN(G50:I50)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K50" s="209">
-        <f>MAX(G50:I50) - J50</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="L50" s="212"/>
@@ -5089,11 +5089,11 @@
       <c r="H51" s="204"/>
       <c r="I51" s="202"/>
       <c r="J51" s="202">
-        <f>MIN(G51:I51)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K51" s="202">
-        <f>MAX(G51:I51) - J51</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="L51" s="202"/>
@@ -5111,11 +5111,11 @@
       <c r="H52" s="217"/>
       <c r="I52" s="212"/>
       <c r="J52" s="209">
-        <f>MIN(G52:I52)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K52" s="209">
-        <f>MAX(G52:I52) - J52</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="L52" s="212"/>
@@ -5133,11 +5133,11 @@
       <c r="H53" s="204"/>
       <c r="I53" s="202"/>
       <c r="J53" s="202">
-        <f>MIN(G53:I53)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K53" s="202">
-        <f>MAX(G53:I53) - J53</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="L53" s="202"/>
@@ -5155,11 +5155,11 @@
       <c r="H54" s="217"/>
       <c r="I54" s="212"/>
       <c r="J54" s="209">
-        <f>MIN(G54:I54)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K54" s="209">
-        <f>MAX(G54:I54) - J54</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="L54" s="212"/>
@@ -5177,11 +5177,11 @@
       <c r="H55" s="204"/>
       <c r="I55" s="202"/>
       <c r="J55" s="202">
-        <f>MIN(G55:I55)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K55" s="202">
-        <f>MAX(G55:I55) - J55</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="L55" s="202"/>
@@ -5199,11 +5199,11 @@
       <c r="H56" s="217"/>
       <c r="I56" s="212"/>
       <c r="J56" s="209">
-        <f>MIN(G56:I56)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K56" s="209">
-        <f>MAX(G56:I56) - J56</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="L56" s="212"/>
@@ -5221,11 +5221,11 @@
       <c r="H57" s="204"/>
       <c r="I57" s="202"/>
       <c r="J57" s="232">
-        <f>MIN(G57:I57)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K57" s="202">
-        <f>MAX(G57:I57) - J57</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="L57" s="202"/>
@@ -5243,11 +5243,11 @@
       <c r="H58" s="217"/>
       <c r="I58" s="212"/>
       <c r="J58" s="209">
-        <f>MIN(G58:I58)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K58" s="209">
-        <f>MAX(G58:I58) - J58</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="L58" s="212"/>
@@ -5265,11 +5265,11 @@
       <c r="H59" s="204"/>
       <c r="I59" s="202"/>
       <c r="J59" s="202">
-        <f>MIN(G59:I59)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K59" s="202">
-        <f>MAX(G59:I59) - J59</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="L59" s="202"/>
@@ -5287,11 +5287,11 @@
       <c r="H60" s="217"/>
       <c r="I60" s="212"/>
       <c r="J60" s="209">
-        <f>MIN(G60:I60)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K60" s="209">
-        <f>MAX(G60:I60) - J60</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="L60" s="212"/>
@@ -5309,11 +5309,11 @@
       <c r="H61" s="204"/>
       <c r="I61" s="202"/>
       <c r="J61" s="202">
-        <f>MIN(G61:I61)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K61" s="202">
-        <f>MAX(G61:I61) - J61</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="L61" s="202"/>
@@ -5331,11 +5331,11 @@
       <c r="H62" s="217"/>
       <c r="I62" s="212"/>
       <c r="J62" s="209">
-        <f>MIN(G62:I62)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K62" s="209">
-        <f>MAX(G62:I62) - J62</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="L62" s="212"/>
@@ -5353,11 +5353,11 @@
       <c r="H63" s="204"/>
       <c r="I63" s="202"/>
       <c r="J63" s="202">
-        <f>MIN(G63:I63)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K63" s="202">
-        <f>MAX(G63:I63) - J63</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="L63" s="202"/>
@@ -5375,11 +5375,11 @@
       <c r="H64" s="217"/>
       <c r="I64" s="212"/>
       <c r="J64" s="209">
-        <f>MIN(G64:I64)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K64" s="209">
-        <f>MAX(G64:I64) - J64</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="L64" s="212"/>
@@ -5397,11 +5397,11 @@
       <c r="H65" s="204"/>
       <c r="I65" s="202"/>
       <c r="J65" s="202">
-        <f>MIN(G65:I65)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K65" s="202">
-        <f>MAX(G65:I65) - J65</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="L65" s="202"/>
@@ -5419,11 +5419,11 @@
       <c r="H66" s="217"/>
       <c r="I66" s="212"/>
       <c r="J66" s="209">
-        <f>MIN(G66:I66)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K66" s="209">
-        <f>MAX(G66:I66) - J66</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="L66" s="212"/>
@@ -5441,11 +5441,11 @@
       <c r="H67" s="204"/>
       <c r="I67" s="202"/>
       <c r="J67" s="202">
-        <f>MIN(G67:I67)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K67" s="202">
-        <f>MAX(G67:I67) - J67</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="L67" s="202"/>
@@ -5463,11 +5463,11 @@
       <c r="H68" s="217"/>
       <c r="I68" s="212"/>
       <c r="J68" s="209">
-        <f>MIN(G68:I68)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K68" s="209">
-        <f>MAX(G68:I68) - J68</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="L68" s="212"/>
@@ -5485,11 +5485,11 @@
       <c r="H69" s="204"/>
       <c r="I69" s="202"/>
       <c r="J69" s="202">
-        <f>MIN(G69:I69)</f>
+        <f t="shared" ref="J69:J100" si="4">MIN(G69:I69)</f>
         <v>0</v>
       </c>
       <c r="K69" s="202">
-        <f>MAX(G69:I69) - J69</f>
+        <f t="shared" ref="K69:K100" si="5">MAX(G69:I69) - J69</f>
         <v>0</v>
       </c>
       <c r="L69" s="202"/>
@@ -5507,11 +5507,11 @@
       <c r="H70" s="217"/>
       <c r="I70" s="212"/>
       <c r="J70" s="209">
-        <f>MIN(G70:I70)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K70" s="209">
-        <f>MAX(G70:I70) - J70</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="L70" s="212"/>
@@ -5529,11 +5529,11 @@
       <c r="H71" s="204"/>
       <c r="I71" s="202"/>
       <c r="J71" s="202">
-        <f>MIN(G71:I71)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K71" s="202">
-        <f>MAX(G71:I71) - J71</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="L71" s="202"/>
@@ -5551,11 +5551,11 @@
       <c r="H72" s="217"/>
       <c r="I72" s="212"/>
       <c r="J72" s="209">
-        <f>MIN(G72:I72)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K72" s="209">
-        <f>MAX(G72:I72) - J72</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="L72" s="212"/>
@@ -5573,11 +5573,11 @@
       <c r="H73" s="204"/>
       <c r="I73" s="202"/>
       <c r="J73" s="202">
-        <f>MIN(G73:I73)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K73" s="202">
-        <f>MAX(G73:I73) - J73</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="L73" s="202"/>
@@ -5595,11 +5595,11 @@
       <c r="H74" s="217"/>
       <c r="I74" s="212"/>
       <c r="J74" s="209">
-        <f>MIN(G74:I74)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K74" s="209">
-        <f>MAX(G74:I74) - J74</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="L74" s="212"/>
@@ -5617,11 +5617,11 @@
       <c r="H75" s="204"/>
       <c r="I75" s="202"/>
       <c r="J75" s="202">
-        <f>MIN(G75:I75)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K75" s="202">
-        <f>MAX(G75:I75) - J75</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="L75" s="202"/>
@@ -5639,11 +5639,11 @@
       <c r="H76" s="217"/>
       <c r="I76" s="212"/>
       <c r="J76" s="209">
-        <f>MIN(G76:I76)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K76" s="209">
-        <f>MAX(G76:I76) - J76</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="L76" s="212"/>
@@ -5661,11 +5661,11 @@
       <c r="H77" s="204"/>
       <c r="I77" s="202"/>
       <c r="J77" s="202">
-        <f>MIN(G77:I77)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K77" s="202">
-        <f>MAX(G77:I77) - J77</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="L77" s="202"/>
@@ -5683,11 +5683,11 @@
       <c r="H78" s="217"/>
       <c r="I78" s="212"/>
       <c r="J78" s="209">
-        <f>MIN(G78:I78)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K78" s="209">
-        <f>MAX(G78:I78) - J78</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="L78" s="212"/>
@@ -5705,11 +5705,11 @@
       <c r="H79" s="204"/>
       <c r="I79" s="202"/>
       <c r="J79" s="202">
-        <f>MIN(G79:I79)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K79" s="202">
-        <f>MAX(G79:I79) - J79</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="L79" s="202"/>
@@ -5727,11 +5727,11 @@
       <c r="H80" s="217"/>
       <c r="I80" s="212"/>
       <c r="J80" s="209">
-        <f>MIN(G80:I80)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K80" s="209">
-        <f>MAX(G80:I80) - J80</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="L80" s="212"/>
@@ -5749,11 +5749,11 @@
       <c r="H81" s="204"/>
       <c r="I81" s="202"/>
       <c r="J81" s="202">
-        <f>MIN(G81:I81)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K81" s="202">
-        <f>MAX(G81:I81) - J81</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="L81" s="202"/>
@@ -5771,11 +5771,11 @@
       <c r="H82" s="217"/>
       <c r="I82" s="212"/>
       <c r="J82" s="209">
-        <f>MIN(G82:I82)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K82" s="209">
-        <f>MAX(G82:I82) - J82</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="L82" s="212"/>
@@ -5793,11 +5793,11 @@
       <c r="H83" s="204"/>
       <c r="I83" s="202"/>
       <c r="J83" s="202">
-        <f>MIN(G83:I83)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K83" s="202">
-        <f>MAX(G83:I83) - J83</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="L83" s="202"/>
@@ -5815,11 +5815,11 @@
       <c r="H84" s="217"/>
       <c r="I84" s="212"/>
       <c r="J84" s="209">
-        <f>MIN(G84:I84)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K84" s="209">
-        <f>MAX(G84:I84) - J84</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="L84" s="212"/>
@@ -5837,11 +5837,11 @@
       <c r="H85" s="204"/>
       <c r="I85" s="202"/>
       <c r="J85" s="202">
-        <f>MIN(G85:I85)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K85" s="202">
-        <f>MAX(G85:I85) - J85</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="L85" s="202"/>
@@ -5859,11 +5859,11 @@
       <c r="H86" s="217"/>
       <c r="I86" s="212"/>
       <c r="J86" s="209">
-        <f>MIN(G86:I86)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K86" s="209">
-        <f>MAX(G86:I86) - J86</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="L86" s="212"/>
@@ -5881,11 +5881,11 @@
       <c r="H87" s="204"/>
       <c r="I87" s="202"/>
       <c r="J87" s="202">
-        <f>MIN(G87:I87)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K87" s="202">
-        <f>MAX(G87:I87) - J87</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="L87" s="202"/>
@@ -5903,11 +5903,11 @@
       <c r="H88" s="217"/>
       <c r="I88" s="212"/>
       <c r="J88" s="209">
-        <f>MIN(G88:I88)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K88" s="209">
-        <f>MAX(G88:I88) - J88</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="L88" s="212"/>
@@ -5925,11 +5925,11 @@
       <c r="H89" s="204"/>
       <c r="I89" s="202"/>
       <c r="J89" s="202">
-        <f>MIN(G89:I89)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K89" s="202">
-        <f>MAX(G89:I89) - J89</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="L89" s="202"/>
@@ -5947,11 +5947,11 @@
       <c r="H90" s="217"/>
       <c r="I90" s="212"/>
       <c r="J90" s="209">
-        <f>MIN(G90:I90)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K90" s="209">
-        <f>MAX(G90:I90) - J90</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="L90" s="212"/>
@@ -5969,11 +5969,11 @@
       <c r="H91" s="204"/>
       <c r="I91" s="202"/>
       <c r="J91" s="202">
-        <f>MIN(G91:I91)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K91" s="202">
-        <f>MAX(G91:I91) - J91</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="L91" s="202"/>
@@ -5991,11 +5991,11 @@
       <c r="H92" s="217"/>
       <c r="I92" s="212"/>
       <c r="J92" s="209">
-        <f>MIN(G92:I92)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K92" s="209">
-        <f>MAX(G92:I92) - J92</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="L92" s="212"/>
@@ -6013,11 +6013,11 @@
       <c r="H93" s="204"/>
       <c r="I93" s="202"/>
       <c r="J93" s="202">
-        <f>MIN(G93:I93)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K93" s="202">
-        <f>MAX(G93:I93) - J93</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="L93" s="202"/>
@@ -6035,11 +6035,11 @@
       <c r="H94" s="217"/>
       <c r="I94" s="212"/>
       <c r="J94" s="209">
-        <f>MIN(G94:I94)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K94" s="209">
-        <f>MAX(G94:I94) - J94</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="L94" s="212"/>
@@ -6057,11 +6057,11 @@
       <c r="H95" s="204"/>
       <c r="I95" s="202"/>
       <c r="J95" s="202">
-        <f>MIN(G95:I95)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K95" s="202">
-        <f>MAX(G95:I95) - J95</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="L95" s="202"/>
@@ -6079,11 +6079,11 @@
       <c r="H96" s="217"/>
       <c r="I96" s="212"/>
       <c r="J96" s="209">
-        <f>MIN(G96:I96)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K96" s="209">
-        <f>MAX(G96:I96) - J96</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="L96" s="212"/>
@@ -6101,11 +6101,11 @@
       <c r="H97" s="204"/>
       <c r="I97" s="202"/>
       <c r="J97" s="202">
-        <f>MIN(G97:I97)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K97" s="202">
-        <f>MAX(G97:I97) - J97</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="L97" s="202"/>
@@ -6123,11 +6123,11 @@
       <c r="H98" s="217"/>
       <c r="I98" s="212"/>
       <c r="J98" s="209">
-        <f>MIN(G98:I98)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K98" s="209">
-        <f>MAX(G98:I98) - J98</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="L98" s="212"/>
@@ -6145,11 +6145,11 @@
       <c r="H99" s="204"/>
       <c r="I99" s="202"/>
       <c r="J99" s="202">
-        <f>MIN(G99:I99)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K99" s="202">
-        <f>MAX(G99:I99) - J99</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="L99" s="202"/>
@@ -6167,11 +6167,11 @@
       <c r="H100" s="217"/>
       <c r="I100" s="212"/>
       <c r="J100" s="209">
-        <f>MIN(G100:I100)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K100" s="209">
-        <f>MAX(G100:I100) - J100</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="L100" s="212"/>
@@ -6189,11 +6189,11 @@
       <c r="H101" s="204"/>
       <c r="I101" s="202"/>
       <c r="J101" s="202">
-        <f>MIN(G101:I101)</f>
+        <f t="shared" ref="J101:J132" si="6">MIN(G101:I101)</f>
         <v>0</v>
       </c>
       <c r="K101" s="202">
-        <f>MAX(G101:I101) - J101</f>
+        <f t="shared" ref="K101:K132" si="7">MAX(G101:I101) - J101</f>
         <v>0</v>
       </c>
       <c r="L101" s="202"/>
@@ -6211,11 +6211,11 @@
       <c r="H102" s="217"/>
       <c r="I102" s="212"/>
       <c r="J102" s="209">
-        <f>MIN(G102:I102)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="K102" s="209">
-        <f>MAX(G102:I102) - J102</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="L102" s="212"/>
@@ -6233,11 +6233,11 @@
       <c r="H103" s="204"/>
       <c r="I103" s="202"/>
       <c r="J103" s="202">
-        <f>MIN(G103:I103)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="K103" s="202">
-        <f>MAX(G103:I103) - J103</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="L103" s="202"/>
@@ -6255,11 +6255,11 @@
       <c r="H104" s="217"/>
       <c r="I104" s="212"/>
       <c r="J104" s="209">
-        <f>MIN(G104:I104)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="K104" s="209">
-        <f>MAX(G104:I104) - J104</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="L104" s="212"/>
@@ -6277,11 +6277,11 @@
       <c r="H105" s="204"/>
       <c r="I105" s="202"/>
       <c r="J105" s="202">
-        <f>MIN(G105:I105)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="K105" s="202">
-        <f>MAX(G105:I105) - J105</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="L105" s="202"/>
@@ -6299,11 +6299,11 @@
       <c r="H106" s="217"/>
       <c r="I106" s="212"/>
       <c r="J106" s="209">
-        <f>MIN(G106:I106)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="K106" s="209">
-        <f>MAX(G106:I106) - J106</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="L106" s="212"/>
@@ -6321,11 +6321,11 @@
       <c r="H107" s="204"/>
       <c r="I107" s="202"/>
       <c r="J107" s="202">
-        <f>MIN(G107:I107)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="K107" s="202">
-        <f>MAX(G107:I107) - J107</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="L107" s="202"/>
@@ -6343,11 +6343,11 @@
       <c r="H108" s="217"/>
       <c r="I108" s="212"/>
       <c r="J108" s="209">
-        <f>MIN(G108:I108)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="K108" s="209">
-        <f>MAX(G108:I108) - J108</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="L108" s="212"/>
@@ -6365,11 +6365,11 @@
       <c r="H109" s="204"/>
       <c r="I109" s="202"/>
       <c r="J109" s="202">
-        <f>MIN(G109:I109)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="K109" s="202">
-        <f>MAX(G109:I109) - J109</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="L109" s="202"/>
@@ -6387,11 +6387,11 @@
       <c r="H110" s="217"/>
       <c r="I110" s="212"/>
       <c r="J110" s="209">
-        <f>MIN(G110:I110)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="K110" s="209">
-        <f>MAX(G110:I110) - J110</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="L110" s="212"/>
@@ -6409,11 +6409,11 @@
       <c r="H111" s="204"/>
       <c r="I111" s="202"/>
       <c r="J111" s="202">
-        <f>MIN(G111:I111)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="K111" s="202">
-        <f>MAX(G111:I111) - J111</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="L111" s="202"/>
@@ -6431,11 +6431,11 @@
       <c r="H112" s="217"/>
       <c r="I112" s="212"/>
       <c r="J112" s="209">
-        <f>MIN(G112:I112)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="K112" s="209">
-        <f>MAX(G112:I112) - J112</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="L112" s="212"/>
@@ -6453,11 +6453,11 @@
       <c r="H113" s="204"/>
       <c r="I113" s="202"/>
       <c r="J113" s="202">
-        <f>MIN(G113:I113)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="K113" s="202">
-        <f>MAX(G113:I113) - J113</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="L113" s="202"/>
@@ -6475,11 +6475,11 @@
       <c r="H114" s="217"/>
       <c r="I114" s="212"/>
       <c r="J114" s="209">
-        <f>MIN(G114:I114)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="K114" s="209">
-        <f>MAX(G114:I114) - J114</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="L114" s="212"/>
@@ -6497,11 +6497,11 @@
       <c r="H115" s="204"/>
       <c r="I115" s="202"/>
       <c r="J115" s="202">
-        <f>MIN(G115:I115)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="K115" s="202">
-        <f>MAX(G115:I115) - J115</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="L115" s="202"/>
@@ -6519,11 +6519,11 @@
       <c r="H116" s="217"/>
       <c r="I116" s="212"/>
       <c r="J116" s="209">
-        <f>MIN(G116:I116)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="K116" s="209">
-        <f>MAX(G116:I116) - J116</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="L116" s="212"/>
@@ -6541,11 +6541,11 @@
       <c r="H117" s="204"/>
       <c r="I117" s="202"/>
       <c r="J117" s="202">
-        <f>MIN(G117:I117)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="K117" s="202">
-        <f>MAX(G117:I117) - J117</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="L117" s="202"/>
@@ -6563,11 +6563,11 @@
       <c r="H118" s="217"/>
       <c r="I118" s="212"/>
       <c r="J118" s="209">
-        <f>MIN(G118:I118)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="K118" s="209">
-        <f>MAX(G118:I118) - J118</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="L118" s="212"/>
@@ -6742,40 +6742,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="25.2" thickBot="1">
-      <c r="A1" s="257" t="s">
+      <c r="A1" s="279" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="257"/>
-      <c r="C1" s="257"/>
-      <c r="D1" s="257"/>
-      <c r="E1" s="257"/>
-      <c r="F1" s="257"/>
-      <c r="G1" s="257"/>
-      <c r="H1" s="257"/>
-      <c r="I1" s="257"/>
-      <c r="J1" s="257"/>
-      <c r="K1" s="257"/>
+      <c r="B1" s="279"/>
+      <c r="C1" s="279"/>
+      <c r="D1" s="279"/>
+      <c r="E1" s="279"/>
+      <c r="F1" s="279"/>
+      <c r="G1" s="279"/>
+      <c r="H1" s="279"/>
+      <c r="I1" s="279"/>
+      <c r="J1" s="279"/>
+      <c r="K1" s="279"/>
       <c r="L1" s="70"/>
       <c r="M1" s="70"/>
       <c r="N1" s="70"/>
     </row>
-    <row r="2" spans="1:15" s="255" customFormat="1" ht="23.4" thickTop="1"/>
+    <row r="2" spans="1:15" s="277" customFormat="1" ht="23.4" thickTop="1"/>
     <row r="3" spans="1:15" ht="21">
-      <c r="A3" s="258" t="s">
+      <c r="A3" s="280" t="s">
         <v>49</v>
       </c>
-      <c r="B3" s="258"/>
-      <c r="C3" s="258"/>
+      <c r="B3" s="280"/>
+      <c r="C3" s="280"/>
       <c r="D3" s="67">
         <f>SUM(K6:K180)</f>
         <v>753.6</v>
       </c>
       <c r="E3" s="110"/>
-      <c r="F3" s="258" t="s">
+      <c r="F3" s="280" t="s">
         <v>50</v>
       </c>
-      <c r="G3" s="258"/>
-      <c r="H3" s="258"/>
+      <c r="G3" s="280"/>
+      <c r="H3" s="280"/>
       <c r="I3" s="68">
         <f>SUM(L6:L181)</f>
         <v>111.38</v>

</xml_diff>

<commit_message>
Atualização final do dashboard com estilo premium e novas funcionalidades
</commit_message>
<xml_diff>
--- a/GESTÃO MANUTENÇÃO.xlsx
+++ b/GESTÃO MANUTENÇÃO.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="508" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="179">
   <si>
     <t>AWF-1G58</t>
   </si>
@@ -544,6 +544,18 @@
   </si>
   <si>
     <t>SERVIÇO DE CHUPETA NA BATERIA DO CAMINHÃO EM TERRA NOVA - MT</t>
+  </si>
+  <si>
+    <t>MÃO DE OOBRA + MOTOR DE PARTIDA REALIZAR TROCA</t>
+  </si>
+  <si>
+    <t>PRECISA DE 4 PNEUS NOVOS URGENTES R295.80 R225 LISO</t>
+  </si>
+  <si>
+    <t>SANGRAMENTO DO CAMINHÃO EM SINOP</t>
+  </si>
+  <si>
+    <t>TROCA DOS FARÓIS ANTIGOS PELOS NOVOS!</t>
   </si>
 </sst>
 </file>
@@ -1178,7 +1190,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="281">
+  <cellXfs count="285">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1985,6 +1997,18 @@
     </xf>
     <xf numFmtId="0" fontId="18" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="25" fillId="0" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="24" fillId="23" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2795,7 +2819,7 @@
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -3062,8 +3086,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D44" sqref="D44"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -3111,14 +3135,14 @@
       <c r="C3" s="278"/>
       <c r="D3" s="184">
         <f>SUMIFS(J5:J1000, M5:M1000, "REALIZADO") + SUMIFS(J5:J1000, M5:M1000, "ENVIADO P/ APROVAÇÃO")</f>
-        <v>84100.56</v>
+        <v>89174.760000000009</v>
       </c>
       <c r="E3" s="185" t="s">
         <v>144</v>
       </c>
       <c r="F3" s="186">
         <f>D3+J3</f>
-        <v>126136.95999999999</v>
+        <v>132895.16</v>
       </c>
       <c r="G3" s="278" t="s">
         <v>50</v>
@@ -3127,7 +3151,7 @@
       <c r="I3" s="278"/>
       <c r="J3" s="187">
         <f>SUMIFS(K5:K1000, M5:M1000, "REALIZADO") + SUMIFS(K5:K1000, M5:M1000, "ENVIADO P/ APROVAÇÃO")</f>
-        <v>42036.4</v>
+        <v>43720.4</v>
       </c>
       <c r="K3" s="188"/>
       <c r="L3" s="189"/>
@@ -3266,7 +3290,7 @@
       <c r="M6" s="273" t="s">
         <v>83</v>
       </c>
-      <c r="N6" s="249" t="s">
+      <c r="N6" s="283" t="s">
         <v>40</v>
       </c>
     </row>
@@ -3312,7 +3336,7 @@
       <c r="M7" s="246" t="s">
         <v>82</v>
       </c>
-      <c r="N7" s="239" t="s">
+      <c r="N7" s="284" t="s">
         <v>40</v>
       </c>
     </row>
@@ -3358,7 +3382,7 @@
       <c r="M8" s="222" t="s">
         <v>82</v>
       </c>
-      <c r="N8" s="249" t="s">
+      <c r="N8" s="283" t="s">
         <v>40</v>
       </c>
     </row>
@@ -3416,7 +3440,7 @@
         <v>160</v>
       </c>
       <c r="C10" s="248" t="s">
-        <v>38</v>
+        <v>124</v>
       </c>
       <c r="D10" s="221">
         <v>45724</v>
@@ -3450,7 +3474,7 @@
       <c r="M10" s="222" t="s">
         <v>82</v>
       </c>
-      <c r="N10" s="249" t="s">
+      <c r="N10" s="283" t="s">
         <v>40</v>
       </c>
     </row>
@@ -3726,7 +3750,7 @@
       <c r="M16" s="222" t="s">
         <v>82</v>
       </c>
-      <c r="N16" s="266" t="s">
+      <c r="N16" s="220" t="s">
         <v>40</v>
       </c>
     </row>
@@ -3772,7 +3796,7 @@
       <c r="M17" s="246" t="s">
         <v>82</v>
       </c>
-      <c r="N17" s="239" t="s">
+      <c r="N17" s="284" t="s">
         <v>40</v>
       </c>
     </row>
@@ -3818,7 +3842,7 @@
       <c r="M18" s="222" t="s">
         <v>82</v>
       </c>
-      <c r="N18" s="249" t="s">
+      <c r="N18" s="283" t="s">
         <v>40</v>
       </c>
     </row>
@@ -4278,7 +4302,7 @@
       <c r="M28" s="222" t="s">
         <v>82</v>
       </c>
-      <c r="N28" s="249" t="s">
+      <c r="N28" s="283" t="s">
         <v>40</v>
       </c>
     </row>
@@ -4324,7 +4348,7 @@
       <c r="M29" s="246" t="s">
         <v>82</v>
       </c>
-      <c r="N29" s="239" t="s">
+      <c r="N29" s="284" t="s">
         <v>40</v>
       </c>
     </row>
@@ -4600,7 +4624,7 @@
       <c r="M35" s="244" t="s">
         <v>83</v>
       </c>
-      <c r="N35" s="239" t="s">
+      <c r="N35" s="284" t="s">
         <v>40</v>
       </c>
     </row>
@@ -4704,7 +4728,7 @@
         <v>160</v>
       </c>
       <c r="C38" s="248" t="s">
-        <v>38</v>
+        <v>124</v>
       </c>
       <c r="D38" s="221">
         <v>45749</v>
@@ -4768,15 +4792,15 @@
         <v>7500</v>
       </c>
       <c r="I39" s="232">
-        <v>7200</v>
+        <v>6900</v>
       </c>
       <c r="J39" s="232">
         <f t="shared" si="2"/>
-        <v>7200</v>
+        <v>6900</v>
       </c>
       <c r="K39" s="232">
         <f t="shared" si="3"/>
-        <v>491.5</v>
+        <v>791.5</v>
       </c>
       <c r="L39" s="232" t="s">
         <v>54</v>
@@ -4842,7 +4866,7 @@
         <v>160</v>
       </c>
       <c r="C41" s="276" t="s">
-        <v>38</v>
+        <v>124</v>
       </c>
       <c r="D41" s="227">
         <v>45754</v>
@@ -4881,114 +4905,234 @@
       </c>
     </row>
     <row r="42" spans="1:14" ht="15.6">
-      <c r="A42" s="225"/>
-      <c r="B42" s="206"/>
-      <c r="C42" s="207"/>
-      <c r="D42" s="228"/>
-      <c r="E42" s="215"/>
-      <c r="F42" s="212"/>
-      <c r="G42" s="216"/>
-      <c r="H42" s="217"/>
-      <c r="I42" s="212"/>
+      <c r="A42" s="248">
+        <v>1</v>
+      </c>
+      <c r="B42" s="249" t="s">
+        <v>158</v>
+      </c>
+      <c r="C42" s="248" t="s">
+        <v>0</v>
+      </c>
+      <c r="D42" s="221">
+        <v>45756</v>
+      </c>
+      <c r="E42" s="215" t="s">
+        <v>175</v>
+      </c>
+      <c r="F42" s="212" t="s">
+        <v>44</v>
+      </c>
+      <c r="G42" s="216">
+        <v>825</v>
+      </c>
+      <c r="H42" s="217">
+        <v>1235</v>
+      </c>
+      <c r="I42" s="212">
+        <v>950</v>
+      </c>
       <c r="J42" s="209">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>825</v>
       </c>
       <c r="K42" s="209">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="L42" s="212"/>
-      <c r="M42" s="218"/>
-      <c r="N42" s="224"/>
+        <v>410</v>
+      </c>
+      <c r="L42" s="212" t="s">
+        <v>64</v>
+      </c>
+      <c r="M42" s="218" t="s">
+        <v>83</v>
+      </c>
+      <c r="N42" s="224" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="43" spans="1:14" ht="15.6">
-      <c r="A43" s="198"/>
-      <c r="B43" s="199"/>
-      <c r="C43" s="200"/>
-      <c r="D43" s="201"/>
-      <c r="E43" s="213"/>
-      <c r="F43" s="202"/>
-      <c r="G43" s="203"/>
-      <c r="H43" s="204"/>
-      <c r="I43" s="202"/>
+      <c r="A43" s="198">
+        <v>7</v>
+      </c>
+      <c r="B43" s="199" t="s">
+        <v>19</v>
+      </c>
+      <c r="C43" s="200" t="s">
+        <v>6</v>
+      </c>
+      <c r="D43" s="201">
+        <v>45762</v>
+      </c>
+      <c r="E43" s="213" t="s">
+        <v>176</v>
+      </c>
+      <c r="F43" s="202" t="s">
+        <v>88</v>
+      </c>
+      <c r="G43" s="203">
+        <v>3500</v>
+      </c>
+      <c r="H43" s="204">
+        <v>3400</v>
+      </c>
+      <c r="I43" s="202">
+        <v>3900</v>
+      </c>
       <c r="J43" s="202">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>3400</v>
       </c>
       <c r="K43" s="202">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="L43" s="202"/>
-      <c r="M43" s="214"/>
-      <c r="N43" s="219"/>
+        <v>500</v>
+      </c>
+      <c r="L43" s="202" t="s">
+        <v>54</v>
+      </c>
+      <c r="M43" s="281" t="s">
+        <v>83</v>
+      </c>
+      <c r="N43" s="219" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="44" spans="1:14" ht="15.6">
-      <c r="A44" s="225"/>
-      <c r="B44" s="206"/>
-      <c r="C44" s="207"/>
-      <c r="D44" s="228"/>
-      <c r="E44" s="215"/>
-      <c r="F44" s="212"/>
-      <c r="G44" s="216"/>
-      <c r="H44" s="217"/>
-      <c r="I44" s="212"/>
+      <c r="A44" s="254">
+        <v>4</v>
+      </c>
+      <c r="B44" s="249" t="s">
+        <v>160</v>
+      </c>
+      <c r="C44" s="248" t="s">
+        <v>124</v>
+      </c>
+      <c r="D44" s="221">
+        <v>45754</v>
+      </c>
+      <c r="E44" s="215" t="s">
+        <v>177</v>
+      </c>
+      <c r="F44" s="212" t="s">
+        <v>44</v>
+      </c>
+      <c r="G44" s="216">
+        <v>123.2</v>
+      </c>
+      <c r="H44" s="217">
+        <v>123.2</v>
+      </c>
+      <c r="I44" s="212">
+        <v>123.2</v>
+      </c>
       <c r="J44" s="209">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>123.2</v>
       </c>
       <c r="K44" s="209">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="L44" s="212"/>
-      <c r="M44" s="218"/>
-      <c r="N44" s="224"/>
+      <c r="L44" s="212" t="s">
+        <v>54</v>
+      </c>
+      <c r="M44" s="282" t="s">
+        <v>82</v>
+      </c>
+      <c r="N44" s="224" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="45" spans="1:14" ht="15.6">
-      <c r="A45" s="198"/>
-      <c r="B45" s="199"/>
-      <c r="C45" s="200"/>
-      <c r="D45" s="201"/>
-      <c r="E45" s="213"/>
-      <c r="F45" s="202"/>
-      <c r="G45" s="203"/>
-      <c r="H45" s="204"/>
-      <c r="I45" s="202"/>
+      <c r="A45" s="247">
+        <v>4</v>
+      </c>
+      <c r="B45" s="239" t="s">
+        <v>160</v>
+      </c>
+      <c r="C45" s="238" t="s">
+        <v>124</v>
+      </c>
+      <c r="D45" s="240">
+        <v>45757</v>
+      </c>
+      <c r="E45" s="213" t="s">
+        <v>178</v>
+      </c>
+      <c r="F45" s="202" t="s">
+        <v>44</v>
+      </c>
+      <c r="G45" s="203">
+        <v>750</v>
+      </c>
+      <c r="H45" s="204">
+        <v>546</v>
+      </c>
+      <c r="I45" s="202">
+        <v>546</v>
+      </c>
       <c r="J45" s="202">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>546</v>
       </c>
       <c r="K45" s="202">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="L45" s="202"/>
-      <c r="M45" s="214"/>
-      <c r="N45" s="219"/>
+        <v>204</v>
+      </c>
+      <c r="L45" s="202" t="s">
+        <v>54</v>
+      </c>
+      <c r="M45" s="214" t="s">
+        <v>82</v>
+      </c>
+      <c r="N45" s="219" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="46" spans="1:14" ht="15.6">
-      <c r="A46" s="225"/>
-      <c r="B46" s="206"/>
-      <c r="C46" s="207"/>
-      <c r="D46" s="228"/>
-      <c r="E46" s="215"/>
-      <c r="F46" s="212"/>
-      <c r="G46" s="216"/>
-      <c r="H46" s="217"/>
-      <c r="I46" s="212"/>
+      <c r="A46" s="248">
+        <v>10</v>
+      </c>
+      <c r="B46" s="249" t="s">
+        <v>161</v>
+      </c>
+      <c r="C46" s="248" t="s">
+        <v>9</v>
+      </c>
+      <c r="D46" s="221">
+        <v>45762</v>
+      </c>
+      <c r="E46" s="215" t="s">
+        <v>178</v>
+      </c>
+      <c r="F46" s="212" t="s">
+        <v>44</v>
+      </c>
+      <c r="G46" s="216">
+        <v>750</v>
+      </c>
+      <c r="H46" s="217">
+        <v>550</v>
+      </c>
+      <c r="I46" s="212">
+        <v>480</v>
+      </c>
       <c r="J46" s="209">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>480</v>
       </c>
       <c r="K46" s="209">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="L46" s="212"/>
-      <c r="M46" s="218"/>
-      <c r="N46" s="224"/>
+        <v>270</v>
+      </c>
+      <c r="L46" s="212" t="s">
+        <v>54</v>
+      </c>
+      <c r="M46" s="218" t="s">
+        <v>83</v>
+      </c>
+      <c r="N46" s="224" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="47" spans="1:14" ht="15.6">
       <c r="A47" s="198"/>
@@ -6189,11 +6333,11 @@
       <c r="H101" s="204"/>
       <c r="I101" s="202"/>
       <c r="J101" s="202">
-        <f t="shared" ref="J101:J132" si="6">MIN(G101:I101)</f>
+        <f t="shared" ref="J101:J118" si="6">MIN(G101:I101)</f>
         <v>0</v>
       </c>
       <c r="K101" s="202">
-        <f t="shared" ref="K101:K132" si="7">MAX(G101:I101) - J101</f>
+        <f t="shared" ref="K101:K118" si="7">MAX(G101:I101) - J101</f>
         <v>0</v>
       </c>
       <c r="L101" s="202"/>

</xml_diff>

<commit_message>
🔥 Atualização completa: novo estilo premium, logo, e melhorias no dashboard
</commit_message>
<xml_diff>
--- a/GESTÃO MANUTENÇÃO.xlsx
+++ b/GESTÃO MANUTENÇÃO.xlsx
@@ -1190,7 +1190,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="285">
+  <cellXfs count="297">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1986,6 +1986,18 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="44" fontId="25" fillId="0" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="24" fillId="23" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1998,17 +2010,41 @@
     <xf numFmtId="0" fontId="18" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="25" fillId="0" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="24" fillId="23" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="17" fillId="0" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="5" fillId="2" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="17" fillId="2" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="5" fillId="2" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="17" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="5" fillId="23" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="17" fillId="23" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="5" fillId="23" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3086,8 +3122,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E54" sqref="E54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -3109,16 +3145,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="25.2" thickBot="1">
-      <c r="A1" s="279" t="s">
+      <c r="A1" s="283" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="279"/>
-      <c r="C1" s="279"/>
-      <c r="D1" s="279"/>
-      <c r="E1" s="279"/>
-      <c r="F1" s="279"/>
-      <c r="G1" s="279"/>
-      <c r="H1" s="279"/>
+      <c r="B1" s="283"/>
+      <c r="C1" s="283"/>
+      <c r="D1" s="283"/>
+      <c r="E1" s="283"/>
+      <c r="F1" s="283"/>
+      <c r="G1" s="283"/>
+      <c r="H1" s="283"/>
       <c r="I1" s="70"/>
       <c r="J1" s="70"/>
       <c r="K1" s="70"/>
@@ -3126,13 +3162,13 @@
       <c r="M1" s="182"/>
       <c r="N1" s="178"/>
     </row>
-    <row r="2" spans="1:14" s="277" customFormat="1" ht="23.4" thickTop="1"/>
+    <row r="2" spans="1:14" s="281" customFormat="1" ht="23.4" thickTop="1"/>
     <row r="3" spans="1:14" ht="26.4">
-      <c r="A3" s="278" t="s">
+      <c r="A3" s="282" t="s">
         <v>49</v>
       </c>
-      <c r="B3" s="278"/>
-      <c r="C3" s="278"/>
+      <c r="B3" s="282"/>
+      <c r="C3" s="282"/>
       <c r="D3" s="184">
         <f>SUMIFS(J5:J1000, M5:M1000, "REALIZADO") + SUMIFS(J5:J1000, M5:M1000, "ENVIADO P/ APROVAÇÃO")</f>
         <v>89174.760000000009</v>
@@ -3142,16 +3178,16 @@
       </c>
       <c r="F3" s="186">
         <f>D3+J3</f>
-        <v>132895.16</v>
-      </c>
-      <c r="G3" s="278" t="s">
+        <v>132956.96000000002</v>
+      </c>
+      <c r="G3" s="282" t="s">
         <v>50</v>
       </c>
-      <c r="H3" s="278"/>
-      <c r="I3" s="278"/>
+      <c r="H3" s="282"/>
+      <c r="I3" s="282"/>
       <c r="J3" s="187">
         <f>SUMIFS(K5:K1000, M5:M1000, "REALIZADO") + SUMIFS(K5:K1000, M5:M1000, "ENVIADO P/ APROVAÇÃO")</f>
-        <v>43720.4</v>
+        <v>43782.200000000004</v>
       </c>
       <c r="K3" s="188"/>
       <c r="L3" s="189"/>
@@ -3290,7 +3326,7 @@
       <c r="M6" s="273" t="s">
         <v>83</v>
       </c>
-      <c r="N6" s="283" t="s">
+      <c r="N6" s="279" t="s">
         <v>40</v>
       </c>
     </row>
@@ -3336,7 +3372,7 @@
       <c r="M7" s="246" t="s">
         <v>82</v>
       </c>
-      <c r="N7" s="284" t="s">
+      <c r="N7" s="280" t="s">
         <v>40</v>
       </c>
     </row>
@@ -3382,7 +3418,7 @@
       <c r="M8" s="222" t="s">
         <v>82</v>
       </c>
-      <c r="N8" s="283" t="s">
+      <c r="N8" s="279" t="s">
         <v>40</v>
       </c>
     </row>
@@ -3474,7 +3510,7 @@
       <c r="M10" s="222" t="s">
         <v>82</v>
       </c>
-      <c r="N10" s="283" t="s">
+      <c r="N10" s="279" t="s">
         <v>40</v>
       </c>
     </row>
@@ -3796,7 +3832,7 @@
       <c r="M17" s="246" t="s">
         <v>82</v>
       </c>
-      <c r="N17" s="284" t="s">
+      <c r="N17" s="280" t="s">
         <v>40</v>
       </c>
     </row>
@@ -3842,7 +3878,7 @@
       <c r="M18" s="222" t="s">
         <v>82</v>
       </c>
-      <c r="N18" s="283" t="s">
+      <c r="N18" s="279" t="s">
         <v>40</v>
       </c>
     </row>
@@ -4302,7 +4338,7 @@
       <c r="M28" s="222" t="s">
         <v>82</v>
       </c>
-      <c r="N28" s="283" t="s">
+      <c r="N28" s="279" t="s">
         <v>40</v>
       </c>
     </row>
@@ -4348,7 +4384,7 @@
       <c r="M29" s="246" t="s">
         <v>82</v>
       </c>
-      <c r="N29" s="284" t="s">
+      <c r="N29" s="280" t="s">
         <v>40</v>
       </c>
     </row>
@@ -4624,7 +4660,7 @@
       <c r="M35" s="244" t="s">
         <v>83</v>
       </c>
-      <c r="N35" s="284" t="s">
+      <c r="N35" s="280" t="s">
         <v>40</v>
       </c>
     </row>
@@ -4785,20 +4821,20 @@
       <c r="F39" s="232" t="s">
         <v>44</v>
       </c>
-      <c r="G39" s="242">
+      <c r="G39" s="285">
         <v>7691.5</v>
       </c>
-      <c r="H39" s="243">
+      <c r="H39" s="286">
         <v>7500</v>
       </c>
-      <c r="I39" s="232">
+      <c r="I39" s="287">
         <v>6900</v>
       </c>
-      <c r="J39" s="232">
+      <c r="J39" s="287">
         <f t="shared" si="2"/>
         <v>6900</v>
       </c>
-      <c r="K39" s="232">
+      <c r="K39" s="287">
         <f t="shared" si="3"/>
         <v>791.5</v>
       </c>
@@ -4831,20 +4867,20 @@
       <c r="F40" s="209" t="s">
         <v>88</v>
       </c>
-      <c r="G40" s="210">
+      <c r="G40" s="288">
         <v>11553.8</v>
       </c>
-      <c r="H40" s="211">
+      <c r="H40" s="289">
         <v>11553.8</v>
       </c>
-      <c r="I40" s="209">
+      <c r="I40" s="290">
         <v>11553.8</v>
       </c>
-      <c r="J40" s="209">
+      <c r="J40" s="290">
         <f t="shared" si="2"/>
         <v>11553.8</v>
       </c>
-      <c r="K40" s="209">
+      <c r="K40" s="290">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -4877,20 +4913,20 @@
       <c r="F41" s="202" t="s">
         <v>44</v>
       </c>
-      <c r="G41" s="203">
+      <c r="G41" s="291">
         <v>200</v>
       </c>
-      <c r="H41" s="204">
+      <c r="H41" s="292">
         <v>150</v>
       </c>
-      <c r="I41" s="202">
+      <c r="I41" s="293">
         <v>280</v>
       </c>
-      <c r="J41" s="202">
+      <c r="J41" s="293">
         <f t="shared" si="2"/>
         <v>150</v>
       </c>
-      <c r="K41" s="202">
+      <c r="K41" s="293">
         <f t="shared" si="3"/>
         <v>130</v>
       </c>
@@ -4923,20 +4959,20 @@
       <c r="F42" s="212" t="s">
         <v>44</v>
       </c>
-      <c r="G42" s="216">
+      <c r="G42" s="294">
         <v>825</v>
       </c>
-      <c r="H42" s="217">
+      <c r="H42" s="295">
         <v>1235</v>
       </c>
-      <c r="I42" s="212">
+      <c r="I42" s="296">
         <v>950</v>
       </c>
-      <c r="J42" s="209">
+      <c r="J42" s="290">
         <f t="shared" si="2"/>
         <v>825</v>
       </c>
-      <c r="K42" s="209">
+      <c r="K42" s="290">
         <f t="shared" si="3"/>
         <v>410</v>
       </c>
@@ -4969,27 +5005,27 @@
       <c r="F43" s="202" t="s">
         <v>88</v>
       </c>
-      <c r="G43" s="203">
+      <c r="G43" s="291">
         <v>3500</v>
       </c>
-      <c r="H43" s="204">
+      <c r="H43" s="292">
         <v>3400</v>
       </c>
-      <c r="I43" s="202">
+      <c r="I43" s="293">
         <v>3900</v>
       </c>
-      <c r="J43" s="202">
+      <c r="J43" s="293">
         <f t="shared" si="2"/>
         <v>3400</v>
       </c>
-      <c r="K43" s="202">
+      <c r="K43" s="293">
         <f t="shared" si="3"/>
         <v>500</v>
       </c>
       <c r="L43" s="202" t="s">
         <v>54</v>
       </c>
-      <c r="M43" s="281" t="s">
+      <c r="M43" s="277" t="s">
         <v>83</v>
       </c>
       <c r="N43" s="219" t="s">
@@ -5015,27 +5051,27 @@
       <c r="F44" s="212" t="s">
         <v>44</v>
       </c>
-      <c r="G44" s="216">
+      <c r="G44" s="294">
         <v>123.2</v>
       </c>
-      <c r="H44" s="217">
-        <v>123.2</v>
-      </c>
-      <c r="I44" s="212">
-        <v>123.2</v>
-      </c>
-      <c r="J44" s="209">
+      <c r="H44" s="295">
+        <v>150</v>
+      </c>
+      <c r="I44" s="296">
+        <v>185</v>
+      </c>
+      <c r="J44" s="290">
         <f t="shared" si="2"/>
         <v>123.2</v>
       </c>
-      <c r="K44" s="209">
+      <c r="K44" s="290">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>61.8</v>
       </c>
       <c r="L44" s="212" t="s">
         <v>54</v>
       </c>
-      <c r="M44" s="282" t="s">
+      <c r="M44" s="278" t="s">
         <v>82</v>
       </c>
       <c r="N44" s="224" t="s">
@@ -5061,20 +5097,20 @@
       <c r="F45" s="202" t="s">
         <v>44</v>
       </c>
-      <c r="G45" s="203">
+      <c r="G45" s="291">
         <v>750</v>
       </c>
-      <c r="H45" s="204">
+      <c r="H45" s="292">
         <v>546</v>
       </c>
-      <c r="I45" s="202">
+      <c r="I45" s="293">
         <v>546</v>
       </c>
-      <c r="J45" s="202">
+      <c r="J45" s="293">
         <f t="shared" si="2"/>
         <v>546</v>
       </c>
-      <c r="K45" s="202">
+      <c r="K45" s="293">
         <f t="shared" si="3"/>
         <v>204</v>
       </c>
@@ -5107,20 +5143,20 @@
       <c r="F46" s="212" t="s">
         <v>44</v>
       </c>
-      <c r="G46" s="216">
+      <c r="G46" s="294">
         <v>750</v>
       </c>
-      <c r="H46" s="217">
+      <c r="H46" s="295">
         <v>550</v>
       </c>
-      <c r="I46" s="212">
+      <c r="I46" s="296">
         <v>480</v>
       </c>
-      <c r="J46" s="209">
+      <c r="J46" s="290">
         <f t="shared" si="2"/>
         <v>480</v>
       </c>
-      <c r="K46" s="209">
+      <c r="K46" s="290">
         <f t="shared" si="3"/>
         <v>270</v>
       </c>
@@ -6886,40 +6922,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="25.2" thickBot="1">
-      <c r="A1" s="279" t="s">
+      <c r="A1" s="283" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="279"/>
-      <c r="C1" s="279"/>
-      <c r="D1" s="279"/>
-      <c r="E1" s="279"/>
-      <c r="F1" s="279"/>
-      <c r="G1" s="279"/>
-      <c r="H1" s="279"/>
-      <c r="I1" s="279"/>
-      <c r="J1" s="279"/>
-      <c r="K1" s="279"/>
+      <c r="B1" s="283"/>
+      <c r="C1" s="283"/>
+      <c r="D1" s="283"/>
+      <c r="E1" s="283"/>
+      <c r="F1" s="283"/>
+      <c r="G1" s="283"/>
+      <c r="H1" s="283"/>
+      <c r="I1" s="283"/>
+      <c r="J1" s="283"/>
+      <c r="K1" s="283"/>
       <c r="L1" s="70"/>
       <c r="M1" s="70"/>
       <c r="N1" s="70"/>
     </row>
-    <row r="2" spans="1:15" s="277" customFormat="1" ht="23.4" thickTop="1"/>
+    <row r="2" spans="1:15" s="281" customFormat="1" ht="23.4" thickTop="1"/>
     <row r="3" spans="1:15" ht="21">
-      <c r="A3" s="280" t="s">
+      <c r="A3" s="284" t="s">
         <v>49</v>
       </c>
-      <c r="B3" s="280"/>
-      <c r="C3" s="280"/>
+      <c r="B3" s="284"/>
+      <c r="C3" s="284"/>
       <c r="D3" s="67">
         <f>SUM(K6:K180)</f>
         <v>753.6</v>
       </c>
       <c r="E3" s="110"/>
-      <c r="F3" s="280" t="s">
+      <c r="F3" s="284" t="s">
         <v>50</v>
       </c>
-      <c r="G3" s="280"/>
-      <c r="H3" s="280"/>
+      <c r="G3" s="284"/>
+      <c r="H3" s="284"/>
       <c r="I3" s="68">
         <f>SUM(L6:L181)</f>
         <v>111.38</v>

</xml_diff>

<commit_message>
Primeiro commit - dashboard de manutenção
</commit_message>
<xml_diff>
--- a/GESTÃO MANUTENÇÃO.xlsx
+++ b/GESTÃO MANUTENÇÃO.xlsx
@@ -4,23 +4,24 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="EstaPasta_de_trabalho" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="BaseVeiculos" sheetId="5" r:id="rId1"/>
     <sheet name="MANUTENÇÃO POR VEÍCULO" sheetId="8" r:id="rId2"/>
     <sheet name="POSIÇÃO VEÍCULOS" sheetId="9" r:id="rId3"/>
+    <sheet name="DOCS VEÍCULOS" sheetId="10" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">BaseVeiculos!$A$1:$I$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'MANUTENÇÃO POR VEÍCULO'!$A$4:$N$118</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'MANUTENÇÃO POR VEÍCULO'!$A$4:$N$120</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="743" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="963" uniqueCount="274">
   <si>
     <t>AWF-1G58</t>
   </si>
@@ -577,9 +578,6 @@
     <t>KM RODADOS NO DIA</t>
   </si>
   <si>
-    <t>MOTORISTA</t>
-  </si>
-  <si>
     <t>ATIVIDADES EXERCICIDAS</t>
   </si>
   <si>
@@ -598,24 +596,12 @@
     <t>SANTA RITA DO TRIVELATO - MT</t>
   </si>
   <si>
-    <t>DATA : 21/05/2025</t>
-  </si>
-  <si>
-    <t>JOSÉ WALQUES</t>
-  </si>
-  <si>
     <t>S/MOTORISTA</t>
   </si>
   <si>
-    <t>EMERSON</t>
-  </si>
-  <si>
     <t>(REBOQUE)</t>
   </si>
   <si>
-    <t>ZÉ GILSON</t>
-  </si>
-  <si>
     <t>(MANUTENÇÃO!)</t>
   </si>
   <si>
@@ -631,64 +617,232 @@
     <t>DEVA</t>
   </si>
   <si>
-    <t>7,6 KM</t>
-  </si>
-  <si>
-    <t>BUSCOU O CAMINHÃO NA OFICINA E LEVOU AO BARRACÃO!</t>
-  </si>
-  <si>
     <t>0 KM</t>
   </si>
   <si>
-    <t>30,6 KM</t>
-  </si>
-  <si>
     <t>ALLAN</t>
   </si>
   <si>
-    <t>VEÍCULO PARADO NA CIDADE</t>
-  </si>
-  <si>
     <t>ATENDENDO DEMANDAS NA CIDADE</t>
   </si>
   <si>
-    <t>62,1 KM</t>
-  </si>
-  <si>
     <t>PARADO NO BARRACÃO</t>
   </si>
   <si>
-    <t>16,3 KM</t>
-  </si>
-  <si>
     <t>O KM</t>
   </si>
   <si>
-    <t>NA OFICINA ESPERANDO NOVO MOTOR</t>
-  </si>
-  <si>
-    <t>NA OFICINA FINALIZANDO SERVIÇO</t>
-  </si>
-  <si>
-    <t>SINOP X ROSÁRIO INDO ATENDER DEMANDAS</t>
-  </si>
-  <si>
-    <t>257,9 KM</t>
-  </si>
-  <si>
-    <t>184 KM</t>
-  </si>
-  <si>
-    <t>40,6 KM</t>
-  </si>
-  <si>
     <t>S/ INFORMAÇÕES</t>
   </si>
   <si>
-    <t>ATENDENDO DEMANDAS NA CIDADE -  ROSÁRIO X SINOP</t>
-  </si>
-  <si>
     <t>CONSERTO DE PARTE ELÉTRICA E BUZINA NOVA</t>
+  </si>
+  <si>
+    <t>PROCESSO DE TRANSFERÊNCIA</t>
+  </si>
+  <si>
+    <t>PAGO</t>
+  </si>
+  <si>
+    <t>IPVA VALOR</t>
+  </si>
+  <si>
+    <t>LICENCIAMENTO VALOR</t>
+  </si>
+  <si>
+    <t>MULTAS VALOR</t>
+  </si>
+  <si>
+    <t>FALTA PAGAMENTO DE ÚLTIMA PARCELA PARA COMEÇAR PROCESSO DE TRANSF.</t>
+  </si>
+  <si>
+    <t>FALTA ABRIR PROCESSO DE TRANSFERÊNCIA</t>
+  </si>
+  <si>
+    <t>FALTA PRRENCHIMENTO DE RECIBO E RECONHECIMENTO DE FIRMA MONTENEGRO</t>
+  </si>
+  <si>
+    <t>FALTA PAG. DE MULTA E VISTORIA</t>
+  </si>
+  <si>
+    <t>FALTA PAGAMENTO DE LICENCI. IPVA. E MULTAS PARA REGULARIZAR!</t>
+  </si>
+  <si>
+    <t>FALTA PAG. DE DÉBITOS E VISTORIA</t>
+  </si>
+  <si>
+    <t>FALTA PAG. DE IPVA E VISTORIA</t>
+  </si>
+  <si>
+    <t>FALTA PAG. IPVA,  MULTAS E VISTORIA</t>
+  </si>
+  <si>
+    <t>FALTA PAG. IPVA, RECONHECIMENTO DE FIRMA MARCOS X MONTENEGRO E VISTORIA</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> PROCESSOS OK!</t>
+  </si>
+  <si>
+    <t>PROCESSOS OK!</t>
+  </si>
+  <si>
+    <t>FALTA BAIXA NO AGRAVAME E DEPOIS VISTORIA!</t>
+  </si>
+  <si>
+    <t>FALTA PAG. DE DÉBITOS E EMPLACAMENTO NOVO!</t>
+  </si>
+  <si>
+    <t>FALTA PAG. DE DÉBITOS VISTORIA E EMPLACAMENTO NOVO</t>
+  </si>
+  <si>
+    <t>S/INF.</t>
+  </si>
+  <si>
+    <t>FALTA VISTORIA</t>
+  </si>
+  <si>
+    <t>VALOR TOTAL A PAGAR:</t>
+  </si>
+  <si>
+    <t>SID-3E24</t>
+  </si>
+  <si>
+    <t>ONIX LT 2 BRANCO (2023/24)</t>
+  </si>
+  <si>
+    <t>195/55R 16</t>
+  </si>
+  <si>
+    <t>COMPRA DE BATERIA NOVA PRO CAMINHÃO POIS A ANTIGA ARRIOU</t>
+  </si>
+  <si>
+    <t>CONSERTO DO UNO BRANCO, TERMINAIS DE FOLGAS, FREIO, JOGO E CABO DE VELAS, ALINHAMENTO E CAMBAGENS NAS RODAS</t>
+  </si>
+  <si>
+    <t>ONIX LT 2 BRANCO</t>
+  </si>
+  <si>
+    <t>COMPRA DE CAPA DO RETROVISOR LADO DO PASSAGEIRO, POIS SOLTOU SOZINHA ANTIGA DURANTE VIAGEM</t>
+  </si>
+  <si>
+    <t>DATA : 28-29/05/2025</t>
+  </si>
+  <si>
+    <t>ROGÉRIO</t>
+  </si>
+  <si>
+    <t>CONDUTOR</t>
+  </si>
+  <si>
+    <t>CAMINHÃO PARADO NO EVENTO DE TORIXORÉU</t>
+  </si>
+  <si>
+    <t>345,1 KM</t>
+  </si>
+  <si>
+    <t>TANGARÁ X ROSÁRIO OESTE - MONTAGEM!</t>
+  </si>
+  <si>
+    <t>256,7 KM</t>
+  </si>
+  <si>
+    <t>SINOP X PRÓX. UNIÃO DO SUL - MONTAGEM/DESMONTAGEM</t>
+  </si>
+  <si>
+    <t>JOSE GILSON</t>
+  </si>
+  <si>
+    <t>CUIABÁ X ARENAPOLIS X ROSÁRIO OESTE - EQUIPE MONTAGEM</t>
+  </si>
+  <si>
+    <t>555,2 KM</t>
+  </si>
+  <si>
+    <t>26,4 KM</t>
+  </si>
+  <si>
+    <t>DELSON</t>
+  </si>
+  <si>
+    <t>841,6 KM</t>
+  </si>
+  <si>
+    <t>TORIXORÉU X ROSÁRIO ATENDENDO AS DEMANDAS DE EVENTOS</t>
+  </si>
+  <si>
+    <t>300,4 KM</t>
+  </si>
+  <si>
+    <t>Ñ IDENTIFICADO</t>
+  </si>
+  <si>
+    <t>ROSÁRIO X VARZEA GRANDE X ROSÁRIO OESTE - DESMONTAGEM</t>
+  </si>
+  <si>
+    <t>16,8 KM</t>
+  </si>
+  <si>
+    <t>JOABE</t>
+  </si>
+  <si>
+    <t>RODANDO EM TORIXORÉU</t>
+  </si>
+  <si>
+    <t>0,6 KM</t>
+  </si>
+  <si>
+    <t>FICOU PRONTO HOJE APÓS OS TESTES!</t>
+  </si>
+  <si>
+    <t>139,3 KM</t>
+  </si>
+  <si>
+    <t>CUIABÁ X ROSÁRIO OESTE - DESMONTAGEM</t>
+  </si>
+  <si>
+    <t>TORIXORÉU - MT</t>
+  </si>
+  <si>
+    <t>345,6 KM</t>
+  </si>
+  <si>
+    <t>PRIMAVERA DO LESTE X TORIXORÉU - EVENTO</t>
+  </si>
+  <si>
+    <t>66,9 KM</t>
+  </si>
+  <si>
+    <t>ATENDENDO EVENTO DE TORIXORÉU - PARTE ELÉTRICA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NA OFICINA DE VOLTA PARA MANUTENÇÃO </t>
+  </si>
+  <si>
+    <t>CUIABÁ - MT</t>
+  </si>
+  <si>
+    <t>45 KM</t>
+  </si>
+  <si>
+    <t>LUCAS</t>
+  </si>
+  <si>
+    <t>REALIZANDO DEMANDAS MUNICIPAIS</t>
+  </si>
+  <si>
+    <t>PAGAMENTO DO SERVIÇO DE DESMONTAGEM E MONTAGEM DO MOTOR E RETIFICA DO 1114</t>
+  </si>
+  <si>
+    <t>REVISÃO DE CUICAS, LONAS DE FREIO, CUBO DE ROLAMENTO E VAZAMENTOS NAS MANGUEIRAS DE AR E INTERCOOLER</t>
+  </si>
+  <si>
+    <t>CONSERTO DAS MANGAS DE EIXO, CASTER NAS RODAS DIANTEIRAS E CAMBAGEM RODA DIANTEIRA ESQUERDA</t>
+  </si>
+  <si>
+    <t>TROCA DE 1 BOLSA DE AR E REVISÃO DAS MANGUEIRAS DE AR DOS FREIOS</t>
+  </si>
+  <si>
+    <t>DATA : 30/05/2025</t>
   </si>
 </sst>
 </file>
@@ -700,7 +854,7 @@
     <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
     <numFmt numFmtId="165" formatCode="&quot;R$&quot;\ #,##0.00"/>
   </numFmts>
-  <fonts count="25">
+  <fonts count="27">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -865,6 +1019,20 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color rgb="FFFF0000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="19">
     <fill>
@@ -976,7 +1144,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="27">
     <border>
       <left/>
       <right/>
@@ -1184,12 +1352,144 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="3" tint="-0.499984740745262"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="3" tint="-0.499984740745262"/>
+      </top>
+      <bottom style="thin">
+        <color theme="3" tint="-0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="3" tint="-0.499984740745262"/>
+      </left>
+      <right style="thin">
+        <color theme="3" tint="-0.499984740745262"/>
+      </right>
+      <top style="thin">
+        <color theme="3" tint="-0.499984740745262"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="3" tint="-0.499984740745262"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="3" tint="-0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="3" tint="-0.499984740745262"/>
+      </left>
+      <right style="thin">
+        <color theme="3" tint="-0.499984740745262"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="3" tint="-0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="190">
+  <cellXfs count="224">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1599,30 +1899,6 @@
     <xf numFmtId="0" fontId="6" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1742,10 +2018,132 @@
     <xf numFmtId="0" fontId="12" fillId="18" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="44" fontId="9" fillId="0" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="44" fontId="7" fillId="0" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="8" fillId="0" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="17" fillId="0" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="44" fontId="9" fillId="0" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="44" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="7" fillId="12" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="24" fillId="17" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="24" fillId="17" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="24" fillId="17" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="17" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="26" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="4" fillId="3" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2070,10 +2468,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Plan1"/>
-  <dimension ref="A1:I29"/>
+  <dimension ref="A1:I31"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2144,645 +2542,694 @@
         <v>4</v>
       </c>
       <c r="I2" s="126">
-        <f t="shared" ref="I2:I21" si="0">G2*E2</f>
+        <f t="shared" ref="I2:I23" si="0">G2*E2</f>
         <v>20412.239999999998</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="15.6">
-      <c r="A3" s="131">
+      <c r="A3" s="134">
+        <v>2</v>
+      </c>
+      <c r="B3" s="137" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="134" t="s">
+        <v>153</v>
+      </c>
+      <c r="D3" s="134" t="s">
+        <v>27</v>
+      </c>
+      <c r="E3" s="110"/>
+      <c r="F3" s="111"/>
+      <c r="G3" s="121"/>
+      <c r="H3" s="110"/>
+      <c r="I3" s="126"/>
+    </row>
+    <row r="4" spans="1:9" ht="15.6">
+      <c r="A4" s="131">
         <v>3</v>
       </c>
-      <c r="B3" s="138" t="s">
+      <c r="B4" s="138" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="131" t="s">
+      <c r="C4" s="131" t="s">
         <v>164</v>
       </c>
-      <c r="D3" s="131" t="s">
-        <v>27</v>
-      </c>
-      <c r="E3" s="110">
+      <c r="D4" s="131" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" s="110">
         <v>6</v>
       </c>
-      <c r="F3" s="111" t="s">
+      <c r="F4" s="111" t="s">
         <v>118</v>
       </c>
-      <c r="G3" s="121">
+      <c r="G4" s="121">
         <v>800.67</v>
       </c>
-      <c r="H3" s="110">
+      <c r="H4" s="110">
         <v>4</v>
       </c>
-      <c r="I3" s="126">
+      <c r="I4" s="126">
         <f t="shared" si="0"/>
         <v>4804.0199999999995</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="15.6">
-      <c r="A4" s="134">
+    <row r="5" spans="1:9" ht="15.6">
+      <c r="A5" s="134">
         <v>4</v>
       </c>
-      <c r="B4" s="137" t="s">
+      <c r="B5" s="137" t="s">
         <v>66</v>
       </c>
-      <c r="C4" s="134" t="s">
+      <c r="C5" s="134" t="s">
         <v>165</v>
       </c>
-      <c r="D4" s="134" t="s">
-        <v>27</v>
-      </c>
-      <c r="E4" s="112">
+      <c r="D5" s="134" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" s="112">
         <v>10</v>
       </c>
-      <c r="F4" s="113" t="s">
+      <c r="F5" s="113" t="s">
         <v>114</v>
       </c>
-      <c r="G4" s="123">
+      <c r="G5" s="123">
         <v>1615.1</v>
       </c>
-      <c r="H4" s="112">
+      <c r="H5" s="112">
         <v>4</v>
       </c>
-      <c r="I4" s="127">
+      <c r="I5" s="127">
         <f t="shared" si="0"/>
         <v>16151</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="15.6">
-      <c r="A5" s="134">
+    <row r="6" spans="1:9" ht="15.6">
+      <c r="A6" s="134">
         <v>5</v>
       </c>
-      <c r="B5" s="137" t="s">
+      <c r="B6" s="137" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="134" t="s">
+      <c r="C6" s="134" t="s">
         <v>166</v>
       </c>
-      <c r="D5" s="134" t="s">
+      <c r="D6" s="134" t="s">
         <v>28</v>
       </c>
-      <c r="E5" s="110">
+      <c r="E6" s="110">
         <v>4</v>
       </c>
-      <c r="F5" s="111" t="s">
+      <c r="F6" s="111" t="s">
         <v>117</v>
       </c>
-      <c r="G5" s="121">
+      <c r="G6" s="121">
         <v>273.64999999999998</v>
       </c>
-      <c r="H5" s="110">
+      <c r="H6" s="110">
         <v>2</v>
       </c>
-      <c r="I5" s="126">
+      <c r="I6" s="126">
         <f t="shared" si="0"/>
         <v>1094.5999999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="15.6">
-      <c r="A6" s="134">
+    <row r="7" spans="1:9" ht="15.6">
+      <c r="A7" s="134">
         <v>6</v>
       </c>
-      <c r="B6" s="137" t="s">
+      <c r="B7" s="137" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="134" t="s">
+      <c r="C7" s="134" t="s">
         <v>167</v>
       </c>
-      <c r="D6" s="134" t="s">
+      <c r="D7" s="134" t="s">
         <v>28</v>
       </c>
-      <c r="E6" s="112">
+      <c r="E7" s="112">
         <v>4</v>
       </c>
-      <c r="F6" s="113" t="s">
+      <c r="F7" s="113" t="s">
         <v>122</v>
       </c>
-      <c r="G6" s="123">
+      <c r="G7" s="123">
         <v>1615.1</v>
       </c>
-      <c r="H6" s="112">
+      <c r="H7" s="112">
         <v>2</v>
       </c>
-      <c r="I6" s="127">
+      <c r="I7" s="127">
         <f t="shared" si="0"/>
         <v>6460.4</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="15.6">
-      <c r="A7" s="134">
+    <row r="8" spans="1:9" ht="15.6">
+      <c r="A8" s="134">
         <v>7</v>
       </c>
-      <c r="B7" s="135" t="s">
+      <c r="B8" s="135" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="135" t="s">
+      <c r="C8" s="135" t="s">
         <v>168</v>
       </c>
-      <c r="D7" s="136" t="s">
-        <v>27</v>
-      </c>
-      <c r="E7" s="110">
+      <c r="D8" s="136" t="s">
+        <v>27</v>
+      </c>
+      <c r="E8" s="110">
         <v>8</v>
       </c>
-      <c r="F7" s="114" t="s">
+      <c r="F8" s="114" t="s">
         <v>116</v>
       </c>
-      <c r="G7" s="121">
+      <c r="G8" s="121">
         <v>1701.02</v>
       </c>
-      <c r="H7" s="115">
+      <c r="H8" s="115">
         <v>4</v>
       </c>
-      <c r="I7" s="126">
+      <c r="I8" s="126">
         <f t="shared" si="0"/>
         <v>13608.16</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="15.6">
-      <c r="A8" s="134">
+    <row r="9" spans="1:9" ht="15.6">
+      <c r="A9" s="134">
         <v>8</v>
       </c>
-      <c r="B8" s="135" t="s">
+      <c r="B9" s="135" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="135" t="s">
+      <c r="C9" s="135" t="s">
         <v>169</v>
       </c>
-      <c r="D8" s="136" t="s">
-        <v>27</v>
-      </c>
-      <c r="E8" s="112">
+      <c r="D9" s="136" t="s">
+        <v>27</v>
+      </c>
+      <c r="E9" s="112">
         <v>10</v>
       </c>
-      <c r="F8" s="116" t="s">
+      <c r="F9" s="116" t="s">
         <v>116</v>
       </c>
-      <c r="G8" s="125">
+      <c r="G9" s="125">
         <v>1701.02</v>
       </c>
-      <c r="H8" s="117">
+      <c r="H9" s="117">
         <v>4</v>
       </c>
-      <c r="I8" s="127">
+      <c r="I9" s="127">
         <f t="shared" si="0"/>
         <v>17010.2</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="15.6">
-      <c r="A9" s="134">
+    <row r="10" spans="1:9" ht="15.6">
+      <c r="A10" s="134">
         <v>9</v>
       </c>
-      <c r="B9" s="135" t="s">
+      <c r="B10" s="135" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="135" t="s">
+      <c r="C10" s="135" t="s">
         <v>170</v>
       </c>
-      <c r="D9" s="136" t="s">
-        <v>27</v>
-      </c>
-      <c r="E9" s="110">
+      <c r="D10" s="136" t="s">
+        <v>27</v>
+      </c>
+      <c r="E10" s="110">
         <v>6</v>
       </c>
-      <c r="F9" s="114" t="s">
+      <c r="F10" s="114" t="s">
         <v>118</v>
       </c>
-      <c r="G9" s="121">
+      <c r="G10" s="121">
         <v>800.67</v>
       </c>
-      <c r="H9" s="115">
+      <c r="H10" s="115">
         <v>2</v>
       </c>
-      <c r="I9" s="126">
+      <c r="I10" s="126">
         <f t="shared" si="0"/>
         <v>4804.0199999999995</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="15.6">
-      <c r="A10" s="131">
+    <row r="11" spans="1:9" ht="15.6">
+      <c r="A11" s="131">
         <v>10</v>
       </c>
-      <c r="B10" s="133" t="s">
+      <c r="B11" s="133" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="133" t="s">
+      <c r="C11" s="133" t="s">
         <v>171</v>
       </c>
-      <c r="D10" s="133" t="s">
-        <v>27</v>
-      </c>
-      <c r="E10" s="112">
+      <c r="D11" s="133" t="s">
+        <v>27</v>
+      </c>
+      <c r="E11" s="112">
         <v>4</v>
       </c>
-      <c r="F10" s="117" t="s">
+      <c r="F11" s="117" t="s">
         <v>113</v>
       </c>
-      <c r="G10" s="122">
+      <c r="G11" s="122">
         <v>996.87</v>
       </c>
-      <c r="H10" s="117">
-        <v>0</v>
-      </c>
-      <c r="I10" s="127">
+      <c r="H11" s="117">
+        <v>0</v>
+      </c>
+      <c r="I11" s="127">
         <f t="shared" si="0"/>
         <v>3987.48</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="15.6">
-      <c r="A11" s="134">
+    <row r="12" spans="1:9" ht="15.6">
+      <c r="A12" s="134">
         <v>11</v>
       </c>
-      <c r="B11" s="136" t="s">
+      <c r="B12" s="136" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="136" t="s">
+      <c r="C12" s="136" t="s">
         <v>172</v>
       </c>
-      <c r="D11" s="136" t="s">
-        <v>27</v>
-      </c>
-      <c r="E11" s="110">
+      <c r="D12" s="136" t="s">
+        <v>27</v>
+      </c>
+      <c r="E12" s="110">
         <v>6</v>
       </c>
-      <c r="F11" s="115" t="s">
+      <c r="F12" s="115" t="s">
         <v>114</v>
       </c>
-      <c r="G11" s="124">
+      <c r="G12" s="124">
         <v>1615.1</v>
       </c>
-      <c r="H11" s="115">
+      <c r="H12" s="115">
         <v>2</v>
       </c>
-      <c r="I11" s="126">
+      <c r="I12" s="126">
         <f t="shared" si="0"/>
         <v>9690.5999999999985</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="15.6">
-      <c r="A12" s="134">
+    <row r="13" spans="1:9" ht="15.6">
+      <c r="A13" s="134">
         <v>13</v>
       </c>
-      <c r="B12" s="136" t="s">
+      <c r="B13" s="136" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="135" t="s">
+      <c r="C13" s="135" t="s">
         <v>162</v>
       </c>
-      <c r="D12" s="136" t="s">
-        <v>27</v>
-      </c>
-      <c r="E12" s="112">
+      <c r="D13" s="136" t="s">
+        <v>27</v>
+      </c>
+      <c r="E13" s="112">
         <v>12</v>
       </c>
-      <c r="F12" s="116" t="s">
+      <c r="F13" s="116" t="s">
         <v>116</v>
       </c>
-      <c r="G12" s="125">
+      <c r="G13" s="125">
         <v>1701.02</v>
       </c>
-      <c r="H12" s="117">
+      <c r="H13" s="117">
         <v>6</v>
       </c>
-      <c r="I12" s="127">
+      <c r="I13" s="127">
         <f t="shared" si="0"/>
         <v>20412.239999999998</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="15.6">
-      <c r="A13" s="135">
+    <row r="14" spans="1:9" ht="15.6">
+      <c r="A14" s="135">
         <v>14</v>
       </c>
-      <c r="B13" s="135" t="s">
+      <c r="B14" s="135" t="s">
         <v>44</v>
       </c>
-      <c r="C13" s="135" t="s">
+      <c r="C14" s="135" t="s">
         <v>161</v>
       </c>
-      <c r="D13" s="135" t="s">
-        <v>27</v>
-      </c>
-      <c r="E13" s="118">
+      <c r="D14" s="135" t="s">
+        <v>27</v>
+      </c>
+      <c r="E14" s="118">
         <v>6</v>
       </c>
-      <c r="F13" s="114" t="s">
+      <c r="F14" s="114" t="s">
         <v>118</v>
       </c>
-      <c r="G13" s="121">
+      <c r="G14" s="121">
         <v>800.67</v>
       </c>
-      <c r="H13" s="114">
-        <v>0</v>
-      </c>
-      <c r="I13" s="126">
+      <c r="H14" s="114">
+        <v>0</v>
+      </c>
+      <c r="I14" s="126">
         <f t="shared" si="0"/>
         <v>4804.0199999999995</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="15.6">
-      <c r="A14" s="131">
+    <row r="15" spans="1:9" ht="15.6">
+      <c r="A15" s="131">
         <v>15</v>
       </c>
-      <c r="B14" s="132" t="s">
+      <c r="B15" s="132" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="132" t="s">
+      <c r="C15" s="132" t="s">
         <v>160</v>
       </c>
-      <c r="D14" s="133" t="s">
-        <v>27</v>
-      </c>
-      <c r="E14" s="112">
+      <c r="D15" s="133" t="s">
+        <v>27</v>
+      </c>
+      <c r="E15" s="112">
         <v>10</v>
       </c>
-      <c r="F14" s="116" t="s">
+      <c r="F15" s="116" t="s">
         <v>116</v>
       </c>
-      <c r="G14" s="125">
+      <c r="G15" s="125">
         <v>1701.02</v>
       </c>
-      <c r="H14" s="117">
+      <c r="H15" s="117">
         <v>4</v>
       </c>
-      <c r="I14" s="127">
+      <c r="I15" s="127">
         <f t="shared" si="0"/>
         <v>17010.2</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="15.6">
-      <c r="A15" s="134">
+    <row r="16" spans="1:9" ht="15.6">
+      <c r="A16" s="134">
         <v>16</v>
       </c>
-      <c r="B15" s="135" t="s">
+      <c r="B16" s="135" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="135" t="s">
+      <c r="C16" s="135" t="s">
         <v>159</v>
       </c>
-      <c r="D15" s="136" t="s">
-        <v>27</v>
-      </c>
-      <c r="E15" s="110">
+      <c r="D16" s="136" t="s">
+        <v>27</v>
+      </c>
+      <c r="E16" s="110">
         <v>8</v>
       </c>
-      <c r="F15" s="114" t="s">
+      <c r="F16" s="114" t="s">
         <v>116</v>
       </c>
-      <c r="G15" s="121">
+      <c r="G16" s="121">
         <v>1701.02</v>
       </c>
-      <c r="H15" s="115">
+      <c r="H16" s="115">
         <v>4</v>
       </c>
-      <c r="I15" s="126">
+      <c r="I16" s="126">
         <f t="shared" si="0"/>
         <v>13608.16</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="15.6">
-      <c r="A16" s="134">
+    <row r="17" spans="1:9" ht="15.6">
+      <c r="A17" s="134">
         <v>17</v>
       </c>
-      <c r="B16" s="135" t="s">
+      <c r="B17" s="135" t="s">
         <v>85</v>
       </c>
-      <c r="C16" s="135" t="s">
+      <c r="C17" s="135" t="s">
         <v>158</v>
       </c>
-      <c r="D16" s="136" t="s">
-        <v>27</v>
-      </c>
-      <c r="E16" s="112">
+      <c r="D17" s="136" t="s">
+        <v>27</v>
+      </c>
+      <c r="E17" s="112">
         <v>8</v>
       </c>
-      <c r="F16" s="116" t="s">
+      <c r="F17" s="116" t="s">
         <v>116</v>
       </c>
-      <c r="G16" s="125">
+      <c r="G17" s="125">
         <v>1701.02</v>
       </c>
-      <c r="H16" s="117">
+      <c r="H17" s="117">
         <v>4</v>
       </c>
-      <c r="I16" s="127">
+      <c r="I17" s="127">
         <f t="shared" si="0"/>
         <v>13608.16</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="15.6">
-      <c r="A17" s="136">
+    <row r="18" spans="1:9" ht="15.6">
+      <c r="A18" s="136">
         <v>18</v>
       </c>
-      <c r="B17" s="135" t="s">
+      <c r="B18" s="135" t="s">
         <v>141</v>
       </c>
-      <c r="C17" s="135" t="s">
+      <c r="C18" s="135" t="s">
         <v>154</v>
       </c>
-      <c r="D17" s="136" t="s">
+      <c r="D18" s="136" t="s">
         <v>28</v>
       </c>
-      <c r="E17" s="115">
+      <c r="E18" s="115">
         <v>4</v>
       </c>
-      <c r="F17" s="111" t="s">
+      <c r="F18" s="111" t="s">
         <v>117</v>
       </c>
-      <c r="G17" s="121">
+      <c r="G18" s="121">
         <v>273.64999999999998</v>
       </c>
-      <c r="H17" s="110">
+      <c r="H18" s="110">
         <v>2</v>
       </c>
-      <c r="I17" s="126">
+      <c r="I18" s="126">
         <f t="shared" si="0"/>
         <v>1094.5999999999999</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="15.6">
-      <c r="A18" s="131">
+    <row r="19" spans="1:9" ht="15.6">
+      <c r="A19" s="131">
         <v>19</v>
       </c>
-      <c r="B18" s="132" t="s">
+      <c r="B19" s="132" t="s">
         <v>140</v>
       </c>
-      <c r="C18" s="132" t="s">
+      <c r="C19" s="132" t="s">
         <v>155</v>
       </c>
-      <c r="D18" s="133" t="s">
+      <c r="D19" s="133" t="s">
         <v>28</v>
       </c>
-      <c r="E18" s="112">
+      <c r="E19" s="112">
         <v>4</v>
       </c>
-      <c r="F18" s="116" t="s">
+      <c r="F19" s="116" t="s">
         <v>119</v>
       </c>
-      <c r="G18" s="125">
+      <c r="G19" s="125">
         <v>298.67</v>
       </c>
-      <c r="H18" s="117">
-        <v>0</v>
-      </c>
-      <c r="I18" s="127">
+      <c r="H19" s="117">
+        <v>0</v>
+      </c>
+      <c r="I19" s="127">
         <f t="shared" si="0"/>
         <v>1194.68</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="15.6">
-      <c r="A19" s="133">
+    <row r="20" spans="1:9" ht="15.6">
+      <c r="A20" s="133">
         <v>20</v>
       </c>
-      <c r="B19" s="132" t="s">
+      <c r="B20" s="132" t="s">
         <v>138</v>
       </c>
-      <c r="C19" s="132" t="s">
+      <c r="C20" s="132" t="s">
         <v>156</v>
       </c>
-      <c r="D19" s="133" t="s">
+      <c r="D20" s="133" t="s">
         <v>28</v>
       </c>
-      <c r="E19" s="115">
+      <c r="E20" s="115">
         <v>4</v>
       </c>
-      <c r="F19" s="114" t="s">
+      <c r="F20" s="114" t="s">
         <v>119</v>
       </c>
-      <c r="G19" s="120">
+      <c r="G20" s="120">
         <v>298.67</v>
       </c>
-      <c r="H19" s="115">
-        <v>0</v>
-      </c>
-      <c r="I19" s="126">
+      <c r="H20" s="115">
+        <v>0</v>
+      </c>
+      <c r="I20" s="126">
         <f t="shared" si="0"/>
         <v>1194.68</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="15.6">
-      <c r="A20" s="131">
+    <row r="21" spans="1:9" ht="15.6">
+      <c r="A21" s="131">
         <v>21</v>
       </c>
-      <c r="B20" s="132" t="s">
+      <c r="B21" s="132" t="s">
         <v>139</v>
       </c>
-      <c r="C20" s="132" t="s">
+      <c r="C21" s="132" t="s">
         <v>157</v>
       </c>
-      <c r="D20" s="133" t="s">
+      <c r="D21" s="133" t="s">
         <v>28</v>
       </c>
-      <c r="E20" s="112">
+      <c r="E21" s="112">
         <v>4</v>
       </c>
-      <c r="F20" s="116" t="s">
+      <c r="F21" s="116" t="s">
         <v>119</v>
       </c>
-      <c r="G20" s="125">
+      <c r="G21" s="125">
         <v>298.67</v>
       </c>
-      <c r="H20" s="117">
-        <v>0</v>
-      </c>
-      <c r="I20" s="127">
+      <c r="H21" s="117">
+        <v>0</v>
+      </c>
+      <c r="I21" s="127">
         <f t="shared" si="0"/>
         <v>1194.68</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="15.6">
-      <c r="A21" s="133">
+    <row r="22" spans="1:9" ht="15.6">
+      <c r="A22" s="133">
         <v>22</v>
       </c>
-      <c r="B21" s="132" t="s">
+      <c r="B22" s="132" t="s">
         <v>71</v>
       </c>
-      <c r="C21" s="132" t="s">
+      <c r="C22" s="132" t="s">
         <v>176</v>
       </c>
-      <c r="D21" s="133" t="s">
+      <c r="D22" s="133" t="s">
         <v>28</v>
       </c>
-      <c r="E21" s="115">
+      <c r="E22" s="115">
         <v>4</v>
       </c>
-      <c r="F21" s="114" t="s">
+      <c r="F22" s="114" t="s">
         <v>177</v>
       </c>
-      <c r="G21" s="120">
+      <c r="G22" s="120">
         <v>550</v>
       </c>
-      <c r="H21" s="115">
-        <v>0</v>
-      </c>
-      <c r="I21" s="126">
+      <c r="H22" s="115">
+        <v>0</v>
+      </c>
+      <c r="I22" s="126">
         <f t="shared" si="0"/>
         <v>2200</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="30" customHeight="1">
-      <c r="A22" s="139"/>
-      <c r="B22" s="140"/>
-      <c r="C22" s="140"/>
-      <c r="D22" s="140"/>
-      <c r="E22" s="140"/>
-      <c r="F22" s="140"/>
-      <c r="G22" s="140"/>
-      <c r="H22" s="140"/>
-      <c r="I22" s="141"/>
-    </row>
-    <row r="23" spans="1:9" ht="22.2">
-      <c r="A23" s="139"/>
-      <c r="B23" s="140"/>
-      <c r="C23" s="140"/>
-      <c r="D23" s="140"/>
-      <c r="E23" s="140"/>
-      <c r="F23" s="141"/>
-      <c r="G23" s="142" t="s">
+    <row r="23" spans="1:9" ht="15.6">
+      <c r="A23" s="133">
+        <v>23</v>
+      </c>
+      <c r="B23" s="132" t="s">
+        <v>227</v>
+      </c>
+      <c r="C23" s="132" t="s">
+        <v>228</v>
+      </c>
+      <c r="D23" s="133" t="s">
+        <v>28</v>
+      </c>
+      <c r="E23" s="115">
+        <v>4</v>
+      </c>
+      <c r="F23" s="114" t="s">
+        <v>229</v>
+      </c>
+      <c r="G23" s="120">
+        <v>361.25</v>
+      </c>
+      <c r="H23" s="115">
+        <v>0</v>
+      </c>
+      <c r="I23" s="126">
+        <f t="shared" si="0"/>
+        <v>1445</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="30" customHeight="1">
+      <c r="A24" s="204"/>
+      <c r="B24" s="205"/>
+      <c r="C24" s="205"/>
+      <c r="D24" s="205"/>
+      <c r="E24" s="205"/>
+      <c r="F24" s="205"/>
+      <c r="G24" s="205"/>
+      <c r="H24" s="205"/>
+      <c r="I24" s="206"/>
+    </row>
+    <row r="25" spans="1:9" ht="22.2">
+      <c r="A25" s="204"/>
+      <c r="B25" s="205"/>
+      <c r="C25" s="205"/>
+      <c r="D25" s="205"/>
+      <c r="E25" s="205"/>
+      <c r="F25" s="206"/>
+      <c r="G25" s="207" t="s">
         <v>121</v>
       </c>
-      <c r="H23" s="143"/>
-      <c r="I23" s="128">
-        <f>SUM(I2:I21)</f>
+      <c r="H25" s="208"/>
+      <c r="I25" s="128">
+        <f>SUM(I2:I22)</f>
         <v>174344.13999999998</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="15.6">
-      <c r="A26" s="134">
+    <row r="28" spans="1:9" ht="15.6">
+      <c r="A28" s="134">
         <v>2</v>
       </c>
-      <c r="B26" s="137" t="s">
+      <c r="B28" s="137" t="s">
         <v>1</v>
       </c>
-      <c r="C26" s="134" t="s">
+      <c r="C28" s="134" t="s">
         <v>153</v>
       </c>
-      <c r="D26" s="134" t="s">
-        <v>27</v>
-      </c>
-      <c r="E26" s="112">
+      <c r="D28" s="134" t="s">
+        <v>27</v>
+      </c>
+      <c r="E28" s="112">
         <v>6</v>
       </c>
-      <c r="F26" s="113" t="s">
+      <c r="F28" s="113" t="s">
         <v>114</v>
       </c>
-      <c r="G26" s="123">
+      <c r="G28" s="123">
         <v>1615.1</v>
       </c>
-      <c r="H26" s="112">
+      <c r="H28" s="112">
         <v>4</v>
       </c>
-      <c r="I26" s="127">
-        <f t="shared" ref="I26" si="1">G26*E26</f>
+      <c r="I28" s="127">
+        <f t="shared" ref="I28" si="1">G28*E28</f>
         <v>9690.5999999999985</v>
       </c>
     </row>
-    <row r="29" spans="1:9">
-      <c r="D29" s="54"/>
+    <row r="31" spans="1:9">
+      <c r="D31" s="54"/>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="A22:I22"/>
-    <mergeCell ref="A23:F23"/>
-    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="A24:I24"/>
+    <mergeCell ref="A25:F25"/>
+    <mergeCell ref="G25:H25"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2791,16 +3238,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N125"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:O127"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E63" sqref="E63"/>
+    <sheetView topLeftCell="A62" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection sqref="A1:XFD88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.6640625" customWidth="1"/>
     <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.88671875" customWidth="1"/>
     <col min="5" max="5" width="154.21875" bestFit="1" customWidth="1"/>
@@ -2816,16 +3266,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="25.2" thickBot="1">
-      <c r="A1" s="146" t="s">
+      <c r="A1" s="211" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="146"/>
-      <c r="C1" s="146"/>
-      <c r="D1" s="146"/>
-      <c r="E1" s="146"/>
-      <c r="F1" s="146"/>
-      <c r="G1" s="146"/>
-      <c r="H1" s="146"/>
+      <c r="B1" s="211"/>
+      <c r="C1" s="211"/>
+      <c r="D1" s="211"/>
+      <c r="E1" s="211"/>
+      <c r="F1" s="211"/>
+      <c r="G1" s="211"/>
+      <c r="H1" s="211"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
@@ -2833,32 +3283,32 @@
       <c r="M1" s="3"/>
       <c r="N1" s="2"/>
     </row>
-    <row r="2" spans="1:14" s="144" customFormat="1" ht="23.4" thickTop="1"/>
+    <row r="2" spans="1:14" s="209" customFormat="1" ht="23.4" thickTop="1"/>
     <row r="3" spans="1:14" ht="26.4">
-      <c r="A3" s="145" t="s">
+      <c r="A3" s="210" t="s">
         <v>36</v>
       </c>
-      <c r="B3" s="145"/>
-      <c r="C3" s="145"/>
+      <c r="B3" s="210"/>
+      <c r="C3" s="210"/>
       <c r="D3" s="5">
-        <f>SUMIFS(J5:J1000, M5:M1000, "REALIZADO") + SUMIFS(J5:J1000, M5:M1000, "ENVIADO P/ APROVAÇÃO")</f>
-        <v>191546.09999999998</v>
+        <f>SUMIFS(J5:J1002, M5:M1002, "REALIZADO") + SUMIFS(J5:J1002, M5:M1002, "ENVIADO P/ APROVAÇÃO")</f>
+        <v>215527.96999999997</v>
       </c>
       <c r="E3" s="6" t="s">
         <v>80</v>
       </c>
       <c r="F3" s="7">
         <f>D3+J3</f>
-        <v>282141.15999999997</v>
-      </c>
-      <c r="G3" s="145" t="s">
+        <v>316673.15999999997</v>
+      </c>
+      <c r="G3" s="210" t="s">
         <v>37</v>
       </c>
-      <c r="H3" s="145"/>
-      <c r="I3" s="145"/>
+      <c r="H3" s="210"/>
+      <c r="I3" s="210"/>
       <c r="J3" s="8">
-        <f>SUMIFS(K5:K1000, M5:M1000, "REALIZADO") + SUMIFS(K5:K1000, M5:M1000, "ENVIADO P/ APROVAÇÃO")</f>
-        <v>90595.06</v>
+        <f>SUMIFS(K5:K1002, M5:M1002, "REALIZADO") + SUMIFS(K5:K1002, M5:M1002, "ENVIADO P/ APROVAÇÃO")</f>
+        <v>101145.18999999999</v>
       </c>
       <c r="K3" s="9"/>
       <c r="L3" s="10"/>
@@ -5669,7 +6119,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="65" spans="1:14" ht="15.6">
+    <row r="65" spans="1:15" ht="15.6">
       <c r="A65" s="55">
         <v>8</v>
       </c>
@@ -5715,7 +6165,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="66" spans="1:14" ht="15.6">
+    <row r="66" spans="1:15" ht="15.6">
       <c r="A66" s="67">
         <v>15</v>
       </c>
@@ -5761,7 +6211,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="67" spans="1:14" ht="15.6">
+    <row r="67" spans="1:15" ht="15.6">
       <c r="A67" s="55">
         <v>2</v>
       </c>
@@ -5807,7 +6257,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="68" spans="1:14" ht="15.6">
+    <row r="68" spans="1:15" ht="15.6">
       <c r="A68" s="67">
         <v>15</v>
       </c>
@@ -5853,7 +6303,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="69" spans="1:14" ht="15.6">
+    <row r="69" spans="1:15" ht="15.6">
       <c r="A69" s="64">
         <v>11</v>
       </c>
@@ -5882,11 +6332,11 @@
         <v>32000</v>
       </c>
       <c r="J69" s="23">
-        <f t="shared" ref="J69:J100" si="4">MIN(G69:I69)</f>
+        <f t="shared" ref="J69:J102" si="4">MIN(G69:I69)</f>
         <v>28000</v>
       </c>
       <c r="K69" s="23">
-        <f t="shared" ref="K69:K100" si="5">MAX(G69:I69) - J69</f>
+        <f t="shared" ref="K69:K102" si="5">MAX(G69:I69) - J69</f>
         <v>7400</v>
       </c>
       <c r="L69" s="23" t="s">
@@ -5899,7 +6349,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="70" spans="1:14" ht="15.6" customHeight="1">
+    <row r="70" spans="1:15" ht="15.6" customHeight="1">
       <c r="A70" s="29">
         <v>22</v>
       </c>
@@ -5945,7 +6395,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="71" spans="1:14" ht="15.6">
+    <row r="71" spans="1:15" ht="15.6">
       <c r="A71" s="55">
         <v>1</v>
       </c>
@@ -5991,7 +6441,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="72" spans="1:14" ht="15.6">
+    <row r="72" spans="1:15" ht="15.6">
       <c r="A72" s="65">
         <v>1</v>
       </c>
@@ -6037,7 +6487,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="73" spans="1:14" ht="15.6">
+    <row r="73" spans="1:15" ht="15.6">
       <c r="A73" s="62">
         <v>14</v>
       </c>
@@ -6083,12 +6533,12 @@
         <v>27</v>
       </c>
     </row>
-    <row r="74" spans="1:14" ht="15.6">
+    <row r="74" spans="1:15" ht="15.6">
       <c r="A74" s="46">
         <v>20</v>
       </c>
       <c r="B74" s="27" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C74" s="28" t="s">
         <v>138</v>
@@ -6097,7 +6547,7 @@
         <v>45798</v>
       </c>
       <c r="E74" s="36" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F74" s="33" t="s">
         <v>58</v>
@@ -6129,7 +6579,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="75" spans="1:14" ht="15.6">
+    <row r="75" spans="1:15" ht="15.6">
       <c r="A75" s="55">
         <v>1</v>
       </c>
@@ -6143,7 +6593,7 @@
         <v>45798</v>
       </c>
       <c r="E75" s="34" t="s">
-        <v>222</v>
+        <v>204</v>
       </c>
       <c r="F75" s="23" t="s">
         <v>58</v>
@@ -6175,159 +6625,328 @@
         <v>27</v>
       </c>
     </row>
-    <row r="76" spans="1:14" ht="15.6">
-      <c r="A76" s="46"/>
-      <c r="B76" s="27"/>
-      <c r="C76" s="28"/>
-      <c r="D76" s="49"/>
-      <c r="E76" s="36"/>
-      <c r="F76" s="33"/>
-      <c r="G76" s="37"/>
-      <c r="H76" s="38"/>
-      <c r="I76" s="33"/>
+    <row r="76" spans="1:15" ht="15.6">
+      <c r="A76" s="71">
+        <v>11</v>
+      </c>
+      <c r="B76" s="66" t="s">
+        <v>94</v>
+      </c>
+      <c r="C76" s="65" t="s">
+        <v>10</v>
+      </c>
+      <c r="D76" s="42">
+        <v>45798</v>
+      </c>
+      <c r="E76" s="36" t="s">
+        <v>230</v>
+      </c>
+      <c r="F76" s="33" t="s">
+        <v>58</v>
+      </c>
+      <c r="G76" s="37">
+        <v>661.91</v>
+      </c>
+      <c r="H76" s="38">
+        <v>958</v>
+      </c>
+      <c r="I76" s="33">
+        <v>851.91</v>
+      </c>
       <c r="J76" s="30">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>661.91</v>
       </c>
       <c r="K76" s="30">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="L76" s="33"/>
-      <c r="M76" s="39"/>
-      <c r="N76" s="45"/>
-    </row>
-    <row r="77" spans="1:14" ht="15.6">
-      <c r="A77" s="19"/>
-      <c r="B77" s="20"/>
-      <c r="C77" s="21"/>
-      <c r="D77" s="22"/>
-      <c r="E77" s="34"/>
-      <c r="F77" s="23"/>
-      <c r="G77" s="24"/>
-      <c r="H77" s="25"/>
-      <c r="I77" s="23"/>
+        <v>296.09000000000003</v>
+      </c>
+      <c r="L76" s="33" t="s">
+        <v>41</v>
+      </c>
+      <c r="M76" s="94" t="s">
+        <v>53</v>
+      </c>
+      <c r="N76" s="45" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="77" spans="1:15" ht="15">
+      <c r="A77" s="62">
+        <v>5</v>
+      </c>
+      <c r="B77" s="70" t="s">
+        <v>99</v>
+      </c>
+      <c r="C77" s="57" t="s">
+        <v>3</v>
+      </c>
+      <c r="D77" s="57">
+        <v>45805</v>
+      </c>
+      <c r="E77" s="34" t="s">
+        <v>231</v>
+      </c>
+      <c r="F77" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="G77" s="24">
+        <v>6740</v>
+      </c>
+      <c r="H77" s="25">
+        <v>8498</v>
+      </c>
+      <c r="I77" s="23">
+        <v>11589</v>
+      </c>
       <c r="J77" s="23">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>6740</v>
       </c>
       <c r="K77" s="23">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="L77" s="23"/>
-      <c r="M77" s="35"/>
-      <c r="N77" s="40"/>
-    </row>
-    <row r="78" spans="1:14" ht="15.6">
-      <c r="A78" s="46"/>
-      <c r="B78" s="27"/>
-      <c r="C78" s="28"/>
-      <c r="D78" s="49"/>
-      <c r="E78" s="36"/>
-      <c r="F78" s="33"/>
-      <c r="G78" s="37"/>
-      <c r="H78" s="38"/>
-      <c r="I78" s="33"/>
+        <v>4849</v>
+      </c>
+      <c r="L77" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="M77" s="35" t="s">
+        <v>53</v>
+      </c>
+      <c r="N77" s="40" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="78" spans="1:15" ht="15">
+      <c r="A78" s="67">
+        <v>23</v>
+      </c>
+      <c r="B78" s="87" t="s">
+        <v>232</v>
+      </c>
+      <c r="C78" s="42" t="s">
+        <v>227</v>
+      </c>
+      <c r="D78" s="42">
+        <v>45805</v>
+      </c>
+      <c r="E78" s="67" t="s">
+        <v>271</v>
+      </c>
+      <c r="F78" s="30" t="s">
+        <v>58</v>
+      </c>
+      <c r="G78" s="31">
+        <v>1295</v>
+      </c>
+      <c r="H78" s="32">
+        <v>1895</v>
+      </c>
+      <c r="I78" s="30">
+        <v>1650</v>
+      </c>
       <c r="J78" s="30">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>1295</v>
       </c>
       <c r="K78" s="30">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="L78" s="33"/>
-      <c r="M78" s="39"/>
-      <c r="N78" s="45"/>
-    </row>
-    <row r="79" spans="1:14" ht="15.6">
-      <c r="A79" s="19"/>
-      <c r="B79" s="20"/>
-      <c r="C79" s="21"/>
-      <c r="D79" s="22"/>
-      <c r="E79" s="34"/>
-      <c r="F79" s="23"/>
-      <c r="G79" s="24"/>
-      <c r="H79" s="25"/>
-      <c r="I79" s="23"/>
-      <c r="J79" s="23">
+        <v>600</v>
+      </c>
+      <c r="L78" s="30" t="s">
+        <v>38</v>
+      </c>
+      <c r="M78" s="43" t="s">
+        <v>53</v>
+      </c>
+      <c r="N78" s="44" t="s">
+        <v>28</v>
+      </c>
+      <c r="O78" s="219"/>
+    </row>
+    <row r="79" spans="1:15" ht="15.6">
+      <c r="A79" s="221">
+        <v>15</v>
+      </c>
+      <c r="B79" s="220" t="s">
+        <v>146</v>
+      </c>
+      <c r="C79" s="48" t="s">
+        <v>14</v>
+      </c>
+      <c r="D79" s="222">
+        <v>45805</v>
+      </c>
+      <c r="E79" s="34" t="s">
+        <v>272</v>
+      </c>
+      <c r="F79" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="G79" s="24">
+        <v>1400</v>
+      </c>
+      <c r="H79" s="25">
+        <v>1890</v>
+      </c>
+      <c r="I79" s="23">
+        <v>1850</v>
+      </c>
+      <c r="J79" s="223">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="K79" s="23">
+        <v>1400</v>
+      </c>
+      <c r="K79" s="223">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="L79" s="23"/>
-      <c r="M79" s="35"/>
-      <c r="N79" s="40"/>
-    </row>
-    <row r="80" spans="1:14" ht="15.6">
-      <c r="A80" s="46"/>
-      <c r="B80" s="27"/>
-      <c r="C80" s="28"/>
-      <c r="D80" s="49"/>
-      <c r="E80" s="36"/>
-      <c r="F80" s="33"/>
-      <c r="G80" s="37"/>
-      <c r="H80" s="38"/>
-      <c r="I80" s="33"/>
+        <v>490</v>
+      </c>
+      <c r="L79" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="M79" s="35" t="s">
+        <v>53</v>
+      </c>
+      <c r="N79" s="40" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="80" spans="1:15" ht="15.6">
+      <c r="A80" s="46">
+        <v>23</v>
+      </c>
+      <c r="B80" s="27" t="s">
+        <v>232</v>
+      </c>
+      <c r="C80" s="28" t="s">
+        <v>227</v>
+      </c>
+      <c r="D80" s="49">
+        <v>45805</v>
+      </c>
+      <c r="E80" s="36" t="s">
+        <v>233</v>
+      </c>
+      <c r="F80" s="33" t="s">
+        <v>58</v>
+      </c>
+      <c r="G80" s="37">
+        <v>184.96</v>
+      </c>
+      <c r="H80" s="38">
+        <v>289</v>
+      </c>
+      <c r="I80" s="33">
+        <v>350</v>
+      </c>
       <c r="J80" s="30">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>184.96</v>
       </c>
       <c r="K80" s="30">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="L80" s="33"/>
-      <c r="M80" s="39"/>
-      <c r="N80" s="45"/>
+        <v>165.04</v>
+      </c>
+      <c r="L80" s="33" t="s">
+        <v>41</v>
+      </c>
+      <c r="M80" s="94" t="s">
+        <v>53</v>
+      </c>
+      <c r="N80" s="45" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="81" spans="1:14" ht="15.6">
-      <c r="A81" s="19"/>
-      <c r="B81" s="20"/>
-      <c r="C81" s="21"/>
-      <c r="D81" s="22"/>
-      <c r="E81" s="34"/>
-      <c r="F81" s="23"/>
-      <c r="G81" s="24"/>
-      <c r="H81" s="25"/>
-      <c r="I81" s="23"/>
+      <c r="A81" s="64">
+        <v>11</v>
+      </c>
+      <c r="B81" s="56" t="s">
+        <v>94</v>
+      </c>
+      <c r="C81" s="55" t="s">
+        <v>10</v>
+      </c>
+      <c r="D81" s="57">
+        <v>45807</v>
+      </c>
+      <c r="E81" s="34" t="s">
+        <v>269</v>
+      </c>
+      <c r="F81" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="G81" s="24">
+        <v>5850</v>
+      </c>
+      <c r="H81" s="25">
+        <v>7250</v>
+      </c>
+      <c r="I81" s="23">
+        <v>8900</v>
+      </c>
       <c r="J81" s="23">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>5850</v>
       </c>
       <c r="K81" s="23">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="L81" s="23"/>
-      <c r="M81" s="35"/>
-      <c r="N81" s="40"/>
+        <v>3050</v>
+      </c>
+      <c r="L81" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="M81" s="35" t="s">
+        <v>53</v>
+      </c>
+      <c r="N81" s="40" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="82" spans="1:14" ht="15.6">
-      <c r="A82" s="46"/>
-      <c r="B82" s="27"/>
-      <c r="C82" s="28"/>
-      <c r="D82" s="49"/>
-      <c r="E82" s="36"/>
-      <c r="F82" s="33"/>
-      <c r="G82" s="37"/>
-      <c r="H82" s="38"/>
-      <c r="I82" s="33"/>
+      <c r="A82" s="65">
+        <v>8</v>
+      </c>
+      <c r="B82" s="83" t="s">
+        <v>100</v>
+      </c>
+      <c r="C82" s="71" t="s">
+        <v>7</v>
+      </c>
+      <c r="D82" s="42">
+        <v>45807</v>
+      </c>
+      <c r="E82" s="36" t="s">
+        <v>270</v>
+      </c>
+      <c r="F82" s="33" t="s">
+        <v>31</v>
+      </c>
+      <c r="G82" s="37">
+        <v>7850</v>
+      </c>
+      <c r="H82" s="38">
+        <v>8950</v>
+      </c>
+      <c r="I82" s="33">
+        <v>8950</v>
+      </c>
       <c r="J82" s="30">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>7850</v>
       </c>
       <c r="K82" s="30">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="L82" s="33"/>
-      <c r="M82" s="39"/>
-      <c r="N82" s="45"/>
+        <v>1100</v>
+      </c>
+      <c r="L82" s="33" t="s">
+        <v>49</v>
+      </c>
+      <c r="M82" s="94" t="s">
+        <v>53</v>
+      </c>
+      <c r="N82" s="45" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="83" spans="1:14" ht="15.6">
       <c r="A83" s="19"/>
@@ -6736,11 +7355,11 @@
       <c r="H101" s="25"/>
       <c r="I101" s="23"/>
       <c r="J101" s="23">
-        <f t="shared" ref="J101:J118" si="6">MIN(G101:I101)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K101" s="23">
-        <f t="shared" ref="K101:K118" si="7">MAX(G101:I101) - J101</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="L101" s="23"/>
@@ -6758,11 +7377,11 @@
       <c r="H102" s="38"/>
       <c r="I102" s="33"/>
       <c r="J102" s="30">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K102" s="30">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="L102" s="33"/>
@@ -6780,11 +7399,11 @@
       <c r="H103" s="25"/>
       <c r="I103" s="23"/>
       <c r="J103" s="23">
-        <f t="shared" si="6"/>
+        <f t="shared" ref="J103:J120" si="6">MIN(G103:I103)</f>
         <v>0</v>
       </c>
       <c r="K103" s="23">
-        <f t="shared" si="7"/>
+        <f t="shared" ref="K103:K120" si="7">MAX(G103:I103) - J103</f>
         <v>0</v>
       </c>
       <c r="L103" s="23"/>
@@ -7131,43 +7750,55 @@
       <c r="G119" s="24"/>
       <c r="H119" s="25"/>
       <c r="I119" s="23"/>
-      <c r="J119" s="23"/>
-      <c r="K119" s="23"/>
+      <c r="J119" s="23">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="K119" s="23">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
       <c r="L119" s="23"/>
       <c r="M119" s="35"/>
       <c r="N119" s="40"/>
     </row>
-    <row r="120" spans="1:14">
-      <c r="A120" s="50"/>
-      <c r="B120" s="50"/>
-      <c r="C120" s="50"/>
-      <c r="D120" s="50"/>
-      <c r="E120" s="50"/>
-      <c r="F120" s="50"/>
-      <c r="G120" s="51"/>
-      <c r="H120" s="50"/>
-      <c r="I120" s="50"/>
-      <c r="J120" s="50"/>
-      <c r="K120" s="50"/>
-      <c r="L120" s="50"/>
-      <c r="M120" s="50"/>
-      <c r="N120" s="50"/>
-    </row>
-    <row r="121" spans="1:14">
-      <c r="A121" s="50"/>
-      <c r="B121" s="50"/>
-      <c r="C121" s="50"/>
-      <c r="D121" s="50"/>
-      <c r="E121" s="50"/>
-      <c r="F121" s="50"/>
-      <c r="G121" s="51"/>
-      <c r="H121" s="50"/>
-      <c r="I121" s="50"/>
-      <c r="J121" s="50"/>
-      <c r="K121" s="50"/>
-      <c r="L121" s="50"/>
-      <c r="M121" s="50"/>
-      <c r="N121" s="50"/>
+    <row r="120" spans="1:14" ht="15.6">
+      <c r="A120" s="46"/>
+      <c r="B120" s="27"/>
+      <c r="C120" s="28"/>
+      <c r="D120" s="49"/>
+      <c r="E120" s="36"/>
+      <c r="F120" s="33"/>
+      <c r="G120" s="37"/>
+      <c r="H120" s="38"/>
+      <c r="I120" s="33"/>
+      <c r="J120" s="30">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="K120" s="30">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="L120" s="33"/>
+      <c r="M120" s="39"/>
+      <c r="N120" s="45"/>
+    </row>
+    <row r="121" spans="1:14" ht="15.6">
+      <c r="A121" s="19"/>
+      <c r="B121" s="20"/>
+      <c r="C121" s="21"/>
+      <c r="D121" s="22"/>
+      <c r="E121" s="34"/>
+      <c r="F121" s="23"/>
+      <c r="G121" s="24"/>
+      <c r="H121" s="25"/>
+      <c r="I121" s="23"/>
+      <c r="J121" s="23"/>
+      <c r="K121" s="23"/>
+      <c r="L121" s="23"/>
+      <c r="M121" s="35"/>
+      <c r="N121" s="40"/>
     </row>
     <row r="122" spans="1:14">
       <c r="A122" s="50"/>
@@ -7233,8 +7864,40 @@
       <c r="M125" s="50"/>
       <c r="N125" s="50"/>
     </row>
+    <row r="126" spans="1:14">
+      <c r="A126" s="50"/>
+      <c r="B126" s="50"/>
+      <c r="C126" s="50"/>
+      <c r="D126" s="50"/>
+      <c r="E126" s="50"/>
+      <c r="F126" s="50"/>
+      <c r="G126" s="51"/>
+      <c r="H126" s="50"/>
+      <c r="I126" s="50"/>
+      <c r="J126" s="50"/>
+      <c r="K126" s="50"/>
+      <c r="L126" s="50"/>
+      <c r="M126" s="50"/>
+      <c r="N126" s="50"/>
+    </row>
+    <row r="127" spans="1:14">
+      <c r="A127" s="50"/>
+      <c r="B127" s="50"/>
+      <c r="C127" s="50"/>
+      <c r="D127" s="50"/>
+      <c r="E127" s="50"/>
+      <c r="F127" s="50"/>
+      <c r="G127" s="51"/>
+      <c r="H127" s="50"/>
+      <c r="I127" s="50"/>
+      <c r="J127" s="50"/>
+      <c r="K127" s="50"/>
+      <c r="L127" s="50"/>
+      <c r="M127" s="50"/>
+      <c r="N127" s="50"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A4:N118"/>
+  <autoFilter ref="A4:N120"/>
   <mergeCells count="4">
     <mergeCell ref="A2:XFD2"/>
     <mergeCell ref="A3:C3"/>
@@ -7256,17 +7919,20 @@
       <formula>G5=_xludf.MAX($G5:$I5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="23" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J23"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:J24"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E40" sqref="E40"/>
+      <selection sqref="A1:J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -7279,590 +7945,1334 @@
     <col min="6" max="6" width="34.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="30.21875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="30" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="62.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="70" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="4.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="17.399999999999999">
-      <c r="A1" s="177"/>
-      <c r="B1" s="187" t="s">
+      <c r="A1" s="169"/>
+      <c r="B1" s="179" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="147" t="s">
+      <c r="C1" s="139" t="s">
         <v>22</v>
       </c>
-      <c r="D1" s="147" t="s">
+      <c r="D1" s="139" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="147" t="s">
+      <c r="E1" s="139" t="s">
         <v>26</v>
       </c>
-      <c r="F1" s="147" t="s">
+      <c r="F1" s="139" t="s">
         <v>183</v>
       </c>
-      <c r="G1" s="147" t="s">
+      <c r="G1" s="139" t="s">
         <v>184</v>
       </c>
-      <c r="H1" s="178" t="s">
+      <c r="H1" s="170" t="s">
+        <v>236</v>
+      </c>
+      <c r="I1" s="172" t="s">
         <v>185</v>
       </c>
-      <c r="I1" s="180" t="s">
-        <v>186</v>
-      </c>
-      <c r="J1" s="177"/>
+      <c r="J1" s="169"/>
     </row>
     <row r="2" spans="1:10" ht="15.6">
-      <c r="A2" s="177"/>
-      <c r="B2" s="181">
+      <c r="A2" s="169"/>
+      <c r="B2" s="173">
         <v>1</v>
       </c>
-      <c r="C2" s="149" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="148" t="s">
+      <c r="C2" s="141" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="140" t="s">
         <v>163</v>
       </c>
-      <c r="E2" s="148" t="s">
-        <v>27</v>
-      </c>
-      <c r="F2" s="150" t="s">
+      <c r="E2" s="140" t="s">
+        <v>27</v>
+      </c>
+      <c r="F2" s="142" t="s">
+        <v>259</v>
+      </c>
+      <c r="G2" s="143" t="s">
+        <v>198</v>
+      </c>
+      <c r="H2" s="144" t="s">
+        <v>235</v>
+      </c>
+      <c r="I2" s="171" t="s">
+        <v>237</v>
+      </c>
+      <c r="J2" s="162"/>
+    </row>
+    <row r="3" spans="1:10" ht="15.6">
+      <c r="A3" s="169"/>
+      <c r="B3" s="174">
+        <v>3</v>
+      </c>
+      <c r="C3" s="146" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="145" t="s">
+        <v>164</v>
+      </c>
+      <c r="E3" s="145" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3" s="147" t="s">
         <v>189</v>
       </c>
-      <c r="G2" s="151" t="s">
+      <c r="G3" s="148" t="s">
+        <v>238</v>
+      </c>
+      <c r="H3" s="149" t="s">
+        <v>194</v>
+      </c>
+      <c r="I3" s="147" t="s">
+        <v>239</v>
+      </c>
+      <c r="J3" s="162"/>
+    </row>
+    <row r="4" spans="1:10" ht="15.6">
+      <c r="A4" s="169"/>
+      <c r="B4" s="173">
+        <v>4</v>
+      </c>
+      <c r="C4" s="141" t="s">
+        <v>66</v>
+      </c>
+      <c r="D4" s="140" t="s">
+        <v>165</v>
+      </c>
+      <c r="E4" s="140" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4" s="142" t="s">
+        <v>188</v>
+      </c>
+      <c r="G4" s="143" t="s">
+        <v>240</v>
+      </c>
+      <c r="H4" s="144" t="s">
+        <v>199</v>
+      </c>
+      <c r="I4" s="142" t="s">
+        <v>241</v>
+      </c>
+      <c r="J4" s="162"/>
+    </row>
+    <row r="5" spans="1:10" ht="15.6">
+      <c r="A5" s="169"/>
+      <c r="B5" s="173">
+        <v>5</v>
+      </c>
+      <c r="C5" s="141" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="140" t="s">
+        <v>166</v>
+      </c>
+      <c r="E5" s="140" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5" s="142" t="s">
+        <v>189</v>
+      </c>
+      <c r="G5" s="143" t="s">
+        <v>244</v>
+      </c>
+      <c r="H5" s="144" t="s">
+        <v>250</v>
+      </c>
+      <c r="I5" s="142" t="s">
+        <v>243</v>
+      </c>
+      <c r="J5" s="162"/>
+    </row>
+    <row r="6" spans="1:10" ht="15.6">
+      <c r="A6" s="169"/>
+      <c r="B6" s="173">
+        <v>6</v>
+      </c>
+      <c r="C6" s="141" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="140" t="s">
+        <v>167</v>
+      </c>
+      <c r="E6" s="140" t="s">
+        <v>28</v>
+      </c>
+      <c r="F6" s="142" t="s">
+        <v>188</v>
+      </c>
+      <c r="G6" s="143" t="s">
+        <v>245</v>
+      </c>
+      <c r="H6" s="144" t="s">
+        <v>246</v>
+      </c>
+      <c r="I6" s="142" t="s">
+        <v>200</v>
+      </c>
+      <c r="J6" s="162"/>
+    </row>
+    <row r="7" spans="1:10" ht="15.6" hidden="1">
+      <c r="A7" s="169"/>
+      <c r="B7" s="173">
+        <v>7</v>
+      </c>
+      <c r="C7" s="150" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="150" t="s">
+        <v>168</v>
+      </c>
+      <c r="E7" s="151" t="s">
+        <v>27</v>
+      </c>
+      <c r="F7" s="142" t="s">
+        <v>188</v>
+      </c>
+      <c r="G7" s="152"/>
+      <c r="H7" s="144" t="s">
+        <v>192</v>
+      </c>
+      <c r="I7" s="153"/>
+      <c r="J7" s="162"/>
+    </row>
+    <row r="8" spans="1:10" ht="15.6">
+      <c r="A8" s="169"/>
+      <c r="B8" s="173">
+        <v>8</v>
+      </c>
+      <c r="C8" s="150" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="150" t="s">
+        <v>169</v>
+      </c>
+      <c r="E8" s="151" t="s">
+        <v>27</v>
+      </c>
+      <c r="F8" s="142" t="s">
+        <v>189</v>
+      </c>
+      <c r="G8" s="152" t="s">
+        <v>247</v>
+      </c>
+      <c r="H8" s="154" t="s">
+        <v>195</v>
+      </c>
+      <c r="I8" s="153" t="s">
+        <v>248</v>
+      </c>
+      <c r="J8" s="162"/>
+    </row>
+    <row r="9" spans="1:10" ht="15.6">
+      <c r="A9" s="169"/>
+      <c r="B9" s="173">
+        <v>9</v>
+      </c>
+      <c r="C9" s="150" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="150" t="s">
+        <v>170</v>
+      </c>
+      <c r="E9" s="151" t="s">
+        <v>27</v>
+      </c>
+      <c r="F9" s="142" t="s">
+        <v>189</v>
+      </c>
+      <c r="G9" s="152" t="s">
+        <v>249</v>
+      </c>
+      <c r="H9" s="144" t="s">
+        <v>242</v>
+      </c>
+      <c r="I9" s="153" t="s">
+        <v>251</v>
+      </c>
+      <c r="J9" s="162"/>
+    </row>
+    <row r="10" spans="1:10" ht="15.6">
+      <c r="A10" s="169"/>
+      <c r="B10" s="174">
+        <v>10</v>
+      </c>
+      <c r="C10" s="155" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" s="155" t="s">
+        <v>171</v>
+      </c>
+      <c r="E10" s="155" t="s">
+        <v>27</v>
+      </c>
+      <c r="F10" s="147" t="s">
+        <v>188</v>
+      </c>
+      <c r="G10" s="156" t="s">
+        <v>252</v>
+      </c>
+      <c r="H10" s="157" t="s">
+        <v>253</v>
+      </c>
+      <c r="I10" s="156" t="s">
+        <v>254</v>
+      </c>
+      <c r="J10" s="162"/>
+    </row>
+    <row r="11" spans="1:10" ht="15.6">
+      <c r="A11" s="169"/>
+      <c r="B11" s="173">
+        <v>11</v>
+      </c>
+      <c r="C11" s="151" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="151" t="s">
+        <v>172</v>
+      </c>
+      <c r="E11" s="151" t="s">
+        <v>27</v>
+      </c>
+      <c r="F11" s="142" t="s">
+        <v>188</v>
+      </c>
+      <c r="G11" s="153" t="s">
+        <v>255</v>
+      </c>
+      <c r="H11" s="161" t="s">
+        <v>193</v>
+      </c>
+      <c r="I11" s="153" t="s">
+        <v>256</v>
+      </c>
+      <c r="J11" s="162"/>
+    </row>
+    <row r="12" spans="1:10" ht="15.6" hidden="1">
+      <c r="A12" s="169"/>
+      <c r="B12" s="173">
+        <v>13</v>
+      </c>
+      <c r="C12" s="151" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12" s="150" t="s">
+        <v>162</v>
+      </c>
+      <c r="E12" s="151" t="s">
+        <v>27</v>
+      </c>
+      <c r="F12" s="142" t="s">
+        <v>188</v>
+      </c>
+      <c r="G12" s="152"/>
+      <c r="H12" s="154"/>
+      <c r="I12" s="153"/>
+      <c r="J12" s="162"/>
+    </row>
+    <row r="13" spans="1:10" ht="15.6">
+      <c r="A13" s="169"/>
+      <c r="B13" s="175">
+        <v>14</v>
+      </c>
+      <c r="C13" s="150" t="s">
+        <v>44</v>
+      </c>
+      <c r="D13" s="150" t="s">
+        <v>161</v>
+      </c>
+      <c r="E13" s="150" t="s">
+        <v>27</v>
+      </c>
+      <c r="F13" s="152" t="s">
+        <v>189</v>
+      </c>
+      <c r="G13" s="152" t="s">
+        <v>257</v>
+      </c>
+      <c r="H13" s="144" t="s">
+        <v>194</v>
+      </c>
+      <c r="I13" s="152" t="s">
+        <v>258</v>
+      </c>
+      <c r="J13" s="162"/>
+    </row>
+    <row r="14" spans="1:10" ht="15.6">
+      <c r="A14" s="169"/>
+      <c r="B14" s="174">
+        <v>15</v>
+      </c>
+      <c r="C14" s="158" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14" s="158" t="s">
+        <v>160</v>
+      </c>
+      <c r="E14" s="155" t="s">
+        <v>27</v>
+      </c>
+      <c r="F14" s="147" t="s">
+        <v>259</v>
+      </c>
+      <c r="G14" s="159" t="s">
+        <v>260</v>
+      </c>
+      <c r="H14" s="160" t="s">
+        <v>195</v>
+      </c>
+      <c r="I14" s="156" t="s">
+        <v>261</v>
+      </c>
+      <c r="J14" s="162"/>
+    </row>
+    <row r="15" spans="1:10" ht="15.6" hidden="1">
+      <c r="A15" s="169"/>
+      <c r="B15" s="173">
+        <v>16</v>
+      </c>
+      <c r="C15" s="150" t="s">
+        <v>15</v>
+      </c>
+      <c r="D15" s="150" t="s">
+        <v>159</v>
+      </c>
+      <c r="E15" s="151" t="s">
+        <v>27</v>
+      </c>
+      <c r="F15" s="142" t="s">
+        <v>188</v>
+      </c>
+      <c r="G15" s="152"/>
+      <c r="H15" s="144"/>
+      <c r="I15" s="153"/>
+      <c r="J15" s="162"/>
+    </row>
+    <row r="16" spans="1:10" ht="15.6" hidden="1">
+      <c r="A16" s="169"/>
+      <c r="B16" s="173">
+        <v>17</v>
+      </c>
+      <c r="C16" s="150" t="s">
+        <v>85</v>
+      </c>
+      <c r="D16" s="150" t="s">
+        <v>158</v>
+      </c>
+      <c r="E16" s="151" t="s">
+        <v>27</v>
+      </c>
+      <c r="F16" s="142" t="s">
+        <v>188</v>
+      </c>
+      <c r="G16" s="152"/>
+      <c r="H16" s="154"/>
+      <c r="I16" s="153"/>
+      <c r="J16" s="162"/>
+    </row>
+    <row r="17" spans="1:10" ht="15.6">
+      <c r="A17" s="169"/>
+      <c r="B17" s="176">
+        <v>18</v>
+      </c>
+      <c r="C17" s="150" t="s">
+        <v>141</v>
+      </c>
+      <c r="D17" s="150" t="s">
+        <v>154</v>
+      </c>
+      <c r="E17" s="151" t="s">
+        <v>28</v>
+      </c>
+      <c r="F17" s="153" t="s">
+        <v>188</v>
+      </c>
+      <c r="G17" s="143" t="s">
+        <v>198</v>
+      </c>
+      <c r="H17" s="144" t="s">
+        <v>191</v>
+      </c>
+      <c r="I17" s="202" t="s">
+        <v>201</v>
+      </c>
+      <c r="J17" s="162"/>
+    </row>
+    <row r="18" spans="1:10" ht="15.6">
+      <c r="A18" s="169"/>
+      <c r="B18" s="174">
+        <v>19</v>
+      </c>
+      <c r="C18" s="158" t="s">
+        <v>140</v>
+      </c>
+      <c r="D18" s="158" t="s">
+        <v>155</v>
+      </c>
+      <c r="E18" s="155" t="s">
+        <v>28</v>
+      </c>
+      <c r="F18" s="147" t="s">
+        <v>188</v>
+      </c>
+      <c r="G18" s="159" t="s">
+        <v>262</v>
+      </c>
+      <c r="H18" s="160" t="s">
+        <v>196</v>
+      </c>
+      <c r="I18" s="156" t="s">
+        <v>200</v>
+      </c>
+      <c r="J18" s="162"/>
+    </row>
+    <row r="19" spans="1:10" ht="15.6">
+      <c r="A19" s="169"/>
+      <c r="B19" s="177">
+        <v>20</v>
+      </c>
+      <c r="C19" s="158" t="s">
+        <v>138</v>
+      </c>
+      <c r="D19" s="158" t="s">
+        <v>156</v>
+      </c>
+      <c r="E19" s="155" t="s">
+        <v>28</v>
+      </c>
+      <c r="F19" s="156" t="s">
+        <v>259</v>
+      </c>
+      <c r="G19" s="159" t="s">
         <v>203</v>
       </c>
-      <c r="H2" s="152" t="s">
+      <c r="H19" s="160" t="s">
+        <v>197</v>
+      </c>
+      <c r="I19" s="156" t="s">
+        <v>263</v>
+      </c>
+      <c r="J19" s="162"/>
+    </row>
+    <row r="20" spans="1:10" ht="15.6">
+      <c r="A20" s="169"/>
+      <c r="B20" s="178">
+        <v>21</v>
+      </c>
+      <c r="C20" s="163" t="s">
+        <v>139</v>
+      </c>
+      <c r="D20" s="163" t="s">
+        <v>157</v>
+      </c>
+      <c r="E20" s="164" t="s">
+        <v>28</v>
+      </c>
+      <c r="F20" s="165" t="s">
+        <v>190</v>
+      </c>
+      <c r="G20" s="166" t="s">
+        <v>202</v>
+      </c>
+      <c r="H20" s="167" t="s">
         <v>193</v>
       </c>
-      <c r="I2" s="179" t="s">
-        <v>204</v>
-      </c>
-      <c r="J2" s="170"/>
-    </row>
-    <row r="3" spans="1:10" ht="15.6">
-      <c r="A3" s="177"/>
-      <c r="B3" s="182">
-        <v>3</v>
-      </c>
-      <c r="C3" s="154" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="153" t="s">
-        <v>164</v>
-      </c>
-      <c r="E3" s="153" t="s">
-        <v>27</v>
-      </c>
-      <c r="F3" s="155" t="s">
-        <v>190</v>
-      </c>
-      <c r="G3" s="156" t="s">
-        <v>205</v>
-      </c>
-      <c r="H3" s="157" t="s">
-        <v>194</v>
-      </c>
-      <c r="I3" s="155" t="s">
-        <v>208</v>
-      </c>
-      <c r="J3" s="170"/>
-    </row>
-    <row r="4" spans="1:10" ht="15.6">
-      <c r="A4" s="177"/>
-      <c r="B4" s="181">
-        <v>4</v>
-      </c>
-      <c r="C4" s="149" t="s">
-        <v>66</v>
-      </c>
-      <c r="D4" s="148" t="s">
-        <v>165</v>
-      </c>
-      <c r="E4" s="148" t="s">
-        <v>27</v>
-      </c>
-      <c r="F4" s="150" t="s">
-        <v>189</v>
-      </c>
-      <c r="G4" s="151" t="s">
-        <v>206</v>
-      </c>
-      <c r="H4" s="152" t="s">
-        <v>207</v>
-      </c>
-      <c r="I4" s="150" t="s">
-        <v>209</v>
-      </c>
-      <c r="J4" s="170"/>
-    </row>
-    <row r="5" spans="1:10" ht="15.6">
-      <c r="A5" s="177"/>
-      <c r="B5" s="181">
-        <v>5</v>
-      </c>
-      <c r="C5" s="149" t="s">
-        <v>3</v>
-      </c>
-      <c r="D5" s="148" t="s">
-        <v>166</v>
-      </c>
-      <c r="E5" s="148" t="s">
+      <c r="I20" s="168" t="s">
+        <v>264</v>
+      </c>
+      <c r="J20" s="162"/>
+    </row>
+    <row r="21" spans="1:10" ht="15.6">
+      <c r="A21" s="169"/>
+      <c r="B21" s="196">
+        <v>23</v>
+      </c>
+      <c r="C21" s="200" t="s">
+        <v>227</v>
+      </c>
+      <c r="D21" s="200" t="s">
+        <v>228</v>
+      </c>
+      <c r="E21" s="201" t="s">
         <v>28</v>
       </c>
-      <c r="F5" s="150" t="s">
-        <v>190</v>
-      </c>
-      <c r="G5" s="151" t="s">
-        <v>205</v>
-      </c>
-      <c r="H5" s="152" t="s">
-        <v>194</v>
-      </c>
-      <c r="I5" s="150" t="s">
-        <v>208</v>
-      </c>
-      <c r="J5" s="170"/>
-    </row>
-    <row r="6" spans="1:10" ht="15.6">
-      <c r="A6" s="177"/>
-      <c r="B6" s="181">
-        <v>6</v>
-      </c>
-      <c r="C6" s="149" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" s="148" t="s">
-        <v>167</v>
-      </c>
-      <c r="E6" s="148" t="s">
-        <v>28</v>
-      </c>
-      <c r="F6" s="150" t="s">
-        <v>189</v>
-      </c>
-      <c r="G6" s="151" t="s">
-        <v>210</v>
-      </c>
-      <c r="H6" s="152" t="s">
-        <v>195</v>
-      </c>
-      <c r="I6" s="150" t="s">
-        <v>209</v>
-      </c>
-      <c r="J6" s="170"/>
-    </row>
-    <row r="7" spans="1:10" ht="15.6" hidden="1">
-      <c r="A7" s="177"/>
-      <c r="B7" s="181">
-        <v>7</v>
-      </c>
-      <c r="C7" s="158" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7" s="158" t="s">
-        <v>168</v>
-      </c>
-      <c r="E7" s="159" t="s">
-        <v>27</v>
-      </c>
-      <c r="F7" s="150" t="s">
-        <v>189</v>
-      </c>
-      <c r="G7" s="160"/>
-      <c r="H7" s="152" t="s">
-        <v>196</v>
-      </c>
-      <c r="I7" s="161"/>
-      <c r="J7" s="170"/>
-    </row>
-    <row r="8" spans="1:10" ht="15.6">
-      <c r="A8" s="177"/>
-      <c r="B8" s="181">
-        <v>8</v>
-      </c>
-      <c r="C8" s="158" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" s="158" t="s">
-        <v>169</v>
-      </c>
-      <c r="E8" s="159" t="s">
-        <v>27</v>
-      </c>
-      <c r="F8" s="150" t="s">
-        <v>189</v>
-      </c>
-      <c r="G8" s="160" t="s">
-        <v>205</v>
-      </c>
-      <c r="H8" s="162" t="s">
-        <v>194</v>
-      </c>
-      <c r="I8" s="161" t="s">
-        <v>211</v>
-      </c>
-      <c r="J8" s="170"/>
-    </row>
-    <row r="9" spans="1:10" ht="15.6">
-      <c r="A9" s="177"/>
-      <c r="B9" s="181">
-        <v>9</v>
-      </c>
-      <c r="C9" s="158" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9" s="158" t="s">
-        <v>170</v>
-      </c>
-      <c r="E9" s="159" t="s">
-        <v>27</v>
-      </c>
-      <c r="F9" s="150" t="s">
-        <v>190</v>
-      </c>
-      <c r="G9" s="160" t="s">
-        <v>212</v>
-      </c>
-      <c r="H9" s="152" t="s">
-        <v>197</v>
-      </c>
-      <c r="I9" s="161" t="s">
-        <v>209</v>
-      </c>
-      <c r="J9" s="170"/>
-    </row>
-    <row r="10" spans="1:10" ht="15.6">
-      <c r="A10" s="177"/>
-      <c r="B10" s="182">
-        <v>10</v>
-      </c>
-      <c r="C10" s="163" t="s">
-        <v>9</v>
-      </c>
-      <c r="D10" s="163" t="s">
-        <v>171</v>
-      </c>
-      <c r="E10" s="163" t="s">
-        <v>27</v>
-      </c>
-      <c r="F10" s="155" t="s">
-        <v>189</v>
-      </c>
-      <c r="G10" s="164" t="s">
-        <v>205</v>
-      </c>
-      <c r="H10" s="165" t="s">
-        <v>194</v>
-      </c>
-      <c r="I10" s="164" t="s">
-        <v>211</v>
-      </c>
-      <c r="J10" s="170"/>
-    </row>
-    <row r="11" spans="1:10" ht="15.6">
-      <c r="A11" s="177"/>
-      <c r="B11" s="181">
-        <v>11</v>
-      </c>
-      <c r="C11" s="159" t="s">
-        <v>10</v>
-      </c>
-      <c r="D11" s="159" t="s">
-        <v>172</v>
-      </c>
-      <c r="E11" s="159" t="s">
-        <v>27</v>
-      </c>
-      <c r="F11" s="150" t="s">
-        <v>189</v>
-      </c>
-      <c r="G11" s="161" t="s">
-        <v>205</v>
-      </c>
-      <c r="H11" s="169" t="s">
-        <v>198</v>
-      </c>
-      <c r="I11" s="161" t="s">
-        <v>214</v>
-      </c>
-      <c r="J11" s="170"/>
-    </row>
-    <row r="12" spans="1:10" ht="15.6" hidden="1">
-      <c r="A12" s="177"/>
-      <c r="B12" s="181">
-        <v>13</v>
-      </c>
-      <c r="C12" s="159" t="s">
-        <v>11</v>
-      </c>
-      <c r="D12" s="158" t="s">
-        <v>162</v>
-      </c>
-      <c r="E12" s="159" t="s">
-        <v>27</v>
-      </c>
-      <c r="F12" s="150" t="s">
-        <v>189</v>
-      </c>
-      <c r="G12" s="160"/>
-      <c r="H12" s="162"/>
-      <c r="I12" s="161"/>
-      <c r="J12" s="170"/>
-    </row>
-    <row r="13" spans="1:10" ht="15.6">
-      <c r="A13" s="177"/>
-      <c r="B13" s="183">
-        <v>14</v>
-      </c>
-      <c r="C13" s="158" t="s">
-        <v>44</v>
-      </c>
-      <c r="D13" s="158" t="s">
-        <v>161</v>
-      </c>
-      <c r="E13" s="158" t="s">
-        <v>27</v>
-      </c>
-      <c r="F13" s="160" t="s">
-        <v>190</v>
-      </c>
-      <c r="G13" s="160" t="s">
-        <v>217</v>
-      </c>
-      <c r="H13" s="152" t="s">
-        <v>199</v>
-      </c>
-      <c r="I13" s="160" t="s">
-        <v>216</v>
-      </c>
-      <c r="J13" s="170"/>
-    </row>
-    <row r="14" spans="1:10" ht="15.6">
-      <c r="A14" s="177"/>
-      <c r="B14" s="182">
-        <v>15</v>
-      </c>
-      <c r="C14" s="166" t="s">
-        <v>14</v>
-      </c>
-      <c r="D14" s="166" t="s">
-        <v>160</v>
-      </c>
-      <c r="E14" s="163" t="s">
-        <v>27</v>
-      </c>
-      <c r="F14" s="155" t="s">
-        <v>189</v>
-      </c>
-      <c r="G14" s="167" t="s">
-        <v>218</v>
-      </c>
-      <c r="H14" s="168" t="s">
-        <v>200</v>
-      </c>
-      <c r="I14" s="164" t="s">
-        <v>216</v>
-      </c>
-      <c r="J14" s="170"/>
-    </row>
-    <row r="15" spans="1:10" ht="15.6" hidden="1">
-      <c r="A15" s="177"/>
-      <c r="B15" s="181">
-        <v>16</v>
-      </c>
-      <c r="C15" s="158" t="s">
-        <v>15</v>
-      </c>
-      <c r="D15" s="158" t="s">
-        <v>159</v>
-      </c>
-      <c r="E15" s="159" t="s">
-        <v>27</v>
-      </c>
-      <c r="F15" s="150" t="s">
-        <v>189</v>
-      </c>
-      <c r="G15" s="160"/>
-      <c r="H15" s="152"/>
-      <c r="I15" s="161"/>
-      <c r="J15" s="170"/>
-    </row>
-    <row r="16" spans="1:10" ht="15.6" hidden="1">
-      <c r="A16" s="177"/>
-      <c r="B16" s="181">
-        <v>17</v>
-      </c>
-      <c r="C16" s="158" t="s">
-        <v>85</v>
-      </c>
-      <c r="D16" s="158" t="s">
-        <v>158</v>
-      </c>
-      <c r="E16" s="159" t="s">
-        <v>27</v>
-      </c>
-      <c r="F16" s="150" t="s">
-        <v>189</v>
-      </c>
-      <c r="G16" s="160"/>
-      <c r="H16" s="162"/>
-      <c r="I16" s="161"/>
-      <c r="J16" s="170"/>
-    </row>
-    <row r="17" spans="1:10" ht="15.6">
-      <c r="A17" s="177"/>
-      <c r="B17" s="184">
-        <v>18</v>
-      </c>
-      <c r="C17" s="158" t="s">
-        <v>141</v>
-      </c>
-      <c r="D17" s="158" t="s">
-        <v>154</v>
-      </c>
-      <c r="E17" s="159" t="s">
-        <v>28</v>
-      </c>
-      <c r="F17" s="161" t="s">
-        <v>189</v>
-      </c>
-      <c r="G17" s="151" t="s">
-        <v>205</v>
-      </c>
-      <c r="H17" s="152" t="s">
-        <v>194</v>
-      </c>
-      <c r="I17" s="150" t="s">
-        <v>211</v>
-      </c>
-      <c r="J17" s="170"/>
-    </row>
-    <row r="18" spans="1:10" ht="15.6">
-      <c r="A18" s="177"/>
-      <c r="B18" s="182">
-        <v>19</v>
-      </c>
-      <c r="C18" s="166" t="s">
-        <v>140</v>
-      </c>
-      <c r="D18" s="166" t="s">
-        <v>155</v>
-      </c>
-      <c r="E18" s="163" t="s">
-        <v>28</v>
-      </c>
-      <c r="F18" s="155" t="s">
-        <v>189</v>
-      </c>
-      <c r="G18" s="167" t="s">
-        <v>219</v>
-      </c>
-      <c r="H18" s="168" t="s">
-        <v>201</v>
-      </c>
-      <c r="I18" s="164" t="s">
-        <v>209</v>
-      </c>
-      <c r="J18" s="170"/>
-    </row>
-    <row r="19" spans="1:10" ht="15.6">
-      <c r="A19" s="177"/>
-      <c r="B19" s="185">
-        <v>20</v>
-      </c>
-      <c r="C19" s="166" t="s">
-        <v>138</v>
-      </c>
-      <c r="D19" s="166" t="s">
-        <v>156</v>
-      </c>
-      <c r="E19" s="163" t="s">
-        <v>28</v>
-      </c>
-      <c r="F19" s="164" t="s">
-        <v>190</v>
-      </c>
-      <c r="G19" s="167" t="s">
-        <v>220</v>
-      </c>
-      <c r="H19" s="168" t="s">
-        <v>202</v>
-      </c>
-      <c r="I19" s="164" t="s">
-        <v>221</v>
-      </c>
-      <c r="J19" s="170"/>
-    </row>
-    <row r="20" spans="1:10" ht="15.6">
-      <c r="A20" s="177"/>
-      <c r="B20" s="186">
-        <v>21</v>
-      </c>
-      <c r="C20" s="171" t="s">
-        <v>139</v>
-      </c>
-      <c r="D20" s="171" t="s">
-        <v>157</v>
-      </c>
-      <c r="E20" s="172" t="s">
-        <v>28</v>
-      </c>
-      <c r="F20" s="173" t="s">
-        <v>191</v>
-      </c>
-      <c r="G20" s="174" t="s">
-        <v>213</v>
-      </c>
-      <c r="H20" s="175" t="s">
-        <v>198</v>
-      </c>
-      <c r="I20" s="176" t="s">
-        <v>215</v>
-      </c>
-      <c r="J20" s="170"/>
-    </row>
-    <row r="21" spans="1:10">
-      <c r="A21" s="177"/>
-      <c r="B21" s="188" t="s">
-        <v>192</v>
-      </c>
-      <c r="C21" s="189"/>
-      <c r="D21" s="189"/>
-      <c r="E21" s="189"/>
-      <c r="F21" s="189"/>
-      <c r="G21" s="189"/>
-      <c r="H21" s="189"/>
-      <c r="I21" s="189"/>
-      <c r="J21" s="177"/>
+      <c r="F21" s="197" t="s">
+        <v>265</v>
+      </c>
+      <c r="G21" s="198" t="s">
+        <v>266</v>
+      </c>
+      <c r="H21" s="203" t="s">
+        <v>267</v>
+      </c>
+      <c r="I21" s="199" t="s">
+        <v>268</v>
+      </c>
+      <c r="J21" s="162"/>
     </row>
     <row r="22" spans="1:10">
-      <c r="A22" s="177"/>
-      <c r="B22" s="188"/>
-      <c r="C22" s="189"/>
-      <c r="D22" s="189"/>
-      <c r="E22" s="189"/>
-      <c r="F22" s="189"/>
-      <c r="G22" s="189"/>
-      <c r="H22" s="189"/>
-      <c r="I22" s="189"/>
-      <c r="J22" s="177"/>
-    </row>
-    <row r="23" spans="1:10" ht="4.2" customHeight="1">
-      <c r="A23" s="177"/>
-      <c r="B23" s="188"/>
-      <c r="C23" s="189"/>
-      <c r="D23" s="189"/>
-      <c r="E23" s="189"/>
-      <c r="F23" s="189"/>
-      <c r="G23" s="189"/>
-      <c r="H23" s="189"/>
-      <c r="I23" s="189"/>
-      <c r="J23" s="177"/>
+      <c r="A22" s="169"/>
+      <c r="B22" s="212" t="s">
+        <v>234</v>
+      </c>
+      <c r="C22" s="213"/>
+      <c r="D22" s="213"/>
+      <c r="E22" s="213"/>
+      <c r="F22" s="214"/>
+      <c r="G22" s="214"/>
+      <c r="H22" s="214"/>
+      <c r="I22" s="214"/>
+      <c r="J22" s="169"/>
+    </row>
+    <row r="23" spans="1:10">
+      <c r="A23" s="169"/>
+      <c r="B23" s="212"/>
+      <c r="C23" s="214"/>
+      <c r="D23" s="214"/>
+      <c r="E23" s="214"/>
+      <c r="F23" s="214"/>
+      <c r="G23" s="214"/>
+      <c r="H23" s="214"/>
+      <c r="I23" s="214"/>
+      <c r="J23" s="169"/>
+    </row>
+    <row r="24" spans="1:10" ht="4.2" customHeight="1">
+      <c r="A24" s="169"/>
+      <c r="B24" s="212"/>
+      <c r="C24" s="214"/>
+      <c r="D24" s="214"/>
+      <c r="E24" s="214"/>
+      <c r="F24" s="214"/>
+      <c r="G24" s="214"/>
+      <c r="H24" s="214"/>
+      <c r="I24" s="214"/>
+      <c r="J24" s="169"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B21:I23"/>
+    <mergeCell ref="B22:I24"/>
   </mergeCells>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="56" orientation="landscape" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:J29"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection sqref="A1:I26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="2" max="2" width="4.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="48.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="33.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.109375" customWidth="1"/>
+    <col min="9" max="9" width="102.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="17.399999999999999">
+      <c r="A1" s="169"/>
+      <c r="B1" s="179" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="139" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="139" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="139" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" s="139" t="s">
+        <v>207</v>
+      </c>
+      <c r="G1" s="139" t="s">
+        <v>208</v>
+      </c>
+      <c r="H1" s="170" t="s">
+        <v>209</v>
+      </c>
+      <c r="I1" s="181" t="s">
+        <v>205</v>
+      </c>
+      <c r="J1" s="169"/>
+    </row>
+    <row r="2" spans="1:10" ht="15.6">
+      <c r="A2" s="180"/>
+      <c r="B2" s="182">
+        <v>1</v>
+      </c>
+      <c r="C2" s="190" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="190" t="s">
+        <v>163</v>
+      </c>
+      <c r="E2" s="190" t="s">
+        <v>27</v>
+      </c>
+      <c r="F2" s="183" t="s">
+        <v>206</v>
+      </c>
+      <c r="G2" s="183" t="s">
+        <v>206</v>
+      </c>
+      <c r="H2" s="183" t="s">
+        <v>206</v>
+      </c>
+      <c r="I2" s="186" t="s">
+        <v>213</v>
+      </c>
+      <c r="J2" s="162"/>
+    </row>
+    <row r="3" spans="1:10" ht="15.6">
+      <c r="A3" s="180"/>
+      <c r="B3" s="188">
+        <v>2</v>
+      </c>
+      <c r="C3" s="182" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="182" t="s">
+        <v>153</v>
+      </c>
+      <c r="E3" s="182" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3" s="189" t="s">
+        <v>206</v>
+      </c>
+      <c r="G3" s="183" t="s">
+        <v>206</v>
+      </c>
+      <c r="H3" s="183" t="s">
+        <v>206</v>
+      </c>
+      <c r="I3" s="186" t="s">
+        <v>225</v>
+      </c>
+      <c r="J3" s="162"/>
+    </row>
+    <row r="4" spans="1:10" ht="15.6">
+      <c r="A4" s="180"/>
+      <c r="B4" s="182">
+        <v>3</v>
+      </c>
+      <c r="C4" s="191" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="191" t="s">
+        <v>164</v>
+      </c>
+      <c r="E4" s="191" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4" s="189" t="s">
+        <v>206</v>
+      </c>
+      <c r="G4" s="183" t="s">
+        <v>206</v>
+      </c>
+      <c r="H4" s="183" t="s">
+        <v>206</v>
+      </c>
+      <c r="I4" s="186" t="s">
+        <v>215</v>
+      </c>
+      <c r="J4" s="162"/>
+    </row>
+    <row r="5" spans="1:10" ht="15.6">
+      <c r="A5" s="180"/>
+      <c r="B5" s="182">
+        <v>4</v>
+      </c>
+      <c r="C5" s="182" t="s">
+        <v>66</v>
+      </c>
+      <c r="D5" s="182" t="s">
+        <v>165</v>
+      </c>
+      <c r="E5" s="182" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5" s="189" t="s">
+        <v>206</v>
+      </c>
+      <c r="G5" s="183" t="s">
+        <v>206</v>
+      </c>
+      <c r="H5" s="183" t="s">
+        <v>206</v>
+      </c>
+      <c r="I5" s="186" t="s">
+        <v>216</v>
+      </c>
+      <c r="J5" s="162"/>
+    </row>
+    <row r="6" spans="1:10" ht="15.6">
+      <c r="A6" s="180"/>
+      <c r="B6" s="182">
+        <v>5</v>
+      </c>
+      <c r="C6" s="182" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" s="182" t="s">
+        <v>166</v>
+      </c>
+      <c r="E6" s="182" t="s">
+        <v>28</v>
+      </c>
+      <c r="F6" s="189" t="s">
+        <v>206</v>
+      </c>
+      <c r="G6" s="183" t="s">
+        <v>206</v>
+      </c>
+      <c r="H6" s="183" t="s">
+        <v>206</v>
+      </c>
+      <c r="I6" s="186" t="s">
+        <v>217</v>
+      </c>
+      <c r="J6" s="162"/>
+    </row>
+    <row r="7" spans="1:10" ht="15.6">
+      <c r="A7" s="180"/>
+      <c r="B7" s="182">
+        <v>6</v>
+      </c>
+      <c r="C7" s="182" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="182" t="s">
+        <v>167</v>
+      </c>
+      <c r="E7" s="182" t="s">
+        <v>28</v>
+      </c>
+      <c r="F7" s="189" t="s">
+        <v>206</v>
+      </c>
+      <c r="G7" s="183" t="s">
+        <v>206</v>
+      </c>
+      <c r="H7" s="183" t="s">
+        <v>206</v>
+      </c>
+      <c r="I7" s="186" t="s">
+        <v>218</v>
+      </c>
+      <c r="J7" s="162"/>
+    </row>
+    <row r="8" spans="1:10" ht="15.6">
+      <c r="A8" s="180"/>
+      <c r="B8" s="182">
+        <v>7</v>
+      </c>
+      <c r="C8" s="184" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="184" t="s">
+        <v>168</v>
+      </c>
+      <c r="E8" s="182" t="s">
+        <v>27</v>
+      </c>
+      <c r="F8" s="189" t="s">
+        <v>206</v>
+      </c>
+      <c r="G8" s="183" t="s">
+        <v>206</v>
+      </c>
+      <c r="H8" s="183" t="s">
+        <v>206</v>
+      </c>
+      <c r="I8" s="187" t="s">
+        <v>220</v>
+      </c>
+      <c r="J8" s="162"/>
+    </row>
+    <row r="9" spans="1:10" ht="15.6">
+      <c r="A9" s="180"/>
+      <c r="B9" s="182">
+        <v>8</v>
+      </c>
+      <c r="C9" s="184" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="184" t="s">
+        <v>169</v>
+      </c>
+      <c r="E9" s="182" t="s">
+        <v>27</v>
+      </c>
+      <c r="F9" s="189" t="s">
+        <v>206</v>
+      </c>
+      <c r="G9" s="183" t="s">
+        <v>206</v>
+      </c>
+      <c r="H9" s="183" t="s">
+        <v>206</v>
+      </c>
+      <c r="I9" s="187" t="s">
+        <v>219</v>
+      </c>
+      <c r="J9" s="162"/>
+    </row>
+    <row r="10" spans="1:10" ht="15.6">
+      <c r="A10" s="180"/>
+      <c r="B10" s="182">
+        <v>9</v>
+      </c>
+      <c r="C10" s="184" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="184" t="s">
+        <v>170</v>
+      </c>
+      <c r="E10" s="182" t="s">
+        <v>27</v>
+      </c>
+      <c r="F10" s="189" t="s">
+        <v>206</v>
+      </c>
+      <c r="G10" s="183" t="s">
+        <v>206</v>
+      </c>
+      <c r="H10" s="183" t="s">
+        <v>206</v>
+      </c>
+      <c r="I10" s="187" t="s">
+        <v>220</v>
+      </c>
+      <c r="J10" s="162"/>
+    </row>
+    <row r="11" spans="1:10" ht="15.6">
+      <c r="A11" s="180"/>
+      <c r="B11" s="182">
+        <v>10</v>
+      </c>
+      <c r="C11" s="182" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="182" t="s">
+        <v>171</v>
+      </c>
+      <c r="E11" s="182" t="s">
+        <v>27</v>
+      </c>
+      <c r="F11" s="189" t="s">
+        <v>206</v>
+      </c>
+      <c r="G11" s="183" t="s">
+        <v>206</v>
+      </c>
+      <c r="H11" s="183" t="s">
+        <v>206</v>
+      </c>
+      <c r="I11" s="186" t="s">
+        <v>221</v>
+      </c>
+      <c r="J11" s="162"/>
+    </row>
+    <row r="12" spans="1:10" ht="15.6">
+      <c r="A12" s="180"/>
+      <c r="B12" s="182">
+        <v>11</v>
+      </c>
+      <c r="C12" s="182" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="182" t="s">
+        <v>172</v>
+      </c>
+      <c r="E12" s="182" t="s">
+        <v>27</v>
+      </c>
+      <c r="F12" s="189" t="s">
+        <v>206</v>
+      </c>
+      <c r="G12" s="183" t="s">
+        <v>206</v>
+      </c>
+      <c r="H12" s="183" t="s">
+        <v>206</v>
+      </c>
+      <c r="I12" s="186" t="s">
+        <v>215</v>
+      </c>
+      <c r="J12" s="162"/>
+    </row>
+    <row r="13" spans="1:10" ht="15.6">
+      <c r="A13" s="180"/>
+      <c r="B13" s="182">
+        <v>13</v>
+      </c>
+      <c r="C13" s="182" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" s="184" t="s">
+        <v>162</v>
+      </c>
+      <c r="E13" s="182" t="s">
+        <v>27</v>
+      </c>
+      <c r="F13" s="189" t="s">
+        <v>206</v>
+      </c>
+      <c r="G13" s="183" t="s">
+        <v>206</v>
+      </c>
+      <c r="H13" s="183" t="s">
+        <v>206</v>
+      </c>
+      <c r="I13" s="187" t="s">
+        <v>220</v>
+      </c>
+      <c r="J13" s="162"/>
+    </row>
+    <row r="14" spans="1:10" ht="15.6">
+      <c r="A14" s="180"/>
+      <c r="B14" s="184">
+        <v>14</v>
+      </c>
+      <c r="C14" s="184" t="s">
+        <v>44</v>
+      </c>
+      <c r="D14" s="184" t="s">
+        <v>161</v>
+      </c>
+      <c r="E14" s="184" t="s">
+        <v>27</v>
+      </c>
+      <c r="F14" s="189" t="s">
+        <v>206</v>
+      </c>
+      <c r="G14" s="183" t="s">
+        <v>206</v>
+      </c>
+      <c r="H14" s="183" t="s">
+        <v>206</v>
+      </c>
+      <c r="I14" s="187" t="s">
+        <v>220</v>
+      </c>
+      <c r="J14" s="162"/>
+    </row>
+    <row r="15" spans="1:10" ht="15.6">
+      <c r="A15" s="180"/>
+      <c r="B15" s="182">
+        <v>15</v>
+      </c>
+      <c r="C15" s="184" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15" s="184" t="s">
+        <v>160</v>
+      </c>
+      <c r="E15" s="182" t="s">
+        <v>27</v>
+      </c>
+      <c r="F15" s="189" t="s">
+        <v>206</v>
+      </c>
+      <c r="G15" s="183" t="s">
+        <v>206</v>
+      </c>
+      <c r="H15" s="185" t="s">
+        <v>206</v>
+      </c>
+      <c r="I15" s="186" t="s">
+        <v>222</v>
+      </c>
+      <c r="J15" s="162"/>
+    </row>
+    <row r="16" spans="1:10" ht="15.6">
+      <c r="A16" s="180"/>
+      <c r="B16" s="182">
+        <v>16</v>
+      </c>
+      <c r="C16" s="184" t="s">
+        <v>15</v>
+      </c>
+      <c r="D16" s="184" t="s">
+        <v>159</v>
+      </c>
+      <c r="E16" s="182" t="s">
+        <v>27</v>
+      </c>
+      <c r="F16" s="183" t="s">
+        <v>206</v>
+      </c>
+      <c r="G16" s="183" t="s">
+        <v>206</v>
+      </c>
+      <c r="H16" s="183" t="s">
+        <v>206</v>
+      </c>
+      <c r="I16" s="186" t="s">
+        <v>223</v>
+      </c>
+      <c r="J16" s="162"/>
+    </row>
+    <row r="17" spans="1:10" ht="15.6">
+      <c r="A17" s="180"/>
+      <c r="B17" s="182">
+        <v>17</v>
+      </c>
+      <c r="C17" s="184" t="s">
+        <v>85</v>
+      </c>
+      <c r="D17" s="184" t="s">
+        <v>158</v>
+      </c>
+      <c r="E17" s="182" t="s">
+        <v>27</v>
+      </c>
+      <c r="F17" s="183" t="s">
+        <v>206</v>
+      </c>
+      <c r="G17" s="183" t="s">
+        <v>206</v>
+      </c>
+      <c r="H17" s="185" t="s">
+        <v>206</v>
+      </c>
+      <c r="I17" s="186" t="s">
+        <v>222</v>
+      </c>
+      <c r="J17" s="162"/>
+    </row>
+    <row r="18" spans="1:10" ht="15.6">
+      <c r="A18" s="180"/>
+      <c r="B18" s="182">
+        <v>18</v>
+      </c>
+      <c r="C18" s="184" t="s">
+        <v>141</v>
+      </c>
+      <c r="D18" s="184" t="s">
+        <v>154</v>
+      </c>
+      <c r="E18" s="182" t="s">
+        <v>28</v>
+      </c>
+      <c r="F18" s="183" t="s">
+        <v>224</v>
+      </c>
+      <c r="G18" s="183" t="s">
+        <v>224</v>
+      </c>
+      <c r="H18" s="183" t="s">
+        <v>224</v>
+      </c>
+      <c r="I18" s="186" t="s">
+        <v>212</v>
+      </c>
+      <c r="J18" s="162"/>
+    </row>
+    <row r="19" spans="1:10" ht="15.6">
+      <c r="A19" s="180"/>
+      <c r="B19" s="182">
+        <v>19</v>
+      </c>
+      <c r="C19" s="184" t="s">
+        <v>140</v>
+      </c>
+      <c r="D19" s="184" t="s">
+        <v>155</v>
+      </c>
+      <c r="E19" s="182" t="s">
+        <v>28</v>
+      </c>
+      <c r="F19" s="183" t="s">
+        <v>224</v>
+      </c>
+      <c r="G19" s="183" t="s">
+        <v>224</v>
+      </c>
+      <c r="H19" s="183" t="s">
+        <v>224</v>
+      </c>
+      <c r="I19" s="186" t="s">
+        <v>211</v>
+      </c>
+      <c r="J19" s="162"/>
+    </row>
+    <row r="20" spans="1:10" ht="15.6">
+      <c r="A20" s="180"/>
+      <c r="B20" s="182">
+        <v>20</v>
+      </c>
+      <c r="C20" s="184" t="s">
+        <v>138</v>
+      </c>
+      <c r="D20" s="184" t="s">
+        <v>156</v>
+      </c>
+      <c r="E20" s="182" t="s">
+        <v>28</v>
+      </c>
+      <c r="F20" s="183" t="s">
+        <v>224</v>
+      </c>
+      <c r="G20" s="183" t="s">
+        <v>224</v>
+      </c>
+      <c r="H20" s="183" t="s">
+        <v>224</v>
+      </c>
+      <c r="I20" s="186" t="s">
+        <v>210</v>
+      </c>
+      <c r="J20" s="162"/>
+    </row>
+    <row r="21" spans="1:10" ht="15.6">
+      <c r="A21" s="180"/>
+      <c r="B21" s="182">
+        <v>21</v>
+      </c>
+      <c r="C21" s="184" t="s">
+        <v>139</v>
+      </c>
+      <c r="D21" s="184" t="s">
+        <v>157</v>
+      </c>
+      <c r="E21" s="182" t="s">
+        <v>28</v>
+      </c>
+      <c r="F21" s="183" t="s">
+        <v>224</v>
+      </c>
+      <c r="G21" s="183" t="s">
+        <v>224</v>
+      </c>
+      <c r="H21" s="183" t="s">
+        <v>224</v>
+      </c>
+      <c r="I21" s="186" t="s">
+        <v>211</v>
+      </c>
+      <c r="J21" s="162"/>
+    </row>
+    <row r="22" spans="1:10" ht="15.6">
+      <c r="A22" s="180"/>
+      <c r="B22" s="182">
+        <v>22</v>
+      </c>
+      <c r="C22" s="184" t="s">
+        <v>71</v>
+      </c>
+      <c r="D22" s="184" t="s">
+        <v>176</v>
+      </c>
+      <c r="E22" s="182" t="s">
+        <v>28</v>
+      </c>
+      <c r="F22" s="183" t="s">
+        <v>224</v>
+      </c>
+      <c r="G22" s="183" t="s">
+        <v>224</v>
+      </c>
+      <c r="H22" s="183" t="s">
+        <v>224</v>
+      </c>
+      <c r="I22" s="186" t="s">
+        <v>214</v>
+      </c>
+      <c r="J22" s="162"/>
+    </row>
+    <row r="23" spans="1:10" ht="15.6">
+      <c r="A23" s="180"/>
+      <c r="B23" s="192"/>
+      <c r="C23" s="193"/>
+      <c r="D23" s="193"/>
+      <c r="E23" s="192"/>
+      <c r="F23" s="194"/>
+      <c r="G23" s="194"/>
+      <c r="H23" s="194"/>
+      <c r="I23" s="195"/>
+      <c r="J23" s="162"/>
+    </row>
+    <row r="24" spans="1:10">
+      <c r="A24" s="169"/>
+      <c r="B24" s="215" t="s">
+        <v>273</v>
+      </c>
+      <c r="C24" s="213"/>
+      <c r="D24" s="213"/>
+      <c r="E24" s="213"/>
+      <c r="F24" s="213"/>
+      <c r="G24" s="213"/>
+      <c r="H24" s="213"/>
+      <c r="I24" s="213"/>
+      <c r="J24" s="169"/>
+    </row>
+    <row r="25" spans="1:10">
+      <c r="A25" s="169"/>
+      <c r="B25" s="212"/>
+      <c r="C25" s="214"/>
+      <c r="D25" s="214"/>
+      <c r="E25" s="214"/>
+      <c r="F25" s="214"/>
+      <c r="G25" s="214"/>
+      <c r="H25" s="214"/>
+      <c r="I25" s="214"/>
+      <c r="J25" s="169"/>
+    </row>
+    <row r="26" spans="1:10">
+      <c r="A26" s="169"/>
+      <c r="B26" s="212"/>
+      <c r="C26" s="214"/>
+      <c r="D26" s="214"/>
+      <c r="E26" s="214"/>
+      <c r="F26" s="214"/>
+      <c r="G26" s="214"/>
+      <c r="H26" s="214"/>
+      <c r="I26" s="214"/>
+      <c r="J26" s="169"/>
+    </row>
+    <row r="28" spans="1:10">
+      <c r="G28" s="216" t="s">
+        <v>226</v>
+      </c>
+      <c r="H28" s="216"/>
+      <c r="I28" s="217" t="e">
+        <f>H2+H4+G4+F4+F5+F6+F7+H6+H12+G12+F12+F15+G15+G16+G17</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10">
+      <c r="G29" s="216"/>
+      <c r="H29" s="216"/>
+      <c r="I29" s="218"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B24:I26"/>
+    <mergeCell ref="G28:H29"/>
+    <mergeCell ref="I28:I29"/>
+  </mergeCells>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="50" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>